<commit_message>
Cleaned up some code and added new meta data properties
</commit_message>
<xml_diff>
--- a/IFilterTextReader/Properties.xlsx
+++ b/IFilterTextReader/Properties.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView showHorizontalScroll="0" showVerticalScroll="0" showSheetTabs="0" xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9435"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="522">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="960" uniqueCount="934">
   <si>
     <t>Comments</t>
   </si>
@@ -1590,6 +1590,1242 @@
   </si>
   <si>
     <t>8DEE0300-16C2-101B-B121-08002B2ECDA9/SOLUTION</t>
+  </si>
+  <si>
+    <t>Document Note Count</t>
+  </si>
+  <si>
+    <t>Hidden Slide Count</t>
+  </si>
+  <si>
+    <t>Multimedia Clip Count</t>
+  </si>
+  <si>
+    <t>Scale (set to True (-1) when scaling of thumbnail)</t>
+  </si>
+  <si>
+    <t>Heading Pair (internal property indicating the grouping of different document parts and the number of items in each group)</t>
+  </si>
+  <si>
+    <t>partTitles (DocParts) (names of document parts)</t>
+  </si>
+  <si>
+    <t>Links Dirty</t>
+  </si>
+  <si>
+    <t>CCH with Spaces (number of characters including spaces)</t>
+  </si>
+  <si>
+    <t>GUID (no longer used)</t>
+  </si>
+  <si>
+    <t>Shared Doc</t>
+  </si>
+  <si>
+    <t>Hyperlinks Changed</t>
+  </si>
+  <si>
+    <t>Version</t>
+  </si>
+  <si>
+    <t>Content Type</t>
+  </si>
+  <si>
+    <t>Content Status</t>
+  </si>
+  <si>
+    <t>Language</t>
+  </si>
+  <si>
+    <t>Document hyperlink references</t>
+  </si>
+  <si>
+    <t>Site ID of the document workspace</t>
+  </si>
+  <si>
+    <t>Address of the Source Workspace Library</t>
+  </si>
+  <si>
+    <t>Content Type ID</t>
+  </si>
+  <si>
+    <t>Application Name</t>
+  </si>
+  <si>
+    <t>Document Security</t>
+  </si>
+  <si>
+    <t>F29F85E0-4FF9-1068-AB91-08002B27B3D9/10</t>
+  </si>
+  <si>
+    <t>F29F85E0-4FF9-1068-AB91-08002B27B3D9/12</t>
+  </si>
+  <si>
+    <t>F29F85E0-4FF9-1068-AB91-08002B27B3D9/13</t>
+  </si>
+  <si>
+    <t>F29F85E0-4FF9-1068-AB91-08002B27B3D9/14</t>
+  </si>
+  <si>
+    <t>F29F85E0-4FF9-1068-AB91-08002B27B3D9/15</t>
+  </si>
+  <si>
+    <t>F29F85E0-4FF9-1068-AB91-08002B27B3D9/16</t>
+  </si>
+  <si>
+    <t>F29F85E0-4FF9-1068-AB91-08002B27B3D9/18</t>
+  </si>
+  <si>
+    <t>F29F85E0-4FF9-1068-AB91-08002B27B3D9/19</t>
+  </si>
+  <si>
+    <t>_F29F85E0_4FF9_1068_AB91_08002B27B3D9_10</t>
+  </si>
+  <si>
+    <t>_F29F85E0_4FF9_1068_AB91_08002B27B3D9_12</t>
+  </si>
+  <si>
+    <t>_F29F85E0_4FF9_1068_AB91_08002B27B3D9_13</t>
+  </si>
+  <si>
+    <t>_F29F85E0_4FF9_1068_AB91_08002B27B3D9_14</t>
+  </si>
+  <si>
+    <t>_F29F85E0_4FF9_1068_AB91_08002B27B3D9_15</t>
+  </si>
+  <si>
+    <t>_F29F85E0_4FF9_1068_AB91_08002B27B3D9_16</t>
+  </si>
+  <si>
+    <t>_F29F85E0_4FF9_1068_AB91_08002B27B3D9_18</t>
+  </si>
+  <si>
+    <t>_F29F85E0_4FF9_1068_AB91_08002B27B3D9_19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date (of interest) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Type </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ContentType </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kind </t>
+  </si>
+  <si>
+    <t xml:space="preserve">File Extension </t>
+  </si>
+  <si>
+    <t xml:space="preserve">File Count </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shared </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shared with </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sharing status </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data Accessed </t>
+  </si>
+  <si>
+    <t xml:space="preserve">File Attributes </t>
+  </si>
+  <si>
+    <t xml:space="preserve">File Owner </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Computer </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Encryption Status </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Offline availability </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Offline status </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Link Target Path </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Folder Path </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Search ranking </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Audio Channel Count </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sample Rate </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Length </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Album Artist </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Album ID </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Artist 2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beats Per Minute </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Composer </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Conductor </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lyrics </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mood </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Year </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Part of set (Disc number) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Authors </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contributor </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Line Count </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paragraph Count </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Protected </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Version </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Document ID </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bit depth </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Compression </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Horizontal Resolution </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vertical Resolution </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vertical Size </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Camera Model </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date Taken </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Digital Zoom </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Event </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exposure Bias </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exposure Time </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Light source </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Focal Length </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ISO Speed </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exif Orientation </t>
+  </si>
+  <si>
+    <t xml:space="preserve">People Tags </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shutter Speed </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subject Distance </t>
+  </si>
+  <si>
+    <t xml:space="preserve">White Balance </t>
+  </si>
+  <si>
+    <t xml:space="preserve">35mm (Film) Focal Length </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exif Version </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exposure Program </t>
+  </si>
+  <si>
+    <t xml:space="preserve">F-Stop </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lens Maker </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lens Model </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Program Mode </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Saturation </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Creator Application </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Creator Application Version </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date Encoded </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Duration </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Encoded By </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Frame Count </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Producer </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rating </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Publisher </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subtitle </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parental Rating </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Video Compression </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Director </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data rate </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Frame rate </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Horizontal Aspect ratio </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vertical Aspect ratio </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Company </t>
+  </si>
+  <si>
+    <t xml:space="preserve">File Description </t>
+  </si>
+  <si>
+    <t xml:space="preserve">File Version </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date Last Used </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Product Name </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Product Version </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Copyright </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channel no. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Episode name </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Closed Captioning </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DTV </t>
+  </si>
+  <si>
+    <t xml:space="preserve">HD </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Repeat Broadcast </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Network Affiliation </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Broadcast Date </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Program Description </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Recording Time </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date Acquired </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date Archived </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date Imported </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date Completed </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date Released </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date Visited </t>
+  </si>
+  <si>
+    <t xml:space="preserve">MIME Type </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Status </t>
+  </si>
+  <si>
+    <t>F7DB74B4-4287-4103-AFBA-F1B13DCD75CF/100</t>
+  </si>
+  <si>
+    <t>28636AA6-953D-11D2-B5D6-00C04FD918D0/11</t>
+  </si>
+  <si>
+    <t>D5CDD502-2E9C-101B-9397-08002B2CF9AE/26</t>
+  </si>
+  <si>
+    <t>1E3EE840-BC2B-476C-8237-2ACD1A839B22/3</t>
+  </si>
+  <si>
+    <t>E4F10A3C-49E6-405D-8288-A23BD4EEAA6C/100</t>
+  </si>
+  <si>
+    <t>28636AA6-953D-11D2-B5D6-00C04FD918D0/12</t>
+  </si>
+  <si>
+    <t>EF884C5B-2BFE-41BB-AAE5-76EEDF4F9902/100</t>
+  </si>
+  <si>
+    <t>EF884C5B-2BFE-41BB-AAE5-76EEDF4F9902/200</t>
+  </si>
+  <si>
+    <t>EF884C5B-2BFE-41BB-AAE5-76EEDF4F9902/300</t>
+  </si>
+  <si>
+    <t>B725F130-47EF-101A-A5F1-02608C9EEBAC/16</t>
+  </si>
+  <si>
+    <t>B725F130-47EF-101A-A5F1-02608C9EEBAC/13</t>
+  </si>
+  <si>
+    <t>9B174B34-40FF-11D2-A27E-00C04FC30871/4</t>
+  </si>
+  <si>
+    <t>28636AA6-953D-11D2-B5D6-00C04FD918D0/5</t>
+  </si>
+  <si>
+    <t>90E5E14E-648B-4826-B2AA-ACAF790E3513/10</t>
+  </si>
+  <si>
+    <t>A94688B6-7D9F-4570-A648-E3DFC0AB2B3F/100</t>
+  </si>
+  <si>
+    <t>6D24888F-4718-4BDA-AFED-EA0FB4386CD8/100</t>
+  </si>
+  <si>
+    <t>B9B4B3FC-2B51-4A42-B5D8-324146AFCF25/2</t>
+  </si>
+  <si>
+    <t>E3E0584C-B788-4A5A-BB20-7F5A44C9ACDD/6</t>
+  </si>
+  <si>
+    <t>49691C90-7E17-101A-A91C-08002B2ECDA9}/3</t>
+  </si>
+  <si>
+    <t>64440490-4C8B-11D1-8B70-080036B11A03/7</t>
+  </si>
+  <si>
+    <t>64440490-4C8B-11D1-8B70-080036B11A03/5</t>
+  </si>
+  <si>
+    <t>64440490-4C8B-11D1-8B70-080036B11A03/8</t>
+  </si>
+  <si>
+    <t>56A3372E-CE9C-11D2-9F0E-006097C686F6/13</t>
+  </si>
+  <si>
+    <t>56A3372E-CE9C-11D2-9F0E-006097C686F6/100</t>
+  </si>
+  <si>
+    <t>FD122953-FA93-4EF7-92C3-04C946B2F7C8/100</t>
+  </si>
+  <si>
+    <t>56A3372E-CE9C-11D2-9F0E-006097C686F6/35</t>
+  </si>
+  <si>
+    <t>64440492-4C8B-11D1-8B70-080036B11A03/19</t>
+  </si>
+  <si>
+    <t>56A3372E-CE9C-11D2-9F0E-006097C686F6/36</t>
+  </si>
+  <si>
+    <t>56A3372E-CE9C-11D2-9F0E-006097C686F6/12</t>
+  </si>
+  <si>
+    <t>56A3372E-CE9C-11D2-9F0E-006097C686F6/39</t>
+  </si>
+  <si>
+    <t>56A3372E-CE9C-11D2-9F0E-006097C686F6/37</t>
+  </si>
+  <si>
+    <t>D0A04F0A-462A-48A4-BB2F-3706E88DBD7D/100</t>
+  </si>
+  <si>
+    <t>F334115E-DA1B-4509-9B3D-119504DC7ABB/15</t>
+  </si>
+  <si>
+    <t>D5CDD502-2E9C-101B-9397-08002B2CF9AE/5</t>
+  </si>
+  <si>
+    <t>D5CDD502-2E9C-101B-9397-08002B2CF9AE/6</t>
+  </si>
+  <si>
+    <t>AEAC19E4-89AE-4508-B9B7-BB867ABEE2ED/2</t>
+  </si>
+  <si>
+    <t>D5CDD502-2E9C-101B-9397-08002B2CF9AE/29</t>
+  </si>
+  <si>
+    <t>E08805C8-E395-40DF-80D2-54F0D6C43154/100</t>
+  </si>
+  <si>
+    <t>6444048F-4C8B-11D1-8B70-080036B11A03/7</t>
+  </si>
+  <si>
+    <t>14B81DA1-0135-4D31-96D9-6CBFC9671A99/259</t>
+  </si>
+  <si>
+    <t>6444048F-4C8B-11D1-8B70-080036B11A03/3</t>
+  </si>
+  <si>
+    <t>6444048F-4C8B-11D1-8B70-080036B11A03/4</t>
+  </si>
+  <si>
+    <t>14B81DA1-0135-4D31-96D9-6CBFC9671A99/37378</t>
+  </si>
+  <si>
+    <t>14B81DA1-0135-4D31-96D9-6CBFC9671A99/36867</t>
+  </si>
+  <si>
+    <t>F85BF840-A925-4BC2-B0C4-8E36B598679E/100</t>
+  </si>
+  <si>
+    <t>14B81DA1-0135-4D31-96D9-6CBFC9671A99/18248</t>
+  </si>
+  <si>
+    <t>14B81DA1-0135-4D31-96D9-6CBFC9671A99/37380</t>
+  </si>
+  <si>
+    <t>14B81DA1-0135-4D31-96D9-6CBFC9671A99/33434</t>
+  </si>
+  <si>
+    <t>2D152B40-CA39-40DB-B2CC-573725B2FEC5/100</t>
+  </si>
+  <si>
+    <t>14B81DA1-0135-4D31-96D9-6CBFC9671A99/37386</t>
+  </si>
+  <si>
+    <t>14B81DA1-0135-4D31-96D9-6CBFC9671A99/34855</t>
+  </si>
+  <si>
+    <t>14B81DA1-0135-4D31-96D9-6CBFC9671A99/37383</t>
+  </si>
+  <si>
+    <t>E8309B6E-084C-49B4-B1FC-90A80331B638/100</t>
+  </si>
+  <si>
+    <t>14B81DA1-0135-4D31-96D9-6CBFC9671A99/37377</t>
+  </si>
+  <si>
+    <t>14B81DA1-0135-4D31-96D9-6CBFC9671A99/37382</t>
+  </si>
+  <si>
+    <t>EE3D3D8A-5381-4CFA-B13B-AAF66B5F4EC9/100</t>
+  </si>
+  <si>
+    <t>A0E74609-B84D-4F49-B860-462BD9971F98/100</t>
+  </si>
+  <si>
+    <t>D35F743A-EB2E-47F2-A286-844132CB1427/100</t>
+  </si>
+  <si>
+    <t>14B81DA1-0135-4D31-96D9-6CBFC9671A99/34850</t>
+  </si>
+  <si>
+    <t>14B81DA1-0135-4D31-96D9-6CBFC9671A99}/33437</t>
+  </si>
+  <si>
+    <t>E6DDCAF7-29C5-4F0A-9A68-D19412EC7090/100</t>
+  </si>
+  <si>
+    <t>E1277516-2B5F-4869-89B1-2E585BD38B7A/100</t>
+  </si>
+  <si>
+    <t>6D217F6D-3F6A-4825-B470-5F03CA2FBE9B/100</t>
+  </si>
+  <si>
+    <t>49237325-A95A-4F67-B211-816B2D45D2E0/100</t>
+  </si>
+  <si>
+    <t>64440492-4C8B-11D1-8B70-080036B11A03/27</t>
+  </si>
+  <si>
+    <t>64440492-4C8B-11D1-8B70-080036B11A03/28</t>
+  </si>
+  <si>
+    <t>2E4B640D-5019-46D8-8881-55414CC5CAA0/100</t>
+  </si>
+  <si>
+    <t>64440490-4C8B-11D1-8B70-080036B11A03/3</t>
+  </si>
+  <si>
+    <t>64440492-4C8B-11D1-8B70-080036B11A03/36</t>
+  </si>
+  <si>
+    <t>6444048F-4C8B-11D1-8B70-080036B11A03/12</t>
+  </si>
+  <si>
+    <t>64440492-4C8B-11D1-8B70-080036B11A03/22</t>
+  </si>
+  <si>
+    <t>64440492-4C8B-11D1-8B70-080036B11A03/39</t>
+  </si>
+  <si>
+    <t>64440492-4C8B-11D1-8B70-080036B11A03/30</t>
+  </si>
+  <si>
+    <t>56A3372E-CE9C-11D2-9F0E-006097C686F6/38</t>
+  </si>
+  <si>
+    <t>64440492-4C8B-11D1-8B70-080036B11A03/23</t>
+  </si>
+  <si>
+    <t>64440492-4C8B-11D1-8B70-080036B11A03/21</t>
+  </si>
+  <si>
+    <t>64440491-4C8B-11D1-8B70-080036B11A03/10</t>
+  </si>
+  <si>
+    <t>64440492-4C8B-11D1-8B70-080036B11A03/20</t>
+  </si>
+  <si>
+    <t>64440491-4C8B-11D1-8B70-080036B11A03/8</t>
+  </si>
+  <si>
+    <t>64440491-4C8B-11D1-8B70-080036B11A03/44</t>
+  </si>
+  <si>
+    <t>64440491-4C8B-11D1-8B70-080036B11A03/42</t>
+  </si>
+  <si>
+    <t>64440491-4C8B-11D1-8B70-080036B11A03/45</t>
+  </si>
+  <si>
+    <t>64440491-4C8B-11D1-8B70-080036B11A03/43</t>
+  </si>
+  <si>
+    <t>0CEF7D53-FA64-11D1-A203-0000F81FEDEE/3</t>
+  </si>
+  <si>
+    <t>0CEF7D53-FA64-11D1-A203-0000F81FEDEE/4</t>
+  </si>
+  <si>
+    <t>841E4F90-FF59-4D16-8947-E81BBFFAB36D/16</t>
+  </si>
+  <si>
+    <t>0CEF7D53-FA64-11D1-A203-0000F81FEDEE/7</t>
+  </si>
+  <si>
+    <t>0CEF7D53-FA64-11D1-A203-0000F81FEDEE/8</t>
+  </si>
+  <si>
+    <t>64440492-4C8B-11D1-8B70-080036B11A03/11</t>
+  </si>
+  <si>
+    <t>6D748DE2-8D38-4CC3-AC60-F009B057C557/7</t>
+  </si>
+  <si>
+    <t>6D748DE2-8D38-4CC3-AC60-F009B057C557/2</t>
+  </si>
+  <si>
+    <t>6D748DE2-8D38-4CC3-AC60-F009B057C557/12</t>
+  </si>
+  <si>
+    <t>6D748DE2-8D38-4CC3-AC60-F009B057C557/17</t>
+  </si>
+  <si>
+    <t>6D748DE2-8D38-4CC3-AC60-F009B057C557/18</t>
+  </si>
+  <si>
+    <t>6D748DE2-8D38-4CC3-AC60-F009B057C557/13</t>
+  </si>
+  <si>
+    <t>2C53C813-FB63-4E22-A1AB-0B331CA1E273/100</t>
+  </si>
+  <si>
+    <t>4684FE97-8765-4842-9C13-F006447B178C/100</t>
+  </si>
+  <si>
+    <t>6D748DE2-8D38-4CC3-AC60-F009B057C557/3</t>
+  </si>
+  <si>
+    <t>A5477F61-7A82-4ECA-9DDE-98B69B2479B3/100</t>
+  </si>
+  <si>
+    <t>2CBAA8F5-D81F-47CA-B17A-F8D822300131/100</t>
+  </si>
+  <si>
+    <t>43F8D7B7-A444-4F87-9383-52271C9B915C/100</t>
+  </si>
+  <si>
+    <t>14B81DA1-0135-4D31-96D9-6CBFC9671A99/18258</t>
+  </si>
+  <si>
+    <t>72FAB781-ACDA-43E5-B155-B2434F85E678/100</t>
+  </si>
+  <si>
+    <t>DE41CC29-6971-4290-B472-F59F2E2F31E2/100</t>
+  </si>
+  <si>
+    <t>5CBF2787-48CF-4208-B90E-EE5E5D420294/23</t>
+  </si>
+  <si>
+    <t>64440492-4C8B-11D1-8B70-080036B11A03/9</t>
+  </si>
+  <si>
+    <t>000214A1-0000-0000-C000-000000000046/9</t>
+  </si>
+  <si>
+    <t>28636AA6-953D-11D2-B5D6-00C04FD918D0/14</t>
+  </si>
+  <si>
+    <t>_F7DB74B4-4287-4103-AFBA-F1B13DCD75CF_100</t>
+  </si>
+  <si>
+    <t>_28636AA6-953D-11D2-B5D6-00C04FD918D0_11</t>
+  </si>
+  <si>
+    <t>_D5CDD502-2E9C-101B-9397-08002B2CF9AE_26</t>
+  </si>
+  <si>
+    <t>_1E3EE840-BC2B-476C-8237-2ACD1A839B22_3</t>
+  </si>
+  <si>
+    <t>_E4F10A3C-49E6-405D-8288-A23BD4EEAA6C_100</t>
+  </si>
+  <si>
+    <t>_28636AA6-953D-11D2-B5D6-00C04FD918D0_12</t>
+  </si>
+  <si>
+    <t>_EF884C5B-2BFE-41BB-AAE5-76EEDF4F9902_100</t>
+  </si>
+  <si>
+    <t>_EF884C5B-2BFE-41BB-AAE5-76EEDF4F9902_200</t>
+  </si>
+  <si>
+    <t>_EF884C5B-2BFE-41BB-AAE5-76EEDF4F9902_300</t>
+  </si>
+  <si>
+    <t>_B725F130-47EF-101A-A5F1-02608C9EEBAC_16</t>
+  </si>
+  <si>
+    <t>_B725F130-47EF-101A-A5F1-02608C9EEBAC_13</t>
+  </si>
+  <si>
+    <t>_9B174B34-40FF-11D2-A27E-00C04FC30871_4</t>
+  </si>
+  <si>
+    <t>_28636AA6-953D-11D2-B5D6-00C04FD918D0_5</t>
+  </si>
+  <si>
+    <t>_90E5E14E-648B-4826-B2AA-ACAF790E3513_10</t>
+  </si>
+  <si>
+    <t>_A94688B6-7D9F-4570-A648-E3DFC0AB2B3F_100</t>
+  </si>
+  <si>
+    <t>_6D24888F-4718-4BDA-AFED-EA0FB4386CD8_100</t>
+  </si>
+  <si>
+    <t>_B9B4B3FC-2B51-4A42-B5D8-324146AFCF25_2</t>
+  </si>
+  <si>
+    <t>_E3E0584C-B788-4A5A-BB20-7F5A44C9ACDD_6</t>
+  </si>
+  <si>
+    <t>_49691C90-7E17-101A-A91C-08002B2ECDA9}_3</t>
+  </si>
+  <si>
+    <t>_64440490-4C8B-11D1-8B70-080036B11A03_7</t>
+  </si>
+  <si>
+    <t>_64440490-4C8B-11D1-8B70-080036B11A03_5</t>
+  </si>
+  <si>
+    <t>_64440490-4C8B-11D1-8B70-080036B11A03_8</t>
+  </si>
+  <si>
+    <t>_56A3372E-CE9C-11D2-9F0E-006097C686F6_13</t>
+  </si>
+  <si>
+    <t>_56A3372E-CE9C-11D2-9F0E-006097C686F6_100</t>
+  </si>
+  <si>
+    <t>_FD122953-FA93-4EF7-92C3-04C946B2F7C8_100</t>
+  </si>
+  <si>
+    <t>_56A3372E-CE9C-11D2-9F0E-006097C686F6_35</t>
+  </si>
+  <si>
+    <t>_64440492-4C8B-11D1-8B70-080036B11A03_19</t>
+  </si>
+  <si>
+    <t>_56A3372E-CE9C-11D2-9F0E-006097C686F6_36</t>
+  </si>
+  <si>
+    <t>_56A3372E-CE9C-11D2-9F0E-006097C686F6_12</t>
+  </si>
+  <si>
+    <t>_56A3372E-CE9C-11D2-9F0E-006097C686F6_39</t>
+  </si>
+  <si>
+    <t>_56A3372E-CE9C-11D2-9F0E-006097C686F6_37</t>
+  </si>
+  <si>
+    <t>_D0A04F0A-462A-48A4-BB2F-3706E88DBD7D_100</t>
+  </si>
+  <si>
+    <t>_F334115E-DA1B-4509-9B3D-119504DC7ABB_15</t>
+  </si>
+  <si>
+    <t>_D5CDD502-2E9C-101B-9397-08002B2CF9AE_5</t>
+  </si>
+  <si>
+    <t>_D5CDD502-2E9C-101B-9397-08002B2CF9AE_6</t>
+  </si>
+  <si>
+    <t>_AEAC19E4-89AE-4508-B9B7-BB867ABEE2ED_2</t>
+  </si>
+  <si>
+    <t>_E08805C8-E395-40DF-80D2-54F0D6C43154_100</t>
+  </si>
+  <si>
+    <t>_6444048F-4C8B-11D1-8B70-080036B11A03_7</t>
+  </si>
+  <si>
+    <t>_14B81DA1-0135-4D31-96D9-6CBFC9671A99_259</t>
+  </si>
+  <si>
+    <t>_6444048F-4C8B-11D1-8B70-080036B11A03_3</t>
+  </si>
+  <si>
+    <t>_6444048F-4C8B-11D1-8B70-080036B11A03_4</t>
+  </si>
+  <si>
+    <t>_14B81DA1-0135-4D31-96D9-6CBFC9671A99_37378</t>
+  </si>
+  <si>
+    <t>_14B81DA1-0135-4D31-96D9-6CBFC9671A99_36867</t>
+  </si>
+  <si>
+    <t>_F85BF840-A925-4BC2-B0C4-8E36B598679E_100</t>
+  </si>
+  <si>
+    <t>_14B81DA1-0135-4D31-96D9-6CBFC9671A99_18248</t>
+  </si>
+  <si>
+    <t>_14B81DA1-0135-4D31-96D9-6CBFC9671A99_37380</t>
+  </si>
+  <si>
+    <t>_14B81DA1-0135-4D31-96D9-6CBFC9671A99_33434</t>
+  </si>
+  <si>
+    <t>_2D152B40-CA39-40DB-B2CC-573725B2FEC5_100</t>
+  </si>
+  <si>
+    <t>_14B81DA1-0135-4D31-96D9-6CBFC9671A99_37386</t>
+  </si>
+  <si>
+    <t>_14B81DA1-0135-4D31-96D9-6CBFC9671A99_34855</t>
+  </si>
+  <si>
+    <t>_14B81DA1-0135-4D31-96D9-6CBFC9671A99_37383</t>
+  </si>
+  <si>
+    <t>_E8309B6E-084C-49B4-B1FC-90A80331B638_100</t>
+  </si>
+  <si>
+    <t>_14B81DA1-0135-4D31-96D9-6CBFC9671A99_37377</t>
+  </si>
+  <si>
+    <t>_14B81DA1-0135-4D31-96D9-6CBFC9671A99_37382</t>
+  </si>
+  <si>
+    <t>_EE3D3D8A-5381-4CFA-B13B-AAF66B5F4EC9_100</t>
+  </si>
+  <si>
+    <t>_A0E74609-B84D-4F49-B860-462BD9971F98_100</t>
+  </si>
+  <si>
+    <t>_D35F743A-EB2E-47F2-A286-844132CB1427_100</t>
+  </si>
+  <si>
+    <t>_14B81DA1-0135-4D31-96D9-6CBFC9671A99_34850</t>
+  </si>
+  <si>
+    <t>_14B81DA1-0135-4D31-96D9-6CBFC9671A99}_33437</t>
+  </si>
+  <si>
+    <t>_E6DDCAF7-29C5-4F0A-9A68-D19412EC7090_100</t>
+  </si>
+  <si>
+    <t>_E1277516-2B5F-4869-89B1-2E585BD38B7A_100</t>
+  </si>
+  <si>
+    <t>_6D217F6D-3F6A-4825-B470-5F03CA2FBE9B_100</t>
+  </si>
+  <si>
+    <t>_49237325-A95A-4F67-B211-816B2D45D2E0_100</t>
+  </si>
+  <si>
+    <t>_64440492-4C8B-11D1-8B70-080036B11A03_27</t>
+  </si>
+  <si>
+    <t>_64440492-4C8B-11D1-8B70-080036B11A03_28</t>
+  </si>
+  <si>
+    <t>_2E4B640D-5019-46D8-8881-55414CC5CAA0_100</t>
+  </si>
+  <si>
+    <t>_64440490-4C8B-11D1-8B70-080036B11A03_3</t>
+  </si>
+  <si>
+    <t>_64440492-4C8B-11D1-8B70-080036B11A03_36</t>
+  </si>
+  <si>
+    <t>_6444048F-4C8B-11D1-8B70-080036B11A03_12</t>
+  </si>
+  <si>
+    <t>_64440492-4C8B-11D1-8B70-080036B11A03_22</t>
+  </si>
+  <si>
+    <t>_64440492-4C8B-11D1-8B70-080036B11A03_39</t>
+  </si>
+  <si>
+    <t>_64440492-4C8B-11D1-8B70-080036B11A03_30</t>
+  </si>
+  <si>
+    <t>_56A3372E-CE9C-11D2-9F0E-006097C686F6_38</t>
+  </si>
+  <si>
+    <t>_64440492-4C8B-11D1-8B70-080036B11A03_23</t>
+  </si>
+  <si>
+    <t>_64440492-4C8B-11D1-8B70-080036B11A03_21</t>
+  </si>
+  <si>
+    <t>_64440491-4C8B-11D1-8B70-080036B11A03_10</t>
+  </si>
+  <si>
+    <t>_64440492-4C8B-11D1-8B70-080036B11A03_20</t>
+  </si>
+  <si>
+    <t>_64440491-4C8B-11D1-8B70-080036B11A03_8</t>
+  </si>
+  <si>
+    <t>_64440491-4C8B-11D1-8B70-080036B11A03_44</t>
+  </si>
+  <si>
+    <t>_64440491-4C8B-11D1-8B70-080036B11A03_42</t>
+  </si>
+  <si>
+    <t>_64440491-4C8B-11D1-8B70-080036B11A03_45</t>
+  </si>
+  <si>
+    <t>_64440491-4C8B-11D1-8B70-080036B11A03_43</t>
+  </si>
+  <si>
+    <t>_0CEF7D53-FA64-11D1-A203-0000F81FEDEE_3</t>
+  </si>
+  <si>
+    <t>_0CEF7D53-FA64-11D1-A203-0000F81FEDEE_4</t>
+  </si>
+  <si>
+    <t>_841E4F90-FF59-4D16-8947-E81BBFFAB36D_16</t>
+  </si>
+  <si>
+    <t>_0CEF7D53-FA64-11D1-A203-0000F81FEDEE_7</t>
+  </si>
+  <si>
+    <t>_0CEF7D53-FA64-11D1-A203-0000F81FEDEE_8</t>
+  </si>
+  <si>
+    <t>_D5CDD502-2E9C-101B-9397-08002B2CF9AE_29</t>
+  </si>
+  <si>
+    <t>_64440492-4C8B-11D1-8B70-080036B11A03_11</t>
+  </si>
+  <si>
+    <t>_6D748DE2-8D38-4CC3-AC60-F009B057C557_7</t>
+  </si>
+  <si>
+    <t>_6D748DE2-8D38-4CC3-AC60-F009B057C557_2</t>
+  </si>
+  <si>
+    <t>_6D748DE2-8D38-4CC3-AC60-F009B057C557_12</t>
+  </si>
+  <si>
+    <t>_6D748DE2-8D38-4CC3-AC60-F009B057C557_17</t>
+  </si>
+  <si>
+    <t>_6D748DE2-8D38-4CC3-AC60-F009B057C557_18</t>
+  </si>
+  <si>
+    <t>_6D748DE2-8D38-4CC3-AC60-F009B057C557_13</t>
+  </si>
+  <si>
+    <t>_2C53C813-FB63-4E22-A1AB-0B331CA1E273_100</t>
+  </si>
+  <si>
+    <t>_4684FE97-8765-4842-9C13-F006447B178C_100</t>
+  </si>
+  <si>
+    <t>_6D748DE2-8D38-4CC3-AC60-F009B057C557_3</t>
+  </si>
+  <si>
+    <t>_A5477F61-7A82-4ECA-9DDE-98B69B2479B3_100</t>
+  </si>
+  <si>
+    <t>_2CBAA8F5-D81F-47CA-B17A-F8D822300131_100</t>
+  </si>
+  <si>
+    <t>_43F8D7B7-A444-4F87-9383-52271C9B915C_100</t>
+  </si>
+  <si>
+    <t>_14B81DA1-0135-4D31-96D9-6CBFC9671A99_18258</t>
+  </si>
+  <si>
+    <t>_72FAB781-ACDA-43E5-B155-B2434F85E678_100</t>
+  </si>
+  <si>
+    <t>_DE41CC29-6971-4290-B472-F59F2E2F31E2_100</t>
+  </si>
+  <si>
+    <t>_5CBF2787-48CF-4208-B90E-EE5E5D420294_23</t>
+  </si>
+  <si>
+    <t>_64440492-4C8B-11D1-8B70-080036B11A03_9</t>
+  </si>
+  <si>
+    <t>_000214A1-0000-0000-C000-000000000046_9</t>
+  </si>
+  <si>
+    <t>_28636AA6-953D-11D2-B5D6-00C04FD918D0_14</t>
+  </si>
+  <si>
+    <t>Document last saved</t>
+  </si>
+  <si>
+    <t>Date/time file was last saved, from SummaryInfo propset (Office Docs)</t>
+  </si>
+  <si>
+    <t>Total time spent editting document</t>
+  </si>
+  <si>
+    <t>Document edit time</t>
+  </si>
+  <si>
+    <t>Date/time file was originally created</t>
+  </si>
+  <si>
+    <t>Document created</t>
+  </si>
+  <si>
+    <t>Total number of pages in document</t>
+  </si>
+  <si>
+    <t>Document total pages</t>
+  </si>
+  <si>
+    <t>Total number of characters in document</t>
+  </si>
+  <si>
+    <t>Document character count</t>
+  </si>
+  <si>
+    <t>Total number of words in document</t>
+  </si>
+  <si>
+    <t>Document total words</t>
+  </si>
+  <si>
+    <t>Access control information</t>
+  </si>
+  <si>
+    <t>D5CDD502-2E9C-101B-9397-08002B2CF9AE/8</t>
+  </si>
+  <si>
+    <t>_D5CDD502-2E9C-101B-9397-08002B2CF9AE_8</t>
+  </si>
+  <si>
+    <t>D5CDD502-2E9C-101B-9397-08002B2CF9AE/9</t>
+  </si>
+  <si>
+    <t>_D5CDD502-2E9C-101B-9397-08002B2CF9AE_9</t>
+  </si>
+  <si>
+    <t>D5CDD502-2E9C-101B-9397-08002B2CF9AE/10</t>
+  </si>
+  <si>
+    <t>_D5CDD502-2E9C-101B-9397-08002B2CF9AE_10</t>
+  </si>
+  <si>
+    <t>D5CDD502-2E9C-101B-9397-08002B2CF9AE/11</t>
+  </si>
+  <si>
+    <t>_D5CDD502-2E9C-101B-9397-08002B2CF9AE_11</t>
+  </si>
+  <si>
+    <t>D5CDD502-2E9C-101B-9397-08002B2CF9AE/12</t>
+  </si>
+  <si>
+    <t>_D5CDD502-2E9C-101B-9397-08002B2CF9AE_12</t>
+  </si>
+  <si>
+    <t>D5CDD502-2E9C-101B-9397-08002B2CF9AE/13</t>
+  </si>
+  <si>
+    <t>_D5CDD502-2E9C-101B-9397-08002B2CF9AE_13</t>
+  </si>
+  <si>
+    <t>D5CDD502-2E9C-101B-9397-08002B2CF9AE/16</t>
+  </si>
+  <si>
+    <t>_D5CDD502-2E9C-101B-9397-08002B2CF9AE_16</t>
+  </si>
+  <si>
+    <t>D5CDD502-2E9C-101B-9397-08002B2CF9AE/17</t>
+  </si>
+  <si>
+    <t>_D5CDD502-2E9C-101B-9397-08002B2CF9AE_17</t>
+  </si>
+  <si>
+    <t>D5CDD502-2E9C-101B-9397-08002B2CF9AE/18</t>
+  </si>
+  <si>
+    <t>_D5CDD502-2E9C-101B-9397-08002B2CF9AE_18</t>
+  </si>
+  <si>
+    <t>D5CDD502-2E9C-101B-9397-08002B2CF9AE/19</t>
+  </si>
+  <si>
+    <t>_D5CDD502-2E9C-101B-9397-08002B2CF9AE_19</t>
+  </si>
+  <si>
+    <t>D5CDD502-2E9C-101B-9397-08002B2CF9AE/22</t>
+  </si>
+  <si>
+    <t>_D5CDD502-2E9C-101B-9397-08002B2CF9AE_22</t>
+  </si>
+  <si>
+    <t>D5CDD502-2E9C-101B-9397-08002B2CF9AE/23</t>
+  </si>
+  <si>
+    <t>_D5CDD502-2E9C-101B-9397-08002B2CF9AE_23</t>
+  </si>
+  <si>
+    <t>D5CDD502-2E9C-101B-9397-08002B2CF9AE/27</t>
+  </si>
+  <si>
+    <t>_D5CDD502-2E9C-101B-9397-08002B2CF9AE_27</t>
+  </si>
+  <si>
+    <t>D5CDD502-2E9C-101B-9397-08002B2CF9AE/28</t>
+  </si>
+  <si>
+    <t>_D5CDD502-2E9C-101B-9397-08002B2CF9AE_28</t>
+  </si>
+  <si>
+    <t>D5CDD505-2E9C-101B-9397-08002B2CF9AE/_PID_HLINKS</t>
+  </si>
+  <si>
+    <t>_D5CDD505-2E9C-101B-9397-08002B2CF9AE__PID_HLINKS</t>
+  </si>
+  <si>
+    <t>D5CDD505-2E9C-101B-9397-08002B2CF9AE/_SHAREDFILEINDEX</t>
+  </si>
+  <si>
+    <t>_D5CDD505-2E9C-101B-9397-08002B2CF9AE__SHAREDFILEINDEX</t>
+  </si>
+  <si>
+    <t>D5CDD505-2E9C-101B-9397-08002B2CF9AE/_SOURCEURL</t>
+  </si>
+  <si>
+    <t>_D5CDD505-2E9C-101B-9397-08002B2CF9AE__SOURCEURL</t>
+  </si>
+  <si>
+    <t>D5CDD505-2E9C-101B-9397-08002B2CF9AE/CONTENTTYPE</t>
+  </si>
+  <si>
+    <t>_D5CDD505-2E9C-101B-9397-08002B2CF9AE_CONTENTTYPE</t>
+  </si>
+  <si>
+    <t>D5CDD505-2E9C-101B-9397-08002B2CF9AE/CONTENTTYPEID</t>
+  </si>
+  <si>
+    <t>_D5CDD505-2E9C-101B-9397-08002B2CF9AE_CONTENTTYPEID</t>
   </si>
 </sst>
 </file>
@@ -1631,7 +2867,18 @@
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1907,17 +3154,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E137"/>
+  <dimension ref="A1:E272"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+    <sheetView tabSelected="1" topLeftCell="C250" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:D272"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="26.06640625" customWidth="1"/>
-    <col min="2" max="2" width="21.1328125" customWidth="1"/>
-    <col min="3" max="3" width="17.73046875" customWidth="1"/>
+    <col min="1" max="1" width="65" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="63.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="99.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="94.46484375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1953,7 +3200,7 @@
         <v>243</v>
       </c>
       <c r="E2" t="str">
-        <f t="shared" ref="E2:E65" si="0">CONCATENATE("_properties.Add(""",A2,""", LanguageConsts.",B2,");")</f>
+        <f>CONCATENATE("_properties.Add(""",A2,""", LanguageConsts.",B2,");")</f>
         <v>_properties.Add("0B63E350-9CCC-11D0-BCDB-00805FCCCE04/5", LanguageConsts._0B63E350_9CCC_11D0_BCDB_00805FCCCE04_5);</v>
       </c>
     </row>
@@ -1971,7 +3218,7 @@
         <v>100</v>
       </c>
       <c r="E3" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("_properties.Add(""",A3,""", LanguageConsts.",B3,");")</f>
         <v>_properties.Add("14B81DA1-0135-4D31-96D9-6CBFC9671A99/271", LanguageConsts._14B81DA1_0135_4D31_96D9_6CBFC9671A99_271);</v>
       </c>
     </row>
@@ -1989,7 +3236,7 @@
         <v>101</v>
       </c>
       <c r="E4" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("_properties.Add(""",A4,""", LanguageConsts.",B4,");")</f>
         <v>_properties.Add("14B81DA1-0135-4D31-96D9-6CBFC9671A99/272", LanguageConsts._14B81DA1_0135_4D31_96D9_6CBFC9671A99_272);</v>
       </c>
     </row>
@@ -2007,7 +3254,7 @@
         <v>103</v>
       </c>
       <c r="E5" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("_properties.Add(""",A5,""", LanguageConsts.",B5,");")</f>
         <v>_properties.Add("14B81DA1-0135-4D31-96D9-6CBFC9671A99/274", LanguageConsts._14B81DA1_0135_4D31_96D9_6CBFC9671A99_274);</v>
       </c>
     </row>
@@ -2025,7 +3272,7 @@
         <v>240</v>
       </c>
       <c r="E6" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("_properties.Add(""",A6,""", LanguageConsts.",B6,");")</f>
         <v>_properties.Add("49691C90-7E17-101A-A91C-08002B2ECDA9/9", LanguageConsts._49691C90_7E17_101A_A91C_08002B2ECDA9_9);</v>
       </c>
     </row>
@@ -2043,7 +3290,7 @@
         <v>97</v>
       </c>
       <c r="E7" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("_properties.Add(""",A7,""", LanguageConsts.",B7,");")</f>
         <v>_properties.Add("56A3372E-CE9C-11D2-9F0E-006097C686F6/11", LanguageConsts._56A3372E_CE9C_11D2_9F0E_006097C686F6_11);</v>
       </c>
     </row>
@@ -2061,7 +3308,7 @@
         <v>96</v>
       </c>
       <c r="E8" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("_properties.Add(""",A8,""", LanguageConsts.",B8,");")</f>
         <v>_properties.Add("56A3372E-CE9C-11D2-9F0E-006097C686F6/2", LanguageConsts._56A3372E_CE9C_11D2_9F0E_006097C686F6_2);</v>
       </c>
     </row>
@@ -2079,7 +3326,7 @@
         <v>95</v>
       </c>
       <c r="E9" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("_properties.Add(""",A9,""", LanguageConsts.",B9,");")</f>
         <v>_properties.Add("56A3372E-CE9C-11D2-9F0E-006097C686F6/4", LanguageConsts._56A3372E_CE9C_11D2_9F0E_006097C686F6_4);</v>
       </c>
     </row>
@@ -2097,7 +3344,7 @@
         <v>99</v>
       </c>
       <c r="E10" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("_properties.Add(""",A10,""", LanguageConsts.",B10,");")</f>
         <v>_properties.Add("56A3372E-CE9C-11D2-9F0E-006097C686F6/5", LanguageConsts._56A3372E_CE9C_11D2_9F0E_006097C686F6_5);</v>
       </c>
     </row>
@@ -2115,7 +3362,7 @@
         <v>98</v>
       </c>
       <c r="E11" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("_properties.Add(""",A11,""", LanguageConsts.",B11,");")</f>
         <v>_properties.Add("56A3372E-CE9C-11D2-9F0E-006097C686F6/7", LanguageConsts._56A3372E_CE9C_11D2_9F0E_006097C686F6_7);</v>
       </c>
     </row>
@@ -2133,7 +3380,7 @@
         <v>94</v>
       </c>
       <c r="E12" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("_properties.Add(""",A12,""", LanguageConsts.",B12,");")</f>
         <v>_properties.Add("56A3372E-CE9C-11D2-9F0E-006097C686F6/8", LanguageConsts._56A3372E_CE9C_11D2_9F0E_006097C686F6_8);</v>
       </c>
     </row>
@@ -2151,7 +3398,7 @@
         <v>104</v>
       </c>
       <c r="E13" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("_properties.Add(""",A13,""", LanguageConsts.",B13,");")</f>
         <v>_properties.Add("6444048F-4C8B-11D1-8B70-080036B11A03/13", LanguageConsts._6444048F_4C8B_11D1_8B70_080036B11A03_13);</v>
       </c>
     </row>
@@ -2169,7 +3416,7 @@
         <v>105</v>
       </c>
       <c r="E14" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("_properties.Add(""",A14,""", LanguageConsts.",B14,");")</f>
         <v>_properties.Add("6444048F-4C8B-11D1-8B70-080036B11A03/5", LanguageConsts._6444048F_4C8B_11D1_8B70_080036B11A03_5);</v>
       </c>
     </row>
@@ -2187,7 +3434,7 @@
         <v>106</v>
       </c>
       <c r="E15" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("_properties.Add(""",A15,""", LanguageConsts.",B15,");")</f>
         <v>_properties.Add("6444048F-4C8B-11D1-8B70-080036B11A03/6", LanguageConsts._6444048F_4C8B_11D1_8B70_080036B11A03_6);</v>
       </c>
     </row>
@@ -2205,7 +3452,7 @@
         <v>93</v>
       </c>
       <c r="E16" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("_properties.Add(""",A16,""", LanguageConsts.",B16,");")</f>
         <v>_properties.Add("64440490-4C8B-11D1-8B70-080036B11A03/4", LanguageConsts._64440490_4C8B_11D1_8B70_080036B11A03_4);</v>
       </c>
     </row>
@@ -2223,7 +3470,7 @@
         <v>109</v>
       </c>
       <c r="E17" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("_properties.Add(""",A17,""", LanguageConsts.",B17,");")</f>
         <v>_properties.Add("64440491-4C8B-11D1-8B70-080036B11A03/3", LanguageConsts._64440491_4C8B_11D1_8B70_080036B11A03_3);</v>
       </c>
     </row>
@@ -2241,7 +3488,7 @@
         <v>107</v>
       </c>
       <c r="E18" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("_properties.Add(""",A18,""", LanguageConsts.",B18,");")</f>
         <v>_properties.Add("64440491-4C8B-11D1-8B70-080036B11A03/4", LanguageConsts._64440491_4C8B_11D1_8B70_080036B11A03_4);</v>
       </c>
     </row>
@@ -2259,7 +3506,7 @@
         <v>108</v>
       </c>
       <c r="E19" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("_properties.Add(""",A19,""", LanguageConsts.",B19,");")</f>
         <v>_properties.Add("64440491-4C8B-11D1-8B70-080036B11A03/6", LanguageConsts._64440491_4C8B_11D1_8B70_080036B11A03_6);</v>
       </c>
     </row>
@@ -2277,7 +3524,7 @@
         <v>111</v>
       </c>
       <c r="E20" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("_properties.Add(""",A20,""", LanguageConsts.",B20,");")</f>
         <v>_properties.Add("8DEE0300-16C2-101B-B121-08002B2ECDA9/CLASS", LanguageConsts._8DEE0300_16C2_101B_B121_08002B2ECDA9_class);</v>
       </c>
     </row>
@@ -2295,7 +3542,7 @@
         <v>133</v>
       </c>
       <c r="E21" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("_properties.Add(""",A21,""", LanguageConsts.",B21,");")</f>
         <v>_properties.Add("8DEE0300-16C2-101B-B121-08002B2ECDA9/COMPONENT", LanguageConsts._8DEE0300_16C2_101B_B121_08002B2ECDA9_component);</v>
       </c>
     </row>
@@ -2313,7 +3560,7 @@
         <v>125</v>
       </c>
       <c r="E22" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("_properties.Add(""",A22,""", LanguageConsts.",B22,");")</f>
         <v>_properties.Add("8DEE0300-16C2-101B-B121-08002B2ECDA9/CONST", LanguageConsts._8DEE0300_16C2_101B_B121_08002B2ECDA9_const);</v>
       </c>
     </row>
@@ -2331,7 +3578,7 @@
         <v>131</v>
       </c>
       <c r="E23" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("_properties.Add(""",A23,""", LanguageConsts.",B23,");")</f>
         <v>_properties.Add("8DEE0300-16C2-101B-B121-08002B2ECDA9/DEF", LanguageConsts._8DEE0300_16C2_101B_B121_08002B2ECDA9_def);</v>
       </c>
     </row>
@@ -2349,7 +3596,7 @@
         <v>119</v>
       </c>
       <c r="E24" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("_properties.Add(""",A24,""", LanguageConsts.",B24,");")</f>
         <v>_properties.Add("8DEE0300-16C2-101B-B121-08002B2ECDA9/DELEGATE", LanguageConsts._8DEE0300_16C2_101B_B121_08002B2ECDA9_delegate);</v>
       </c>
     </row>
@@ -2367,7 +3614,7 @@
         <v>123</v>
       </c>
       <c r="E25" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("_properties.Add(""",A25,""", LanguageConsts.",B25,");")</f>
         <v>_properties.Add("8DEE0300-16C2-101B-B121-08002B2ECDA9/ENUM", LanguageConsts._8DEE0300_16C2_101B_B121_08002B2ECDA9_enum);</v>
       </c>
     </row>
@@ -2385,7 +3632,7 @@
         <v>127</v>
       </c>
       <c r="E26" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("_properties.Add(""",A26,""", LanguageConsts.",B26,");")</f>
         <v>_properties.Add("8DEE0300-16C2-101B-B121-08002B2ECDA9/EVENT", LanguageConsts._8DEE0300_16C2_101B_B121_08002B2ECDA9_event);</v>
       </c>
     </row>
@@ -2403,7 +3650,7 @@
         <v>129</v>
       </c>
       <c r="E27" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("_properties.Add(""",A27,""", LanguageConsts.",B27,");")</f>
         <v>_properties.Add("8DEE0300-16C2-101B-B121-08002B2ECDA9/FIELD", LanguageConsts._8DEE0300_16C2_101B_B121_08002B2ECDA9_field);</v>
       </c>
     </row>
@@ -2421,7 +3668,7 @@
         <v>113</v>
       </c>
       <c r="E28" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("_properties.Add(""",A28,""", LanguageConsts.",B28,");")</f>
         <v>_properties.Add("8DEE0300-16C2-101B-B121-08002B2ECDA9/FUNC", LanguageConsts._8DEE0300_16C2_101B_B121_08002B2ECDA9_func);</v>
       </c>
     </row>
@@ -2439,7 +3686,7 @@
         <v>117</v>
       </c>
       <c r="E29" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("_properties.Add(""",A29,""", LanguageConsts.",B29,");")</f>
         <v>_properties.Add("8DEE0300-16C2-101B-B121-08002B2ECDA9/INTERFACE", LanguageConsts._8DEE0300_16C2_101B_B121_08002B2ECDA9_interface);</v>
       </c>
     </row>
@@ -2457,7 +3704,7 @@
         <v>135</v>
       </c>
       <c r="E30" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("_properties.Add(""",A30,""", LanguageConsts.",B30,");")</f>
         <v>_properties.Add("8DEE0300-16C2-101B-B121-08002B2ECDA9/PROJECT", LanguageConsts._8DEE0300_16C2_101B_B121_08002B2ECDA9_project);</v>
       </c>
     </row>
@@ -2475,7 +3722,7 @@
         <v>121</v>
       </c>
       <c r="E31" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("_properties.Add(""",A31,""", LanguageConsts.",B31,");")</f>
         <v>_properties.Add("8DEE0300-16C2-101B-B121-08002B2ECDA9/PROPERTY", LanguageConsts._8DEE0300_16C2_101B_B121_08002B2ECDA9_property);</v>
       </c>
     </row>
@@ -2493,7 +3740,7 @@
         <v>137</v>
       </c>
       <c r="E32" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("_properties.Add(""",A32,""", LanguageConsts.",B32,");")</f>
         <v>_properties.Add("8DEE0300-16C2-101B-B121-08002B2ECDA9/SOLUTION", LanguageConsts._8DEE0300_16C2_101B_B121_08002B2ECDA9_solution);</v>
       </c>
     </row>
@@ -2511,7 +3758,7 @@
         <v>115</v>
       </c>
       <c r="E33" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("_properties.Add(""",A33,""", LanguageConsts.",B33,");")</f>
         <v>_properties.Add("8DEE0300-16C2-101B-B121-08002B2ECDA9/STRUCT", LanguageConsts._8DEE0300_16C2_101B_B121_08002B2ECDA9_struct);</v>
       </c>
     </row>
@@ -2529,7 +3776,7 @@
         <v>37</v>
       </c>
       <c r="E34" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("_properties.Add(""",A34,""", LanguageConsts.",B34,");")</f>
         <v>_properties.Add("B725F130-47EF-101A-A5F1-02608C9EEBAC/10", LanguageConsts._B725F130_47EF_101A_A5F1_02608C9EEBAC_10);</v>
       </c>
     </row>
@@ -2547,7 +3794,7 @@
         <v>17</v>
       </c>
       <c r="E35" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("_properties.Add(""",A35,""", LanguageConsts.",B35,");")</f>
         <v>_properties.Add("B725F130-47EF-101A-A5F1-02608C9EEBAC/12", LanguageConsts._B725F130_47EF_101A_A5F1_02608C9EEBAC_12);</v>
       </c>
     </row>
@@ -2565,7 +3812,7 @@
         <v>21</v>
       </c>
       <c r="E36" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("_properties.Add(""",A36,""", LanguageConsts.",B36,");")</f>
         <v>_properties.Add("B725F130-47EF-101A-A5F1-02608C9EEBAC/14", LanguageConsts._B725F130_47EF_101A_A5F1_02608C9EEBAC_14);</v>
       </c>
     </row>
@@ -2583,7 +3830,7 @@
         <v>1</v>
       </c>
       <c r="E37" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("_properties.Add(""",A37,""", LanguageConsts.",B37,");")</f>
         <v>_properties.Add("B725F130-47EF-101A-A5F1-02608C9EEBAC/15", LanguageConsts._B725F130_47EF_101A_A5F1_02608C9EEBAC_15);</v>
       </c>
     </row>
@@ -2601,7 +3848,7 @@
         <v>38</v>
       </c>
       <c r="E38" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("_properties.Add(""",A38,""", LanguageConsts.",B38,");")</f>
         <v>_properties.Add("B725F130-47EF-101A-A5F1-02608C9EEBAC/20", LanguageConsts._B725F130_47EF_101A_A5F1_02608C9EEBAC_20);</v>
       </c>
     </row>
@@ -2619,7 +3866,7 @@
         <v>90</v>
       </c>
       <c r="E39" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("_properties.Add(""",A39,""", LanguageConsts.",B39,");")</f>
         <v>_properties.Add("D5CDD502-2E9C-101B-9397-08002B2CF9AE/14", LanguageConsts._D5CDD502_2E9C_101B_9397_08002B2CF9AE_14);</v>
       </c>
     </row>
@@ -2637,7 +3884,7 @@
         <v>88</v>
       </c>
       <c r="E40" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("_properties.Add(""",A40,""", LanguageConsts.",B40,");")</f>
         <v>_properties.Add("D5CDD502-2E9C-101B-9397-08002B2CF9AE/15", LanguageConsts._D5CDD502_2E9C_101B_9397_08002B2CF9AE_15);</v>
       </c>
     </row>
@@ -2655,7 +3902,7 @@
         <v>3</v>
       </c>
       <c r="E41" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("_properties.Add(""",A41,""", LanguageConsts.",B41,");")</f>
         <v>_properties.Add("D5CDD502-2E9C-101B-9397-08002B2CF9AE/2", LanguageConsts._D5CDD502_2E9C_101B_9397_08002B2CF9AE_2);</v>
       </c>
     </row>
@@ -2673,7 +3920,7 @@
         <v>91</v>
       </c>
       <c r="E42" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("_properties.Add(""",A42,""", LanguageConsts.",B42,");")</f>
         <v>_properties.Add("D5CDD502-2E9C-101B-9397-08002B2CF9AE/3", LanguageConsts._D5CDD502_2E9C_101B_9397_08002B2CF9AE_3);</v>
       </c>
     </row>
@@ -2691,7 +3938,7 @@
         <v>92</v>
       </c>
       <c r="E43" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("_properties.Add(""",A43,""", LanguageConsts.",B43,");")</f>
         <v>_properties.Add("D5CDD502-2E9C-101B-9397-08002B2CF9AE/7", LanguageConsts._D5CDD502_2E9C_101B_9397_08002B2CF9AE_7);</v>
       </c>
     </row>
@@ -2709,7 +3956,7 @@
         <v>59</v>
       </c>
       <c r="E44" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("_properties.Add(""",A44,""", LanguageConsts.",B44,");")</f>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/ANNIVERSARY", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_Anniversary);</v>
       </c>
     </row>
@@ -2727,7 +3974,7 @@
         <v>60</v>
       </c>
       <c r="E45" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("_properties.Add(""",A45,""", LanguageConsts.",B45,");")</f>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/ASSISTANTNAME", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_AssistantName);</v>
       </c>
     </row>
@@ -2745,7 +3992,7 @@
         <v>61</v>
       </c>
       <c r="E46" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("_properties.Add(""",A46,""", LanguageConsts.",B46,");")</f>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/ASSISTANTTELEPHONE", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_AssistantTelephone);</v>
       </c>
     </row>
@@ -2763,7 +4010,7 @@
         <v>39</v>
       </c>
       <c r="E47" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("_properties.Add(""",A47,""", LanguageConsts.",B47,");")</f>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/ATTACHMENTNAMES", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_AttachmentNames);</v>
       </c>
     </row>
@@ -2781,7 +4028,7 @@
         <v>40</v>
       </c>
       <c r="E48" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("_properties.Add(""",A48,""", LanguageConsts.",B48,");")</f>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/BCCADDRESS", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_BccAddress);</v>
       </c>
     </row>
@@ -2799,7 +4046,7 @@
         <v>41</v>
       </c>
       <c r="E49" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("_properties.Add(""",A49,""", LanguageConsts.",B49,");")</f>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/BCCNAME", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_BccName);</v>
       </c>
     </row>
@@ -2817,7 +4064,7 @@
         <v>63</v>
       </c>
       <c r="E50" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("_properties.Add(""",A50,""", LanguageConsts.",B50,");")</f>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/BIRTHDAY", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_Birthday);</v>
       </c>
     </row>
@@ -2835,7 +4082,7 @@
         <v>64</v>
       </c>
       <c r="E51" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("_properties.Add(""",A51,""", LanguageConsts.",B51,");")</f>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/BUSINESSADDRESSCITY", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_BusinessAddressCity);</v>
       </c>
     </row>
@@ -2853,7 +4100,7 @@
         <v>64</v>
       </c>
       <c r="E52" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("_properties.Add(""",A52,""", LanguageConsts.",B52,");")</f>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/BUSINESSADDRESSCOUNTRY", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_BusinessAddressCountry);</v>
       </c>
     </row>
@@ -2871,7 +4118,7 @@
         <v>64</v>
       </c>
       <c r="E53" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("_properties.Add(""",A53,""", LanguageConsts.",B53,");")</f>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/BUSINESSADDRESSPOSTALCODE", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_BusinessAddressPostalCode);</v>
       </c>
     </row>
@@ -2889,7 +4136,7 @@
         <v>64</v>
       </c>
       <c r="E54" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("_properties.Add(""",A54,""", LanguageConsts.",B54,");")</f>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/BUSINESSADDRESSPOSTOFFICEBOX", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_BusinessAddressPostOfficeBox);</v>
       </c>
     </row>
@@ -2907,7 +4154,7 @@
         <v>64</v>
       </c>
       <c r="E55" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("_properties.Add(""",A55,""", LanguageConsts.",B55,");")</f>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/BUSINESSADDRESSSTATE", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_BusinessAddressState);</v>
       </c>
     </row>
@@ -2925,7 +4172,7 @@
         <v>64</v>
       </c>
       <c r="E56" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("_properties.Add(""",A56,""", LanguageConsts.",B56,");")</f>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/BUSINESSADDRESSSTREET", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_BusinessAddressStreet);</v>
       </c>
     </row>
@@ -2943,7 +4190,7 @@
         <v>77</v>
       </c>
       <c r="E57" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("_properties.Add(""",A57,""", LanguageConsts.",B57,");")</f>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/BUSINESSFAXNUMBER", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_BusinessFaxNumber);</v>
       </c>
     </row>
@@ -2961,7 +4208,7 @@
         <v>65</v>
       </c>
       <c r="E58" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("_properties.Add(""",A58,""", LanguageConsts.",B58,");")</f>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/CALLBACKTELEPHONE", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_CallbackTelephone);</v>
       </c>
     </row>
@@ -2979,7 +4226,7 @@
         <v>66</v>
       </c>
       <c r="E59" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("_properties.Add(""",A59,""", LanguageConsts.",B59,");")</f>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/CARTELEPHONE", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_CarTelephone);</v>
       </c>
     </row>
@@ -2997,7 +4244,7 @@
         <v>42</v>
       </c>
       <c r="E60" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("_properties.Add(""",A60,""", LanguageConsts.",B60,");")</f>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/CCADDRESS", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_CcAddress);</v>
       </c>
     </row>
@@ -3015,7 +4262,7 @@
         <v>43</v>
       </c>
       <c r="E61" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("_properties.Add(""",A61,""", LanguageConsts.",B61,");")</f>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/CCNAME", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_CcName);</v>
       </c>
     </row>
@@ -3033,7 +4280,7 @@
         <v>68</v>
       </c>
       <c r="E62" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("_properties.Add(""",A62,""", LanguageConsts.",B62,");")</f>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/CHILDREN", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_Children);</v>
       </c>
     </row>
@@ -3051,7 +4298,7 @@
         <v>66</v>
       </c>
       <c r="E63" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("_properties.Add(""",A63,""", LanguageConsts.",B63,");")</f>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/COMPANYMAINTELEPHONE", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_CompanyMainTelephone);</v>
       </c>
     </row>
@@ -3069,7 +4316,7 @@
         <v>32</v>
       </c>
       <c r="E64" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("_properties.Add(""",A64,""", LanguageConsts.",B64,");")</f>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/CONTAINERHASH", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_ContainerHash);</v>
       </c>
     </row>
@@ -3087,7 +4334,7 @@
         <v>44</v>
       </c>
       <c r="E65" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("_properties.Add(""",A65,""", LanguageConsts.",B65,");")</f>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/CONVERSATIONID", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_ConversationID);</v>
       </c>
     </row>
@@ -3105,7 +4352,7 @@
         <v>102</v>
       </c>
       <c r="E66" t="str">
-        <f t="shared" ref="E66:E129" si="1">CONCATENATE("_properties.Add(""",A66,""", LanguageConsts.",B66,");")</f>
+        <f>CONCATENATE("_properties.Add(""",A66,""", LanguageConsts.",B66,");")</f>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/DATETAKEN", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_DateTaken);</v>
       </c>
     </row>
@@ -3123,7 +4370,7 @@
         <v>241</v>
       </c>
       <c r="E67" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("_properties.Add(""",A67,""", LanguageConsts.",B67,");")</f>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/DISPLAYFOLDER", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_DisplayFolder);</v>
       </c>
     </row>
@@ -3141,7 +4388,7 @@
         <v>5</v>
       </c>
       <c r="E68" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("_properties.Add(""",A68,""", LanguageConsts.",B68,");")</f>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/DOCTITLEPREFIX", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_DocTitlePrefix);</v>
       </c>
     </row>
@@ -3159,7 +4406,7 @@
         <v>22</v>
       </c>
       <c r="E69" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("_properties.Add(""",A69,""", LanguageConsts.",B69,");")</f>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/DUEDATE", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_DueDate);</v>
       </c>
     </row>
@@ -3177,7 +4424,7 @@
         <v>55</v>
       </c>
       <c r="E70" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("_properties.Add(""",A70,""", LanguageConsts.",B70,");")</f>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/DURATION", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_Duration);</v>
       </c>
     </row>
@@ -3195,7 +4442,7 @@
         <v>69</v>
       </c>
       <c r="E71" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("_properties.Add(""",A71,""", LanguageConsts.",B71,");")</f>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/EMAILADDRESS", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_EmailAddress);</v>
       </c>
     </row>
@@ -3213,7 +4460,7 @@
         <v>70</v>
       </c>
       <c r="E72" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("_properties.Add(""",A72,""", LanguageConsts.",B72,");")</f>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/EMAILNAME", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_EmailName);</v>
       </c>
     </row>
@@ -3231,7 +4478,7 @@
         <v>244</v>
       </c>
       <c r="E73" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("_properties.Add(""",A73,""", LanguageConsts.",B73,");")</f>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/ENDDATE", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_EndDate);</v>
       </c>
     </row>
@@ -3249,7 +4496,7 @@
         <v>36</v>
       </c>
       <c r="E74" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("_properties.Add(""",A74,""", LanguageConsts.",B74,");")</f>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/FILEEXT", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_FileExt);</v>
       </c>
     </row>
@@ -3267,7 +4514,7 @@
         <v>242</v>
       </c>
       <c r="E75" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("_properties.Add(""",A75,""", LanguageConsts.",B75,");")</f>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/FILEEXTDESC", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_FileExtDesc);</v>
       </c>
     </row>
@@ -3285,7 +4532,7 @@
         <v>71</v>
       </c>
       <c r="E76" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("_properties.Add(""",A76,""", LanguageConsts.",B76,");")</f>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/FIRSTNAME", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_FirstName);</v>
       </c>
     </row>
@@ -3303,7 +4550,7 @@
         <v>26</v>
       </c>
       <c r="E77" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("_properties.Add(""",A77,""", LanguageConsts.",B77,");")</f>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/FLAGTEXT", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_FlagText);</v>
       </c>
     </row>
@@ -3321,7 +4568,7 @@
         <v>7</v>
       </c>
       <c r="E78" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("_properties.Add(""",A78,""", LanguageConsts.",B78,");")</f>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/FOLDERNAME", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_FolderName);</v>
       </c>
     </row>
@@ -3339,7 +4586,7 @@
         <v>45</v>
       </c>
       <c r="E79" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("_properties.Add(""",A79,""", LanguageConsts.",B79,");")</f>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/FROMADDRESS", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_FromAddress);</v>
       </c>
     </row>
@@ -3357,7 +4604,7 @@
         <v>46</v>
       </c>
       <c r="E80" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("_properties.Add(""",A80,""", LanguageConsts.",B80,");")</f>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/FROMNAME", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_FromName);</v>
       </c>
     </row>
@@ -3375,7 +4622,7 @@
         <v>72</v>
       </c>
       <c r="E81" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("_properties.Add(""",A81,""", LanguageConsts.",B81,");")</f>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/FULLNAME", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_FullName);</v>
       </c>
     </row>
@@ -3393,7 +4640,7 @@
         <v>47</v>
       </c>
       <c r="E82" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("_properties.Add(""",A82,""", LanguageConsts.",B82,");")</f>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/FWDRPLY", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_FwdRply);</v>
       </c>
     </row>
@@ -3411,7 +4658,7 @@
         <v>245</v>
       </c>
       <c r="E83" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("_properties.Add(""",A83,""", LanguageConsts.",B83,");")</f>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/GENDER", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_Gender);</v>
       </c>
     </row>
@@ -3429,7 +4676,7 @@
         <v>48</v>
       </c>
       <c r="E84" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("_properties.Add(""",A84,""", LanguageConsts.",B84,");")</f>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/HASATTACH", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_HasAttach);</v>
       </c>
     </row>
@@ -3447,7 +4694,7 @@
         <v>75</v>
       </c>
       <c r="E85" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("_properties.Add(""",A85,""", LanguageConsts.",B85,");")</f>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/HOBBY", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_Hobby);</v>
       </c>
     </row>
@@ -3465,7 +4712,7 @@
         <v>76</v>
       </c>
       <c r="E86" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("_properties.Add(""",A86,""", LanguageConsts.",B86,");")</f>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/HOMEADDRESSCITY", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_HomeAddressCity);</v>
       </c>
     </row>
@@ -3483,7 +4730,7 @@
         <v>76</v>
       </c>
       <c r="E87" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("_properties.Add(""",A87,""", LanguageConsts.",B87,");")</f>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/HOMEADDRESSCOUNTRY", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_HomeAddressCountry);</v>
       </c>
     </row>
@@ -3501,7 +4748,7 @@
         <v>76</v>
       </c>
       <c r="E88" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("_properties.Add(""",A88,""", LanguageConsts.",B88,");")</f>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/HOMEADDRESSPOSTALCODE", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_HomeAddressPostalCode);</v>
       </c>
     </row>
@@ -3519,7 +4766,7 @@
         <v>76</v>
       </c>
       <c r="E89" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("_properties.Add(""",A89,""", LanguageConsts.",B89,");")</f>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/HOMEADDRESSSTATE", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_HomeAddressState);</v>
       </c>
     </row>
@@ -3537,7 +4784,7 @@
         <v>76</v>
       </c>
       <c r="E90" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("_properties.Add(""",A90,""", LanguageConsts.",B90,");")</f>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/HOMEADDRESSSTREET", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_HomeAddressStreet);</v>
       </c>
     </row>
@@ -3555,7 +4802,7 @@
         <v>77</v>
       </c>
       <c r="E91" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("_properties.Add(""",A91,""", LanguageConsts.",B91,");")</f>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/HOMEFAXNUMBER", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_HomeFaxNumber);</v>
       </c>
     </row>
@@ -3573,7 +4820,7 @@
         <v>66</v>
       </c>
       <c r="E92" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("_properties.Add(""",A92,""", LanguageConsts.",B92,");")</f>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/HOMETELEPHONE", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_HomeTelephone);</v>
       </c>
     </row>
@@ -3591,7 +4838,7 @@
         <v>28</v>
       </c>
       <c r="E93" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("_properties.Add(""",A93,""", LanguageConsts.",B93,");")</f>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/IDENTITY", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_Identity);</v>
       </c>
     </row>
@@ -3609,7 +4856,7 @@
         <v>78</v>
       </c>
       <c r="E94" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("_properties.Add(""",A94,""", LanguageConsts.",B94,");")</f>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/IMADDRESS", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_IMAddress);</v>
       </c>
     </row>
@@ -3627,7 +4874,7 @@
         <v>31</v>
       </c>
       <c r="E95" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("_properties.Add(""",A95,""", LanguageConsts.",B95,");")</f>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/IMPORTANCE", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_Importance);</v>
       </c>
     </row>
@@ -3645,7 +4892,7 @@
         <v>8</v>
       </c>
       <c r="E96" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("_properties.Add(""",A96,""", LanguageConsts.",B96,");")</f>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/ISATTACHMENT", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_IsAttachment);</v>
       </c>
     </row>
@@ -3663,7 +4910,7 @@
         <v>9</v>
       </c>
       <c r="E97" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("_properties.Add(""",A97,""", LanguageConsts.",B97,");")</f>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/ISDELETED", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_IsDeleted);</v>
       </c>
     </row>
@@ -3681,7 +4928,7 @@
         <v>25</v>
       </c>
       <c r="E98" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("_properties.Add(""",A98,""", LanguageConsts.",B98,");")</f>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/ISFLAGGED", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_IsFlagged);</v>
       </c>
     </row>
@@ -3699,7 +4946,7 @@
         <v>24</v>
       </c>
       <c r="E99" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("_properties.Add(""",A99,""", LanguageConsts.",B99,");")</f>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/ISFLAGGEDCOMPLETED", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_IsFlaggedCompleted);</v>
       </c>
     </row>
@@ -3717,7 +4964,7 @@
         <v>23</v>
       </c>
       <c r="E100" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("_properties.Add(""",A100,""", LanguageConsts.",B100,");")</f>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/ISINCOMPLETE", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_IsIncomplete);</v>
       </c>
     </row>
@@ -3735,7 +4982,7 @@
         <v>29</v>
       </c>
       <c r="E101" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("_properties.Add(""",A101,""", LanguageConsts.",B101,");")</f>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/ISREAD", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_IsRead);</v>
       </c>
     </row>
@@ -3753,7 +5000,7 @@
         <v>53</v>
       </c>
       <c r="E102" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("_properties.Add(""",A102,""", LanguageConsts.",B102,");")</f>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/ISRECURRING", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_IsRecurring);</v>
       </c>
     </row>
@@ -3771,7 +5018,7 @@
         <v>79</v>
       </c>
       <c r="E103" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("_properties.Add(""",A103,""", LanguageConsts.",B103,");")</f>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/JOBTITLE", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_JobTitle);</v>
       </c>
     </row>
@@ -3789,7 +5036,7 @@
         <v>75</v>
       </c>
       <c r="E104" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("_properties.Add(""",A104,""", LanguageConsts.",B104,");")</f>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/LASTNAME", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_LastName);</v>
       </c>
     </row>
@@ -3807,7 +5054,7 @@
         <v>10</v>
       </c>
       <c r="E105" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("_properties.Add(""",A105,""", LanguageConsts.",B105,");")</f>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/LASTVIEWED", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_LastViewed);</v>
       </c>
     </row>
@@ -3825,7 +5072,7 @@
         <v>57</v>
       </c>
       <c r="E106" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("_properties.Add(""",A106,""", LanguageConsts.",B106,");")</f>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/LOCATION", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_Location);</v>
       </c>
     </row>
@@ -3843,7 +5090,7 @@
         <v>75</v>
       </c>
       <c r="E107" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("_properties.Add(""",A107,""", LanguageConsts.",B107,");")</f>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/MIDDLENAME", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_MiddleName);</v>
       </c>
     </row>
@@ -3861,7 +5108,7 @@
         <v>66</v>
       </c>
       <c r="E108" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("_properties.Add(""",A108,""", LanguageConsts.",B108,");")</f>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/MOBILETELEPHONE", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_MobileTelephone);</v>
       </c>
     </row>
@@ -3879,7 +5126,7 @@
         <v>75</v>
       </c>
       <c r="E109" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("_properties.Add(""",A109,""", LanguageConsts.",B109,");")</f>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/NICKNAME", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_NickName);</v>
       </c>
     </row>
@@ -3897,7 +5144,7 @@
         <v>75</v>
       </c>
       <c r="E110" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("_properties.Add(""",A110,""", LanguageConsts.",B110,");")</f>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/OFFICE", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_Office);</v>
       </c>
     </row>
@@ -3915,7 +5162,7 @@
         <v>66</v>
       </c>
       <c r="E111" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("_properties.Add(""",A111,""", LanguageConsts.",B111,");")</f>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/OFFICETELEPHONE", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_OfficeTelephone);</v>
       </c>
     </row>
@@ -3933,7 +5180,7 @@
         <v>66</v>
       </c>
       <c r="E112" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("_properties.Add(""",A112,""", LanguageConsts.",B112,");")</f>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/PAGERTELEPHONE", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_PagerTelephone);</v>
       </c>
     </row>
@@ -3951,7 +5198,7 @@
         <v>12</v>
       </c>
       <c r="E113" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("_properties.Add(""",A113,""", LanguageConsts.",B113,");")</f>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/PEOPLE", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_People);</v>
       </c>
     </row>
@@ -3969,7 +5216,7 @@
         <v>13</v>
       </c>
       <c r="E114" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("_properties.Add(""",A114,""", LanguageConsts.",B114,");")</f>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/PERCEIVEDTYPE", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_PerceivedType);</v>
       </c>
     </row>
@@ -3987,7 +5234,7 @@
         <v>14</v>
       </c>
       <c r="E115" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("_properties.Add(""",A115,""", LanguageConsts.",B115,");")</f>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/PERCEIVEDTYPENAME", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_PerceivedTypeName);</v>
       </c>
     </row>
@@ -4005,7 +5252,7 @@
         <v>81</v>
       </c>
       <c r="E116" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("_properties.Add(""",A116,""", LanguageConsts.",B116,");")</f>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/PERSONALTITLE", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_PersonalTitle);</v>
       </c>
     </row>
@@ -4023,7 +5270,7 @@
         <v>15</v>
       </c>
       <c r="E117" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("_properties.Add(""",A117,""", LanguageConsts.",B117,");")</f>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/PRIMARYDATE", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_PrimaryDate);</v>
       </c>
     </row>
@@ -4041,7 +5288,7 @@
         <v>66</v>
       </c>
       <c r="E118" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("_properties.Add(""",A118,""", LanguageConsts.",B118,");")</f>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/PRIMARYTELEPHONE", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_PrimaryTelephone);</v>
       </c>
     </row>
@@ -4059,7 +5306,7 @@
         <v>75</v>
       </c>
       <c r="E119" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("_properties.Add(""",A119,""", LanguageConsts.",B119,");")</f>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/PROFESSION", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_Profession);</v>
       </c>
     </row>
@@ -4077,7 +5324,7 @@
         <v>49</v>
       </c>
       <c r="E120" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("_properties.Add(""",A120,""", LanguageConsts.",B120,");")</f>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/RECEIVEDDATE", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_ReceivedDate);</v>
       </c>
     </row>
@@ -4095,7 +5342,7 @@
         <v>75</v>
       </c>
       <c r="E121" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("_properties.Add(""",A121,""", LanguageConsts.",B121,");")</f>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/SPOUSE", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_Spouse);</v>
       </c>
     </row>
@@ -4113,7 +5360,7 @@
         <v>246</v>
       </c>
       <c r="E122" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("_properties.Add(""",A122,""", LanguageConsts.",B122,");")</f>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/STARTDATE", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_StartDate);</v>
       </c>
     </row>
@@ -4131,7 +5378,7 @@
         <v>35</v>
       </c>
       <c r="E123" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("_properties.Add(""",A123,""", LanguageConsts.",B123,");")</f>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/STORE", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_Store);</v>
       </c>
     </row>
@@ -4149,7 +5396,7 @@
         <v>75</v>
       </c>
       <c r="E124" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("_properties.Add(""",A124,""", LanguageConsts.",B124,");")</f>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/SUFFIX", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_Suffix);</v>
       </c>
     </row>
@@ -4167,7 +5414,7 @@
         <v>52</v>
       </c>
       <c r="E125" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("_properties.Add(""",A125,""", LanguageConsts.",B125,");")</f>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/TASKSTATUS", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_TaskStatus);</v>
       </c>
     </row>
@@ -4185,7 +5432,7 @@
         <v>85</v>
       </c>
       <c r="E126" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("_properties.Add(""",A126,""", LanguageConsts.",B126,");")</f>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/TELEXNUMBER", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_TelexNumber);</v>
       </c>
     </row>
@@ -4203,7 +5450,7 @@
         <v>50</v>
       </c>
       <c r="E127" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("_properties.Add(""",A127,""", LanguageConsts.",B127,");")</f>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/TOADDRESS", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_ToAddress);</v>
       </c>
     </row>
@@ -4221,7 +5468,7 @@
         <v>51</v>
       </c>
       <c r="E128" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("_properties.Add(""",A128,""", LanguageConsts.",B128,");")</f>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/TONAME", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_ToName);</v>
       </c>
     </row>
@@ -4239,7 +5486,7 @@
         <v>247</v>
       </c>
       <c r="E129" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("_properties.Add(""",A129,""", LanguageConsts.",B129,");")</f>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/TTYTDDTELEPHONE", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_TTYTDDTelephone);</v>
       </c>
     </row>
@@ -4257,140 +5504,2189 @@
         <v>87</v>
       </c>
       <c r="E130" t="str">
-        <f t="shared" ref="E130:E137" si="2">CONCATENATE("_properties.Add(""",A130,""", LanguageConsts.",B130,");")</f>
+        <f>CONCATENATE("_properties.Add(""",A130,""", LanguageConsts.",B130,");")</f>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/WEBPAGE", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_WebPage);</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A131" t="s">
-        <v>487</v>
+        <v>392</v>
       </c>
       <c r="B131" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="C131" t="s">
-        <v>179</v>
+        <v>144</v>
       </c>
       <c r="D131" t="s">
-        <v>89</v>
+        <v>6</v>
       </c>
       <c r="E131" t="str">
-        <f t="shared" si="2"/>
-        <v>_properties.Add("F29F85E0-4FF9-1068-AB91-08002B27B3D9/11", LanguageConsts._F29F85E0_4FF9_1068_AB91_08002B27B3D9_11);</v>
+        <f>CONCATENATE("_properties.Add(""",A131,""", LanguageConsts.",B131,");")</f>
+        <v>_properties.Add("F29F85E0-4FF9-1068-AB91-08002B27B3D9/2", LanguageConsts._F29F85E0_4FF9_1068_AB91_08002B27B3D9_2);</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A132" t="s">
-        <v>392</v>
+        <v>403</v>
       </c>
       <c r="B132" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="C132" t="s">
-        <v>144</v>
+        <v>178</v>
       </c>
       <c r="D132" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="E132" t="str">
-        <f t="shared" si="2"/>
-        <v>_properties.Add("F29F85E0-4FF9-1068-AB91-08002B27B3D9/2", LanguageConsts._F29F85E0_4FF9_1068_AB91_08002B27B3D9_2);</v>
+        <f>CONCATENATE("_properties.Add(""",A132,""", LanguageConsts.",B132,");")</f>
+        <v>_properties.Add("F29F85E0-4FF9-1068-AB91-08002B27B3D9/3", LanguageConsts._F29F85E0_4FF9_1068_AB91_08002B27B3D9_3);</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A133" t="s">
-        <v>403</v>
+        <v>388</v>
       </c>
       <c r="B133" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="C133" t="s">
-        <v>178</v>
+        <v>140</v>
       </c>
       <c r="D133" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="E133" t="str">
-        <f t="shared" si="2"/>
-        <v>_properties.Add("F29F85E0-4FF9-1068-AB91-08002B27B3D9/3", LanguageConsts._F29F85E0_4FF9_1068_AB91_08002B27B3D9_3);</v>
+        <f>CONCATENATE("_properties.Add(""",A133,""", LanguageConsts.",B133,");")</f>
+        <v>_properties.Add("F29F85E0-4FF9-1068-AB91-08002B27B3D9/4", LanguageConsts._F29F85E0_4FF9_1068_AB91_08002B27B3D9_4);</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A134" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="B134" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="C134" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D134" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E134" t="str">
-        <f t="shared" si="2"/>
-        <v>_properties.Add("F29F85E0-4FF9-1068-AB91-08002B27B3D9/4", LanguageConsts._F29F85E0_4FF9_1068_AB91_08002B27B3D9_4);</v>
+        <f>CONCATENATE("_properties.Add(""",A134,""", LanguageConsts.",B134,");")</f>
+        <v>_properties.Add("F29F85E0-4FF9-1068-AB91-08002B27B3D9/5", LanguageConsts._F29F85E0_4FF9_1068_AB91_08002B27B3D9_5);</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A135" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="B135" t="s">
-        <v>383</v>
+        <v>248</v>
       </c>
       <c r="C135" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="D135" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E135" t="str">
-        <f t="shared" si="2"/>
-        <v>_properties.Add("F29F85E0-4FF9-1068-AB91-08002B27B3D9/5", LanguageConsts._F29F85E0_4FF9_1068_AB91_08002B27B3D9_5);</v>
+        <f>CONCATENATE("_properties.Add(""",A135,""", LanguageConsts.",B135,");")</f>
+        <v>_properties.Add("F29F85E0-4FF9-1068-AB91-08002B27B3D9/6", LanguageConsts._F29F85E0_4FF9_1068_AB91_08002B27B3D9_6);</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A136" t="s">
-        <v>385</v>
+        <v>486</v>
       </c>
       <c r="B136" t="s">
-        <v>248</v>
+        <v>384</v>
       </c>
       <c r="C136" t="s">
-        <v>138</v>
+        <v>177</v>
       </c>
       <c r="D136" t="s">
-        <v>0</v>
+        <v>239</v>
       </c>
       <c r="E136" t="str">
-        <f t="shared" si="2"/>
-        <v>_properties.Add("F29F85E0-4FF9-1068-AB91-08002B27B3D9/6", LanguageConsts._F29F85E0_4FF9_1068_AB91_08002B27B3D9_6);</v>
+        <f>CONCATENATE("_properties.Add(""",A136,""", LanguageConsts.",B136,");")</f>
+        <v>_properties.Add("F29F85E0-4FF9-1068-AB91-08002B27B3D9/8", LanguageConsts._F29F85E0_4FF9_1068_AB91_08002B27B3D9_8);</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A137" t="s">
-        <v>486</v>
+        <v>543</v>
       </c>
       <c r="B137" t="s">
-        <v>384</v>
+        <v>551</v>
       </c>
       <c r="C137" t="s">
-        <v>177</v>
+        <v>886</v>
       </c>
       <c r="D137" t="s">
-        <v>239</v>
+        <v>885</v>
       </c>
       <c r="E137" t="str">
+        <f t="shared" ref="E137:E200" si="0">CONCATENATE("_properties.Add(""",A137,""", LanguageConsts.",B137,");")</f>
+        <v>_properties.Add("F29F85E0-4FF9-1068-AB91-08002B27B3D9/10", LanguageConsts._F29F85E0_4FF9_1068_AB91_08002B27B3D9_10);</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A138" t="s">
+        <v>487</v>
+      </c>
+      <c r="B138" t="s">
+        <v>379</v>
+      </c>
+      <c r="C138" t="s">
+        <v>179</v>
+      </c>
+      <c r="D138" t="s">
+        <v>89</v>
+      </c>
+      <c r="E138" t="str">
+        <f t="shared" si="0"/>
+        <v>_properties.Add("F29F85E0-4FF9-1068-AB91-08002B27B3D9/11", LanguageConsts._F29F85E0_4FF9_1068_AB91_08002B27B3D9_11);</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A139" t="s">
+        <v>544</v>
+      </c>
+      <c r="B139" t="s">
+        <v>552</v>
+      </c>
+      <c r="C139" t="s">
+        <v>888</v>
+      </c>
+      <c r="D139" t="s">
+        <v>887</v>
+      </c>
+      <c r="E139" t="str">
+        <f t="shared" si="0"/>
+        <v>_properties.Add("F29F85E0-4FF9-1068-AB91-08002B27B3D9/12", LanguageConsts._F29F85E0_4FF9_1068_AB91_08002B27B3D9_12);</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A140" t="s">
+        <v>545</v>
+      </c>
+      <c r="B140" t="s">
+        <v>553</v>
+      </c>
+      <c r="C140" t="s">
+        <v>883</v>
+      </c>
+      <c r="D140" t="s">
+        <v>884</v>
+      </c>
+      <c r="E140" t="str">
+        <f t="shared" si="0"/>
+        <v>_properties.Add("F29F85E0-4FF9-1068-AB91-08002B27B3D9/13", LanguageConsts._F29F85E0_4FF9_1068_AB91_08002B27B3D9_13);</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A141" t="s">
+        <v>546</v>
+      </c>
+      <c r="B141" t="s">
+        <v>554</v>
+      </c>
+      <c r="C141" t="s">
+        <v>890</v>
+      </c>
+      <c r="D141" t="s">
+        <v>889</v>
+      </c>
+      <c r="E141" t="str">
+        <f t="shared" si="0"/>
+        <v>_properties.Add("F29F85E0-4FF9-1068-AB91-08002B27B3D9/14", LanguageConsts._F29F85E0_4FF9_1068_AB91_08002B27B3D9_14);</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A142" t="s">
+        <v>547</v>
+      </c>
+      <c r="B142" t="s">
+        <v>555</v>
+      </c>
+      <c r="C142" t="s">
+        <v>894</v>
+      </c>
+      <c r="D142" t="s">
+        <v>893</v>
+      </c>
+      <c r="E142" t="str">
+        <f t="shared" si="0"/>
+        <v>_properties.Add("F29F85E0-4FF9-1068-AB91-08002B27B3D9/15", LanguageConsts._F29F85E0_4FF9_1068_AB91_08002B27B3D9_15);</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A143" t="s">
+        <v>548</v>
+      </c>
+      <c r="B143" t="s">
+        <v>556</v>
+      </c>
+      <c r="C143" t="s">
+        <v>892</v>
+      </c>
+      <c r="D143" t="s">
+        <v>891</v>
+      </c>
+      <c r="E143" t="str">
+        <f t="shared" si="0"/>
+        <v>_properties.Add("F29F85E0-4FF9-1068-AB91-08002B27B3D9/16", LanguageConsts._F29F85E0_4FF9_1068_AB91_08002B27B3D9_16);</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A144" t="s">
+        <v>549</v>
+      </c>
+      <c r="B144" t="s">
+        <v>557</v>
+      </c>
+      <c r="C144" t="s">
+        <v>541</v>
+      </c>
+      <c r="E144" t="str">
+        <f t="shared" si="0"/>
+        <v>_properties.Add("F29F85E0-4FF9-1068-AB91-08002B27B3D9/18", LanguageConsts._F29F85E0_4FF9_1068_AB91_08002B27B3D9_18);</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A145" t="s">
+        <v>550</v>
+      </c>
+      <c r="B145" t="s">
+        <v>558</v>
+      </c>
+      <c r="C145" t="s">
+        <v>542</v>
+      </c>
+      <c r="D145" t="s">
+        <v>895</v>
+      </c>
+      <c r="E145" t="str">
+        <f t="shared" si="0"/>
+        <v>_properties.Add("F29F85E0-4FF9-1068-AB91-08002B27B3D9/19", LanguageConsts._F29F85E0_4FF9_1068_AB91_08002B27B3D9_19);</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A146" t="s">
+        <v>667</v>
+      </c>
+      <c r="B146" t="s">
+        <v>775</v>
+      </c>
+      <c r="C146" t="s">
+        <v>559</v>
+      </c>
+      <c r="E146" t="str">
+        <f t="shared" si="0"/>
+        <v>_properties.Add("F7DB74B4-4287-4103-AFBA-F1B13DCD75CF/100", LanguageConsts._F7DB74B4-4287-4103-AFBA-F1B13DCD75CF_100);</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A147" t="s">
+        <v>668</v>
+      </c>
+      <c r="B147" t="s">
+        <v>776</v>
+      </c>
+      <c r="C147" t="s">
+        <v>560</v>
+      </c>
+      <c r="E147" t="str">
+        <f t="shared" si="0"/>
+        <v>_properties.Add("28636AA6-953D-11D2-B5D6-00C04FD918D0/11", LanguageConsts._28636AA6-953D-11D2-B5D6-00C04FD918D0_11);</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A148" t="s">
+        <v>669</v>
+      </c>
+      <c r="B148" t="s">
+        <v>777</v>
+      </c>
+      <c r="C148" t="s">
+        <v>561</v>
+      </c>
+      <c r="E148" t="str">
+        <f t="shared" si="0"/>
+        <v>_properties.Add("D5CDD502-2E9C-101B-9397-08002B2CF9AE/26", LanguageConsts._D5CDD502-2E9C-101B-9397-08002B2CF9AE_26);</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A149" t="s">
+        <v>670</v>
+      </c>
+      <c r="B149" t="s">
+        <v>778</v>
+      </c>
+      <c r="C149" t="s">
+        <v>562</v>
+      </c>
+      <c r="E149" t="str">
+        <f t="shared" si="0"/>
+        <v>_properties.Add("1E3EE840-BC2B-476C-8237-2ACD1A839B22/3", LanguageConsts._1E3EE840-BC2B-476C-8237-2ACD1A839B22_3);</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A150" t="s">
+        <v>671</v>
+      </c>
+      <c r="B150" t="s">
+        <v>779</v>
+      </c>
+      <c r="C150" t="s">
+        <v>563</v>
+      </c>
+      <c r="E150" t="str">
+        <f t="shared" si="0"/>
+        <v>_properties.Add("E4F10A3C-49E6-405D-8288-A23BD4EEAA6C/100", LanguageConsts._E4F10A3C-49E6-405D-8288-A23BD4EEAA6C_100);</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A151" t="s">
+        <v>672</v>
+      </c>
+      <c r="B151" t="s">
+        <v>780</v>
+      </c>
+      <c r="C151" t="s">
+        <v>564</v>
+      </c>
+      <c r="E151" t="str">
+        <f t="shared" si="0"/>
+        <v>_properties.Add("28636AA6-953D-11D2-B5D6-00C04FD918D0/12", LanguageConsts._28636AA6-953D-11D2-B5D6-00C04FD918D0_12);</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A152" t="s">
+        <v>673</v>
+      </c>
+      <c r="B152" t="s">
+        <v>781</v>
+      </c>
+      <c r="C152" t="s">
+        <v>565</v>
+      </c>
+      <c r="E152" t="str">
+        <f t="shared" si="0"/>
+        <v>_properties.Add("EF884C5B-2BFE-41BB-AAE5-76EEDF4F9902/100", LanguageConsts._EF884C5B-2BFE-41BB-AAE5-76EEDF4F9902_100);</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A153" t="s">
+        <v>674</v>
+      </c>
+      <c r="B153" t="s">
+        <v>782</v>
+      </c>
+      <c r="C153" t="s">
+        <v>566</v>
+      </c>
+      <c r="E153" t="str">
+        <f t="shared" si="0"/>
+        <v>_properties.Add("EF884C5B-2BFE-41BB-AAE5-76EEDF4F9902/200", LanguageConsts._EF884C5B-2BFE-41BB-AAE5-76EEDF4F9902_200);</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A154" t="s">
+        <v>675</v>
+      </c>
+      <c r="B154" t="s">
+        <v>783</v>
+      </c>
+      <c r="C154" t="s">
+        <v>567</v>
+      </c>
+      <c r="E154" t="str">
+        <f t="shared" si="0"/>
+        <v>_properties.Add("EF884C5B-2BFE-41BB-AAE5-76EEDF4F9902/300", LanguageConsts._EF884C5B-2BFE-41BB-AAE5-76EEDF4F9902_300);</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A155" t="s">
+        <v>676</v>
+      </c>
+      <c r="B155" t="s">
+        <v>784</v>
+      </c>
+      <c r="C155" t="s">
+        <v>568</v>
+      </c>
+      <c r="E155" t="str">
+        <f t="shared" si="0"/>
+        <v>_properties.Add("B725F130-47EF-101A-A5F1-02608C9EEBAC/16", LanguageConsts._B725F130-47EF-101A-A5F1-02608C9EEBAC_16);</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A156" t="s">
+        <v>677</v>
+      </c>
+      <c r="B156" t="s">
+        <v>785</v>
+      </c>
+      <c r="C156" t="s">
+        <v>569</v>
+      </c>
+      <c r="E156" t="str">
+        <f t="shared" si="0"/>
+        <v>_properties.Add("B725F130-47EF-101A-A5F1-02608C9EEBAC/13", LanguageConsts._B725F130-47EF-101A-A5F1-02608C9EEBAC_13);</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A157" t="s">
+        <v>678</v>
+      </c>
+      <c r="B157" t="s">
+        <v>786</v>
+      </c>
+      <c r="C157" t="s">
+        <v>570</v>
+      </c>
+      <c r="E157" t="str">
+        <f t="shared" si="0"/>
+        <v>_properties.Add("9B174B34-40FF-11D2-A27E-00C04FC30871/4", LanguageConsts._9B174B34-40FF-11D2-A27E-00C04FC30871_4);</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A158" t="s">
+        <v>679</v>
+      </c>
+      <c r="B158" t="s">
+        <v>787</v>
+      </c>
+      <c r="C158" t="s">
+        <v>571</v>
+      </c>
+      <c r="E158" t="str">
+        <f t="shared" si="0"/>
+        <v>_properties.Add("28636AA6-953D-11D2-B5D6-00C04FD918D0/5", LanguageConsts._28636AA6-953D-11D2-B5D6-00C04FD918D0_5);</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A159" t="s">
+        <v>680</v>
+      </c>
+      <c r="B159" t="s">
+        <v>788</v>
+      </c>
+      <c r="C159" t="s">
+        <v>572</v>
+      </c>
+      <c r="E159" t="str">
+        <f t="shared" si="0"/>
+        <v>_properties.Add("90E5E14E-648B-4826-B2AA-ACAF790E3513/10", LanguageConsts._90E5E14E-648B-4826-B2AA-ACAF790E3513_10);</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A160" t="s">
+        <v>681</v>
+      </c>
+      <c r="B160" t="s">
+        <v>789</v>
+      </c>
+      <c r="C160" t="s">
+        <v>573</v>
+      </c>
+      <c r="E160" t="str">
+        <f t="shared" si="0"/>
+        <v>_properties.Add("A94688B6-7D9F-4570-A648-E3DFC0AB2B3F/100", LanguageConsts._A94688B6-7D9F-4570-A648-E3DFC0AB2B3F_100);</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A161" t="s">
+        <v>682</v>
+      </c>
+      <c r="B161" t="s">
+        <v>790</v>
+      </c>
+      <c r="C161" t="s">
+        <v>574</v>
+      </c>
+      <c r="E161" t="str">
+        <f t="shared" si="0"/>
+        <v>_properties.Add("6D24888F-4718-4BDA-AFED-EA0FB4386CD8/100", LanguageConsts._6D24888F-4718-4BDA-AFED-EA0FB4386CD8_100);</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A162" t="s">
+        <v>683</v>
+      </c>
+      <c r="B162" t="s">
+        <v>791</v>
+      </c>
+      <c r="C162" t="s">
+        <v>575</v>
+      </c>
+      <c r="E162" t="str">
+        <f t="shared" si="0"/>
+        <v>_properties.Add("B9B4B3FC-2B51-4A42-B5D8-324146AFCF25/2", LanguageConsts._B9B4B3FC-2B51-4A42-B5D8-324146AFCF25_2);</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A163" t="s">
+        <v>684</v>
+      </c>
+      <c r="B163" t="s">
+        <v>792</v>
+      </c>
+      <c r="C163" t="s">
+        <v>576</v>
+      </c>
+      <c r="E163" t="str">
+        <f t="shared" si="0"/>
+        <v>_properties.Add("E3E0584C-B788-4A5A-BB20-7F5A44C9ACDD/6", LanguageConsts._E3E0584C-B788-4A5A-BB20-7F5A44C9ACDD_6);</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A164" t="s">
+        <v>685</v>
+      </c>
+      <c r="B164" t="s">
+        <v>793</v>
+      </c>
+      <c r="C164" t="s">
+        <v>577</v>
+      </c>
+      <c r="E164" t="str">
+        <f t="shared" si="0"/>
+        <v>_properties.Add("49691C90-7E17-101A-A91C-08002B2ECDA9}/3", LanguageConsts._49691C90-7E17-101A-A91C-08002B2ECDA9}_3);</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A165" t="s">
+        <v>686</v>
+      </c>
+      <c r="B165" t="s">
+        <v>794</v>
+      </c>
+      <c r="C165" t="s">
+        <v>578</v>
+      </c>
+      <c r="E165" t="str">
+        <f t="shared" si="0"/>
+        <v>_properties.Add("64440490-4C8B-11D1-8B70-080036B11A03/7", LanguageConsts._64440490-4C8B-11D1-8B70-080036B11A03_7);</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A166" t="s">
+        <v>687</v>
+      </c>
+      <c r="B166" t="s">
+        <v>795</v>
+      </c>
+      <c r="C166" t="s">
+        <v>579</v>
+      </c>
+      <c r="E166" t="str">
+        <f t="shared" si="0"/>
+        <v>_properties.Add("64440490-4C8B-11D1-8B70-080036B11A03/5", LanguageConsts._64440490-4C8B-11D1-8B70-080036B11A03_5);</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A167" t="s">
+        <v>688</v>
+      </c>
+      <c r="B167" t="s">
+        <v>796</v>
+      </c>
+      <c r="C167" t="s">
+        <v>580</v>
+      </c>
+      <c r="E167" t="str">
+        <f t="shared" si="0"/>
+        <v>_properties.Add("64440490-4C8B-11D1-8B70-080036B11A03/8", LanguageConsts._64440490-4C8B-11D1-8B70-080036B11A03_8);</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A168" t="s">
+        <v>689</v>
+      </c>
+      <c r="B168" t="s">
+        <v>797</v>
+      </c>
+      <c r="C168" t="s">
+        <v>581</v>
+      </c>
+      <c r="E168" t="str">
+        <f t="shared" si="0"/>
+        <v>_properties.Add("56A3372E-CE9C-11D2-9F0E-006097C686F6/13", LanguageConsts._56A3372E-CE9C-11D2-9F0E-006097C686F6_13);</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A169" t="s">
+        <v>690</v>
+      </c>
+      <c r="B169" t="s">
+        <v>798</v>
+      </c>
+      <c r="C169" t="s">
+        <v>582</v>
+      </c>
+      <c r="E169" t="str">
+        <f t="shared" si="0"/>
+        <v>_properties.Add("56A3372E-CE9C-11D2-9F0E-006097C686F6/100", LanguageConsts._56A3372E-CE9C-11D2-9F0E-006097C686F6_100);</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A170" t="s">
+        <v>691</v>
+      </c>
+      <c r="B170" t="s">
+        <v>799</v>
+      </c>
+      <c r="C170" t="s">
+        <v>583</v>
+      </c>
+      <c r="E170" t="str">
+        <f t="shared" si="0"/>
+        <v>_properties.Add("FD122953-FA93-4EF7-92C3-04C946B2F7C8/100", LanguageConsts._FD122953-FA93-4EF7-92C3-04C946B2F7C8_100);</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A171" t="s">
+        <v>692</v>
+      </c>
+      <c r="B171" t="s">
+        <v>800</v>
+      </c>
+      <c r="C171" t="s">
+        <v>584</v>
+      </c>
+      <c r="E171" t="str">
+        <f t="shared" si="0"/>
+        <v>_properties.Add("56A3372E-CE9C-11D2-9F0E-006097C686F6/35", LanguageConsts._56A3372E-CE9C-11D2-9F0E-006097C686F6_35);</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A172" t="s">
+        <v>693</v>
+      </c>
+      <c r="B172" t="s">
+        <v>801</v>
+      </c>
+      <c r="C172" t="s">
+        <v>585</v>
+      </c>
+      <c r="E172" t="str">
+        <f t="shared" si="0"/>
+        <v>_properties.Add("64440492-4C8B-11D1-8B70-080036B11A03/19", LanguageConsts._64440492-4C8B-11D1-8B70-080036B11A03_19);</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A173" t="s">
+        <v>694</v>
+      </c>
+      <c r="B173" t="s">
+        <v>802</v>
+      </c>
+      <c r="C173" t="s">
+        <v>586</v>
+      </c>
+      <c r="E173" t="str">
+        <f t="shared" si="0"/>
+        <v>_properties.Add("56A3372E-CE9C-11D2-9F0E-006097C686F6/36", LanguageConsts._56A3372E-CE9C-11D2-9F0E-006097C686F6_36);</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A174" t="s">
+        <v>695</v>
+      </c>
+      <c r="B174" t="s">
+        <v>803</v>
+      </c>
+      <c r="C174" t="s">
+        <v>587</v>
+      </c>
+      <c r="E174" t="str">
+        <f t="shared" si="0"/>
+        <v>_properties.Add("56A3372E-CE9C-11D2-9F0E-006097C686F6/12", LanguageConsts._56A3372E-CE9C-11D2-9F0E-006097C686F6_12);</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A175" t="s">
+        <v>696</v>
+      </c>
+      <c r="B175" t="s">
+        <v>804</v>
+      </c>
+      <c r="C175" t="s">
+        <v>588</v>
+      </c>
+      <c r="E175" t="str">
+        <f t="shared" si="0"/>
+        <v>_properties.Add("56A3372E-CE9C-11D2-9F0E-006097C686F6/39", LanguageConsts._56A3372E-CE9C-11D2-9F0E-006097C686F6_39);</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A176" t="s">
+        <v>697</v>
+      </c>
+      <c r="B176" t="s">
+        <v>805</v>
+      </c>
+      <c r="C176" t="s">
+        <v>590</v>
+      </c>
+      <c r="E176" t="str">
+        <f t="shared" si="0"/>
+        <v>_properties.Add("56A3372E-CE9C-11D2-9F0E-006097C686F6/37", LanguageConsts._56A3372E-CE9C-11D2-9F0E-006097C686F6_37);</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A177" t="s">
+        <v>698</v>
+      </c>
+      <c r="B177" t="s">
+        <v>806</v>
+      </c>
+      <c r="C177" t="s">
+        <v>591</v>
+      </c>
+      <c r="E177" t="str">
+        <f t="shared" si="0"/>
+        <v>_properties.Add("D0A04F0A-462A-48A4-BB2F-3706E88DBD7D/100", LanguageConsts._D0A04F0A-462A-48A4-BB2F-3706E88DBD7D_100);</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A178" t="s">
+        <v>699</v>
+      </c>
+      <c r="B178" t="s">
+        <v>807</v>
+      </c>
+      <c r="C178" t="s">
+        <v>592</v>
+      </c>
+      <c r="E178" t="str">
+        <f t="shared" si="0"/>
+        <v>_properties.Add("F334115E-DA1B-4509-9B3D-119504DC7ABB/15", LanguageConsts._F334115E-DA1B-4509-9B3D-119504DC7ABB_15);</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A179" t="s">
+        <v>700</v>
+      </c>
+      <c r="B179" t="s">
+        <v>808</v>
+      </c>
+      <c r="C179" t="s">
+        <v>593</v>
+      </c>
+      <c r="E179" t="str">
+        <f t="shared" si="0"/>
+        <v>_properties.Add("D5CDD502-2E9C-101B-9397-08002B2CF9AE/5", LanguageConsts._D5CDD502-2E9C-101B-9397-08002B2CF9AE_5);</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A180" t="s">
+        <v>701</v>
+      </c>
+      <c r="B180" t="s">
+        <v>809</v>
+      </c>
+      <c r="C180" t="s">
+        <v>594</v>
+      </c>
+      <c r="E180" t="str">
+        <f t="shared" si="0"/>
+        <v>_properties.Add("D5CDD502-2E9C-101B-9397-08002B2CF9AE/6", LanguageConsts._D5CDD502-2E9C-101B-9397-08002B2CF9AE_6);</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A181" t="s">
+        <v>702</v>
+      </c>
+      <c r="B181" t="s">
+        <v>810</v>
+      </c>
+      <c r="C181" t="s">
+        <v>595</v>
+      </c>
+      <c r="E181" t="str">
+        <f t="shared" si="0"/>
+        <v>_properties.Add("AEAC19E4-89AE-4508-B9B7-BB867ABEE2ED/2", LanguageConsts._AEAC19E4-89AE-4508-B9B7-BB867ABEE2ED_2);</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A182" t="s">
+        <v>704</v>
+      </c>
+      <c r="B182" t="s">
+        <v>811</v>
+      </c>
+      <c r="C182" t="s">
+        <v>597</v>
+      </c>
+      <c r="E182" t="str">
+        <f t="shared" si="0"/>
+        <v>_properties.Add("E08805C8-E395-40DF-80D2-54F0D6C43154/100", LanguageConsts._E08805C8-E395-40DF-80D2-54F0D6C43154_100);</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A183" t="s">
+        <v>705</v>
+      </c>
+      <c r="B183" t="s">
+        <v>812</v>
+      </c>
+      <c r="C183" t="s">
+        <v>598</v>
+      </c>
+      <c r="E183" t="str">
+        <f t="shared" si="0"/>
+        <v>_properties.Add("6444048F-4C8B-11D1-8B70-080036B11A03/7", LanguageConsts._6444048F-4C8B-11D1-8B70-080036B11A03_7);</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A184" t="s">
+        <v>706</v>
+      </c>
+      <c r="B184" t="s">
+        <v>813</v>
+      </c>
+      <c r="C184" t="s">
+        <v>599</v>
+      </c>
+      <c r="E184" t="str">
+        <f t="shared" si="0"/>
+        <v>_properties.Add("14B81DA1-0135-4D31-96D9-6CBFC9671A99/259", LanguageConsts._14B81DA1-0135-4D31-96D9-6CBFC9671A99_259);</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A185" t="s">
+        <v>707</v>
+      </c>
+      <c r="B185" t="s">
+        <v>814</v>
+      </c>
+      <c r="C185" t="s">
+        <v>600</v>
+      </c>
+      <c r="E185" t="str">
+        <f t="shared" si="0"/>
+        <v>_properties.Add("6444048F-4C8B-11D1-8B70-080036B11A03/3", LanguageConsts._6444048F-4C8B-11D1-8B70-080036B11A03_3);</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A186" t="s">
+        <v>708</v>
+      </c>
+      <c r="B186" t="s">
+        <v>815</v>
+      </c>
+      <c r="C186" t="s">
+        <v>601</v>
+      </c>
+      <c r="E186" t="str">
+        <f t="shared" si="0"/>
+        <v>_properties.Add("6444048F-4C8B-11D1-8B70-080036B11A03/4", LanguageConsts._6444048F-4C8B-11D1-8B70-080036B11A03_4);</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A187" t="s">
+        <v>709</v>
+      </c>
+      <c r="B187" t="s">
+        <v>816</v>
+      </c>
+      <c r="C187" t="s">
+        <v>602</v>
+      </c>
+      <c r="E187" t="str">
+        <f t="shared" si="0"/>
+        <v>_properties.Add("14B81DA1-0135-4D31-96D9-6CBFC9671A99/37378", LanguageConsts._14B81DA1-0135-4D31-96D9-6CBFC9671A99_37378);</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A188" t="s">
+        <v>710</v>
+      </c>
+      <c r="B188" t="s">
+        <v>817</v>
+      </c>
+      <c r="C188" t="s">
+        <v>603</v>
+      </c>
+      <c r="E188" t="str">
+        <f t="shared" si="0"/>
+        <v>_properties.Add("14B81DA1-0135-4D31-96D9-6CBFC9671A99/36867", LanguageConsts._14B81DA1-0135-4D31-96D9-6CBFC9671A99_36867);</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A189" t="s">
+        <v>711</v>
+      </c>
+      <c r="B189" t="s">
+        <v>818</v>
+      </c>
+      <c r="C189" t="s">
+        <v>604</v>
+      </c>
+      <c r="E189" t="str">
+        <f t="shared" si="0"/>
+        <v>_properties.Add("F85BF840-A925-4BC2-B0C4-8E36B598679E/100", LanguageConsts._F85BF840-A925-4BC2-B0C4-8E36B598679E_100);</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A190" t="s">
+        <v>712</v>
+      </c>
+      <c r="B190" t="s">
+        <v>819</v>
+      </c>
+      <c r="C190" t="s">
+        <v>605</v>
+      </c>
+      <c r="E190" t="str">
+        <f t="shared" si="0"/>
+        <v>_properties.Add("14B81DA1-0135-4D31-96D9-6CBFC9671A99/18248", LanguageConsts._14B81DA1-0135-4D31-96D9-6CBFC9671A99_18248);</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A191" t="s">
+        <v>713</v>
+      </c>
+      <c r="B191" t="s">
+        <v>820</v>
+      </c>
+      <c r="C191" t="s">
+        <v>606</v>
+      </c>
+      <c r="E191" t="str">
+        <f t="shared" si="0"/>
+        <v>_properties.Add("14B81DA1-0135-4D31-96D9-6CBFC9671A99/37380", LanguageConsts._14B81DA1-0135-4D31-96D9-6CBFC9671A99_37380);</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A192" t="s">
+        <v>714</v>
+      </c>
+      <c r="B192" t="s">
+        <v>821</v>
+      </c>
+      <c r="C192" t="s">
+        <v>607</v>
+      </c>
+      <c r="E192" t="str">
+        <f t="shared" si="0"/>
+        <v>_properties.Add("14B81DA1-0135-4D31-96D9-6CBFC9671A99/33434", LanguageConsts._14B81DA1-0135-4D31-96D9-6CBFC9671A99_33434);</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A193" t="s">
+        <v>715</v>
+      </c>
+      <c r="B193" t="s">
+        <v>822</v>
+      </c>
+      <c r="C193" t="s">
+        <v>608</v>
+      </c>
+      <c r="E193" t="str">
+        <f t="shared" si="0"/>
+        <v>_properties.Add("2D152B40-CA39-40DB-B2CC-573725B2FEC5/100", LanguageConsts._2D152B40-CA39-40DB-B2CC-573725B2FEC5_100);</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A194" t="s">
+        <v>716</v>
+      </c>
+      <c r="B194" t="s">
+        <v>823</v>
+      </c>
+      <c r="C194" t="s">
+        <v>609</v>
+      </c>
+      <c r="E194" t="str">
+        <f t="shared" si="0"/>
+        <v>_properties.Add("14B81DA1-0135-4D31-96D9-6CBFC9671A99/37386", LanguageConsts._14B81DA1-0135-4D31-96D9-6CBFC9671A99_37386);</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A195" t="s">
+        <v>717</v>
+      </c>
+      <c r="B195" t="s">
+        <v>824</v>
+      </c>
+      <c r="C195" t="s">
+        <v>610</v>
+      </c>
+      <c r="E195" t="str">
+        <f t="shared" si="0"/>
+        <v>_properties.Add("14B81DA1-0135-4D31-96D9-6CBFC9671A99/34855", LanguageConsts._14B81DA1-0135-4D31-96D9-6CBFC9671A99_34855);</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A196" t="s">
+        <v>718</v>
+      </c>
+      <c r="B196" t="s">
+        <v>825</v>
+      </c>
+      <c r="C196" t="s">
+        <v>611</v>
+      </c>
+      <c r="E196" t="str">
+        <f t="shared" si="0"/>
+        <v>_properties.Add("14B81DA1-0135-4D31-96D9-6CBFC9671A99/37383", LanguageConsts._14B81DA1-0135-4D31-96D9-6CBFC9671A99_37383);</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A197" t="s">
+        <v>719</v>
+      </c>
+      <c r="B197" t="s">
+        <v>826</v>
+      </c>
+      <c r="C197" t="s">
+        <v>612</v>
+      </c>
+      <c r="E197" t="str">
+        <f t="shared" si="0"/>
+        <v>_properties.Add("E8309B6E-084C-49B4-B1FC-90A80331B638/100", LanguageConsts._E8309B6E-084C-49B4-B1FC-90A80331B638_100);</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A198" t="s">
+        <v>720</v>
+      </c>
+      <c r="B198" t="s">
+        <v>827</v>
+      </c>
+      <c r="C198" t="s">
+        <v>613</v>
+      </c>
+      <c r="E198" t="str">
+        <f t="shared" si="0"/>
+        <v>_properties.Add("14B81DA1-0135-4D31-96D9-6CBFC9671A99/37377", LanguageConsts._14B81DA1-0135-4D31-96D9-6CBFC9671A99_37377);</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A199" t="s">
+        <v>721</v>
+      </c>
+      <c r="B199" t="s">
+        <v>828</v>
+      </c>
+      <c r="C199" t="s">
+        <v>614</v>
+      </c>
+      <c r="E199" t="str">
+        <f t="shared" si="0"/>
+        <v>_properties.Add("14B81DA1-0135-4D31-96D9-6CBFC9671A99/37382", LanguageConsts._14B81DA1-0135-4D31-96D9-6CBFC9671A99_37382);</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A200" t="s">
+        <v>722</v>
+      </c>
+      <c r="B200" t="s">
+        <v>829</v>
+      </c>
+      <c r="C200" t="s">
+        <v>615</v>
+      </c>
+      <c r="E200" t="str">
+        <f t="shared" si="0"/>
+        <v>_properties.Add("EE3D3D8A-5381-4CFA-B13B-AAF66B5F4EC9/100", LanguageConsts._EE3D3D8A-5381-4CFA-B13B-AAF66B5F4EC9_100);</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A201" t="s">
+        <v>723</v>
+      </c>
+      <c r="B201" t="s">
+        <v>830</v>
+      </c>
+      <c r="C201" t="s">
+        <v>616</v>
+      </c>
+      <c r="E201" t="str">
+        <f t="shared" ref="E201:E264" si="1">CONCATENATE("_properties.Add(""",A201,""", LanguageConsts.",B201,");")</f>
+        <v>_properties.Add("A0E74609-B84D-4F49-B860-462BD9971F98/100", LanguageConsts._A0E74609-B84D-4F49-B860-462BD9971F98_100);</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A202" t="s">
+        <v>724</v>
+      </c>
+      <c r="B202" t="s">
+        <v>831</v>
+      </c>
+      <c r="C202" t="s">
+        <v>617</v>
+      </c>
+      <c r="E202" t="str">
+        <f t="shared" si="1"/>
+        <v>_properties.Add("D35F743A-EB2E-47F2-A286-844132CB1427/100", LanguageConsts._D35F743A-EB2E-47F2-A286-844132CB1427_100);</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A203" t="s">
+        <v>725</v>
+      </c>
+      <c r="B203" t="s">
+        <v>832</v>
+      </c>
+      <c r="C203" t="s">
+        <v>618</v>
+      </c>
+      <c r="E203" t="str">
+        <f t="shared" si="1"/>
+        <v>_properties.Add("14B81DA1-0135-4D31-96D9-6CBFC9671A99/34850", LanguageConsts._14B81DA1-0135-4D31-96D9-6CBFC9671A99_34850);</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A204" t="s">
+        <v>726</v>
+      </c>
+      <c r="B204" t="s">
+        <v>833</v>
+      </c>
+      <c r="C204" t="s">
+        <v>619</v>
+      </c>
+      <c r="E204" t="str">
+        <f t="shared" si="1"/>
+        <v>_properties.Add("14B81DA1-0135-4D31-96D9-6CBFC9671A99}/33437", LanguageConsts._14B81DA1-0135-4D31-96D9-6CBFC9671A99}_33437);</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A205" t="s">
+        <v>727</v>
+      </c>
+      <c r="B205" t="s">
+        <v>834</v>
+      </c>
+      <c r="C205" t="s">
+        <v>620</v>
+      </c>
+      <c r="E205" t="str">
+        <f t="shared" si="1"/>
+        <v>_properties.Add("E6DDCAF7-29C5-4F0A-9A68-D19412EC7090/100", LanguageConsts._E6DDCAF7-29C5-4F0A-9A68-D19412EC7090_100);</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A206" t="s">
+        <v>728</v>
+      </c>
+      <c r="B206" t="s">
+        <v>835</v>
+      </c>
+      <c r="C206" t="s">
+        <v>621</v>
+      </c>
+      <c r="E206" t="str">
+        <f t="shared" si="1"/>
+        <v>_properties.Add("E1277516-2B5F-4869-89B1-2E585BD38B7A/100", LanguageConsts._E1277516-2B5F-4869-89B1-2E585BD38B7A_100);</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A207" t="s">
+        <v>729</v>
+      </c>
+      <c r="B207" t="s">
+        <v>836</v>
+      </c>
+      <c r="C207" t="s">
+        <v>622</v>
+      </c>
+      <c r="E207" t="str">
+        <f t="shared" si="1"/>
+        <v>_properties.Add("6D217F6D-3F6A-4825-B470-5F03CA2FBE9B/100", LanguageConsts._6D217F6D-3F6A-4825-B470-5F03CA2FBE9B_100);</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A208" t="s">
+        <v>730</v>
+      </c>
+      <c r="B208" t="s">
+        <v>837</v>
+      </c>
+      <c r="C208" t="s">
+        <v>623</v>
+      </c>
+      <c r="E208" t="str">
+        <f t="shared" si="1"/>
+        <v>_properties.Add("49237325-A95A-4F67-B211-816B2D45D2E0/100", LanguageConsts._49237325-A95A-4F67-B211-816B2D45D2E0_100);</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A209" t="s">
+        <v>731</v>
+      </c>
+      <c r="B209" t="s">
+        <v>838</v>
+      </c>
+      <c r="C209" t="s">
+        <v>624</v>
+      </c>
+      <c r="E209" t="str">
+        <f t="shared" si="1"/>
+        <v>_properties.Add("64440492-4C8B-11D1-8B70-080036B11A03/27", LanguageConsts._64440492-4C8B-11D1-8B70-080036B11A03_27);</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A210" t="s">
+        <v>732</v>
+      </c>
+      <c r="B210" t="s">
+        <v>839</v>
+      </c>
+      <c r="C210" t="s">
+        <v>625</v>
+      </c>
+      <c r="E210" t="str">
+        <f t="shared" si="1"/>
+        <v>_properties.Add("64440492-4C8B-11D1-8B70-080036B11A03/28", LanguageConsts._64440492-4C8B-11D1-8B70-080036B11A03_28);</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A211" t="s">
+        <v>733</v>
+      </c>
+      <c r="B211" t="s">
+        <v>840</v>
+      </c>
+      <c r="C211" t="s">
+        <v>626</v>
+      </c>
+      <c r="E211" t="str">
+        <f t="shared" si="1"/>
+        <v>_properties.Add("2E4B640D-5019-46D8-8881-55414CC5CAA0/100", LanguageConsts._2E4B640D-5019-46D8-8881-55414CC5CAA0_100);</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A212" t="s">
+        <v>734</v>
+      </c>
+      <c r="B212" t="s">
+        <v>841</v>
+      </c>
+      <c r="C212" t="s">
+        <v>627</v>
+      </c>
+      <c r="E212" t="str">
+        <f t="shared" si="1"/>
+        <v>_properties.Add("64440490-4C8B-11D1-8B70-080036B11A03/3", LanguageConsts._64440490-4C8B-11D1-8B70-080036B11A03_3);</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A213" t="s">
+        <v>735</v>
+      </c>
+      <c r="B213" t="s">
+        <v>842</v>
+      </c>
+      <c r="C213" t="s">
+        <v>628</v>
+      </c>
+      <c r="E213" t="str">
+        <f t="shared" si="1"/>
+        <v>_properties.Add("64440492-4C8B-11D1-8B70-080036B11A03/36", LanguageConsts._64440492-4C8B-11D1-8B70-080036B11A03_36);</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A214" t="s">
+        <v>736</v>
+      </c>
+      <c r="B214" t="s">
+        <v>843</v>
+      </c>
+      <c r="C214" t="s">
+        <v>629</v>
+      </c>
+      <c r="E214" t="str">
+        <f t="shared" si="1"/>
+        <v>_properties.Add("6444048F-4C8B-11D1-8B70-080036B11A03/12", LanguageConsts._6444048F-4C8B-11D1-8B70-080036B11A03_12);</v>
+      </c>
+    </row>
+    <row r="215" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A215" t="s">
+        <v>737</v>
+      </c>
+      <c r="B215" t="s">
+        <v>844</v>
+      </c>
+      <c r="C215" t="s">
+        <v>630</v>
+      </c>
+      <c r="E215" t="str">
+        <f t="shared" si="1"/>
+        <v>_properties.Add("64440492-4C8B-11D1-8B70-080036B11A03/22", LanguageConsts._64440492-4C8B-11D1-8B70-080036B11A03_22);</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A216" t="s">
+        <v>738</v>
+      </c>
+      <c r="B216" t="s">
+        <v>845</v>
+      </c>
+      <c r="C216" t="s">
+        <v>631</v>
+      </c>
+      <c r="E216" t="str">
+        <f t="shared" si="1"/>
+        <v>_properties.Add("64440492-4C8B-11D1-8B70-080036B11A03/39", LanguageConsts._64440492-4C8B-11D1-8B70-080036B11A03_39);</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A217" t="s">
+        <v>739</v>
+      </c>
+      <c r="B217" t="s">
+        <v>846</v>
+      </c>
+      <c r="C217" t="s">
+        <v>632</v>
+      </c>
+      <c r="E217" t="str">
+        <f t="shared" si="1"/>
+        <v>_properties.Add("64440492-4C8B-11D1-8B70-080036B11A03/30", LanguageConsts._64440492-4C8B-11D1-8B70-080036B11A03_30);</v>
+      </c>
+    </row>
+    <row r="218" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A218" t="s">
+        <v>740</v>
+      </c>
+      <c r="B218" t="s">
+        <v>847</v>
+      </c>
+      <c r="C218" t="s">
+        <v>633</v>
+      </c>
+      <c r="E218" t="str">
+        <f t="shared" si="1"/>
+        <v>_properties.Add("56A3372E-CE9C-11D2-9F0E-006097C686F6/38", LanguageConsts._56A3372E-CE9C-11D2-9F0E-006097C686F6_38);</v>
+      </c>
+    </row>
+    <row r="219" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A219" t="s">
+        <v>741</v>
+      </c>
+      <c r="B219" t="s">
+        <v>848</v>
+      </c>
+      <c r="C219" t="s">
+        <v>634</v>
+      </c>
+      <c r="E219" t="str">
+        <f t="shared" si="1"/>
+        <v>_properties.Add("64440492-4C8B-11D1-8B70-080036B11A03/23", LanguageConsts._64440492-4C8B-11D1-8B70-080036B11A03_23);</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A220" t="s">
+        <v>742</v>
+      </c>
+      <c r="B220" t="s">
+        <v>849</v>
+      </c>
+      <c r="C220" t="s">
+        <v>589</v>
+      </c>
+      <c r="E220" t="str">
+        <f t="shared" si="1"/>
+        <v>_properties.Add("64440492-4C8B-11D1-8B70-080036B11A03/21", LanguageConsts._64440492-4C8B-11D1-8B70-080036B11A03_21);</v>
+      </c>
+    </row>
+    <row r="221" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A221" t="s">
+        <v>743</v>
+      </c>
+      <c r="B221" t="s">
+        <v>850</v>
+      </c>
+      <c r="C221" t="s">
+        <v>635</v>
+      </c>
+      <c r="E221" t="str">
+        <f t="shared" si="1"/>
+        <v>_properties.Add("64440491-4C8B-11D1-8B70-080036B11A03/10", LanguageConsts._64440491-4C8B-11D1-8B70-080036B11A03_10);</v>
+      </c>
+    </row>
+    <row r="222" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A222" t="s">
+        <v>744</v>
+      </c>
+      <c r="B222" t="s">
+        <v>851</v>
+      </c>
+      <c r="C222" t="s">
+        <v>636</v>
+      </c>
+      <c r="E222" t="str">
+        <f t="shared" si="1"/>
+        <v>_properties.Add("64440492-4C8B-11D1-8B70-080036B11A03/20", LanguageConsts._64440492-4C8B-11D1-8B70-080036B11A03_20);</v>
+      </c>
+    </row>
+    <row r="223" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A223" t="s">
+        <v>745</v>
+      </c>
+      <c r="B223" t="s">
+        <v>852</v>
+      </c>
+      <c r="C223" t="s">
+        <v>637</v>
+      </c>
+      <c r="E223" t="str">
+        <f t="shared" si="1"/>
+        <v>_properties.Add("64440491-4C8B-11D1-8B70-080036B11A03/8", LanguageConsts._64440491-4C8B-11D1-8B70-080036B11A03_8);</v>
+      </c>
+    </row>
+    <row r="224" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A224" t="s">
+        <v>746</v>
+      </c>
+      <c r="B224" t="s">
+        <v>853</v>
+      </c>
+      <c r="C224" t="s">
+        <v>638</v>
+      </c>
+      <c r="E224" t="str">
+        <f t="shared" si="1"/>
+        <v>_properties.Add("64440491-4C8B-11D1-8B70-080036B11A03/44", LanguageConsts._64440491-4C8B-11D1-8B70-080036B11A03_44);</v>
+      </c>
+    </row>
+    <row r="225" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A225" t="s">
+        <v>747</v>
+      </c>
+      <c r="B225" t="s">
+        <v>854</v>
+      </c>
+      <c r="C225" t="s">
+        <v>639</v>
+      </c>
+      <c r="E225" t="str">
+        <f t="shared" si="1"/>
+        <v>_properties.Add("64440491-4C8B-11D1-8B70-080036B11A03/42", LanguageConsts._64440491-4C8B-11D1-8B70-080036B11A03_42);</v>
+      </c>
+    </row>
+    <row r="226" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A226" t="s">
+        <v>748</v>
+      </c>
+      <c r="B226" t="s">
+        <v>855</v>
+      </c>
+      <c r="C226" t="s">
+        <v>640</v>
+      </c>
+      <c r="E226" t="str">
+        <f t="shared" si="1"/>
+        <v>_properties.Add("64440491-4C8B-11D1-8B70-080036B11A03/45", LanguageConsts._64440491-4C8B-11D1-8B70-080036B11A03_45);</v>
+      </c>
+    </row>
+    <row r="227" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A227" t="s">
+        <v>749</v>
+      </c>
+      <c r="B227" t="s">
+        <v>856</v>
+      </c>
+      <c r="C227" t="s">
+        <v>641</v>
+      </c>
+      <c r="E227" t="str">
+        <f t="shared" si="1"/>
+        <v>_properties.Add("64440491-4C8B-11D1-8B70-080036B11A03/43", LanguageConsts._64440491-4C8B-11D1-8B70-080036B11A03_43);</v>
+      </c>
+    </row>
+    <row r="228" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A228" t="s">
+        <v>750</v>
+      </c>
+      <c r="B228" t="s">
+        <v>857</v>
+      </c>
+      <c r="C228" t="s">
+        <v>642</v>
+      </c>
+      <c r="E228" t="str">
+        <f t="shared" si="1"/>
+        <v>_properties.Add("0CEF7D53-FA64-11D1-A203-0000F81FEDEE/3", LanguageConsts._0CEF7D53-FA64-11D1-A203-0000F81FEDEE_3);</v>
+      </c>
+    </row>
+    <row r="229" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A229" t="s">
+        <v>751</v>
+      </c>
+      <c r="B229" t="s">
+        <v>858</v>
+      </c>
+      <c r="C229" t="s">
+        <v>643</v>
+      </c>
+      <c r="E229" t="str">
+        <f t="shared" si="1"/>
+        <v>_properties.Add("0CEF7D53-FA64-11D1-A203-0000F81FEDEE/4", LanguageConsts._0CEF7D53-FA64-11D1-A203-0000F81FEDEE_4);</v>
+      </c>
+    </row>
+    <row r="230" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A230" t="s">
+        <v>752</v>
+      </c>
+      <c r="B230" t="s">
+        <v>859</v>
+      </c>
+      <c r="C230" t="s">
+        <v>644</v>
+      </c>
+      <c r="E230" t="str">
+        <f t="shared" si="1"/>
+        <v>_properties.Add("841E4F90-FF59-4D16-8947-E81BBFFAB36D/16", LanguageConsts._841E4F90-FF59-4D16-8947-E81BBFFAB36D_16);</v>
+      </c>
+    </row>
+    <row r="231" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A231" t="s">
+        <v>753</v>
+      </c>
+      <c r="B231" t="s">
+        <v>860</v>
+      </c>
+      <c r="C231" t="s">
+        <v>645</v>
+      </c>
+      <c r="E231" t="str">
+        <f t="shared" si="1"/>
+        <v>_properties.Add("0CEF7D53-FA64-11D1-A203-0000F81FEDEE/7", LanguageConsts._0CEF7D53-FA64-11D1-A203-0000F81FEDEE_7);</v>
+      </c>
+    </row>
+    <row r="232" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A232" t="s">
+        <v>754</v>
+      </c>
+      <c r="B232" t="s">
+        <v>861</v>
+      </c>
+      <c r="C232" t="s">
+        <v>646</v>
+      </c>
+      <c r="E232" t="str">
+        <f t="shared" si="1"/>
+        <v>_properties.Add("0CEF7D53-FA64-11D1-A203-0000F81FEDEE/8", LanguageConsts._0CEF7D53-FA64-11D1-A203-0000F81FEDEE_8);</v>
+      </c>
+    </row>
+    <row r="233" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A233" t="s">
+        <v>703</v>
+      </c>
+      <c r="B233" t="s">
+        <v>862</v>
+      </c>
+      <c r="C233" t="s">
+        <v>647</v>
+      </c>
+      <c r="E233" t="str">
+        <f t="shared" si="1"/>
+        <v>_properties.Add("D5CDD502-2E9C-101B-9397-08002B2CF9AE/29", LanguageConsts._D5CDD502-2E9C-101B-9397-08002B2CF9AE_29);</v>
+      </c>
+    </row>
+    <row r="234" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A234" t="s">
+        <v>755</v>
+      </c>
+      <c r="B234" t="s">
+        <v>863</v>
+      </c>
+      <c r="C234" t="s">
+        <v>596</v>
+      </c>
+      <c r="E234" t="str">
+        <f t="shared" si="1"/>
+        <v>_properties.Add("64440492-4C8B-11D1-8B70-080036B11A03/11", LanguageConsts._64440492-4C8B-11D1-8B70-080036B11A03_11);</v>
+      </c>
+    </row>
+    <row r="235" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A235" t="s">
+        <v>756</v>
+      </c>
+      <c r="B235" t="s">
+        <v>864</v>
+      </c>
+      <c r="C235" t="s">
+        <v>648</v>
+      </c>
+      <c r="E235" t="str">
+        <f t="shared" si="1"/>
+        <v>_properties.Add("6D748DE2-8D38-4CC3-AC60-F009B057C557/7", LanguageConsts._6D748DE2-8D38-4CC3-AC60-F009B057C557_7);</v>
+      </c>
+    </row>
+    <row r="236" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A236" t="s">
+        <v>757</v>
+      </c>
+      <c r="B236" t="s">
+        <v>865</v>
+      </c>
+      <c r="C236" t="s">
+        <v>649</v>
+      </c>
+      <c r="E236" t="str">
+        <f t="shared" si="1"/>
+        <v>_properties.Add("6D748DE2-8D38-4CC3-AC60-F009B057C557/2", LanguageConsts._6D748DE2-8D38-4CC3-AC60-F009B057C557_2);</v>
+      </c>
+    </row>
+    <row r="237" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A237" t="s">
+        <v>758</v>
+      </c>
+      <c r="B237" t="s">
+        <v>866</v>
+      </c>
+      <c r="C237" t="s">
+        <v>650</v>
+      </c>
+      <c r="E237" t="str">
+        <f t="shared" si="1"/>
+        <v>_properties.Add("6D748DE2-8D38-4CC3-AC60-F009B057C557/12", LanguageConsts._6D748DE2-8D38-4CC3-AC60-F009B057C557_12);</v>
+      </c>
+    </row>
+    <row r="238" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A238" t="s">
+        <v>759</v>
+      </c>
+      <c r="B238" t="s">
+        <v>867</v>
+      </c>
+      <c r="C238" t="s">
+        <v>651</v>
+      </c>
+      <c r="E238" t="str">
+        <f t="shared" si="1"/>
+        <v>_properties.Add("6D748DE2-8D38-4CC3-AC60-F009B057C557/17", LanguageConsts._6D748DE2-8D38-4CC3-AC60-F009B057C557_17);</v>
+      </c>
+    </row>
+    <row r="239" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A239" t="s">
+        <v>760</v>
+      </c>
+      <c r="B239" t="s">
+        <v>868</v>
+      </c>
+      <c r="C239" t="s">
+        <v>652</v>
+      </c>
+      <c r="E239" t="str">
+        <f t="shared" si="1"/>
+        <v>_properties.Add("6D748DE2-8D38-4CC3-AC60-F009B057C557/18", LanguageConsts._6D748DE2-8D38-4CC3-AC60-F009B057C557_18);</v>
+      </c>
+    </row>
+    <row r="240" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A240" t="s">
+        <v>761</v>
+      </c>
+      <c r="B240" t="s">
+        <v>869</v>
+      </c>
+      <c r="C240" t="s">
+        <v>653</v>
+      </c>
+      <c r="E240" t="str">
+        <f t="shared" si="1"/>
+        <v>_properties.Add("6D748DE2-8D38-4CC3-AC60-F009B057C557/13", LanguageConsts._6D748DE2-8D38-4CC3-AC60-F009B057C557_13);</v>
+      </c>
+    </row>
+    <row r="241" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A241" t="s">
+        <v>762</v>
+      </c>
+      <c r="B241" t="s">
+        <v>870</v>
+      </c>
+      <c r="C241" t="s">
+        <v>654</v>
+      </c>
+      <c r="E241" t="str">
+        <f t="shared" si="1"/>
+        <v>_properties.Add("2C53C813-FB63-4E22-A1AB-0B331CA1E273/100", LanguageConsts._2C53C813-FB63-4E22-A1AB-0B331CA1E273_100);</v>
+      </c>
+    </row>
+    <row r="242" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A242" t="s">
+        <v>763</v>
+      </c>
+      <c r="B242" t="s">
+        <v>871</v>
+      </c>
+      <c r="C242" t="s">
+        <v>655</v>
+      </c>
+      <c r="E242" t="str">
+        <f t="shared" si="1"/>
+        <v>_properties.Add("4684FE97-8765-4842-9C13-F006447B178C/100", LanguageConsts._4684FE97-8765-4842-9C13-F006447B178C_100);</v>
+      </c>
+    </row>
+    <row r="243" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A243" t="s">
+        <v>764</v>
+      </c>
+      <c r="B243" t="s">
+        <v>872</v>
+      </c>
+      <c r="C243" t="s">
+        <v>656</v>
+      </c>
+      <c r="E243" t="str">
+        <f t="shared" si="1"/>
+        <v>_properties.Add("6D748DE2-8D38-4CC3-AC60-F009B057C557/3", LanguageConsts._6D748DE2-8D38-4CC3-AC60-F009B057C557_3);</v>
+      </c>
+    </row>
+    <row r="244" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A244" t="s">
+        <v>765</v>
+      </c>
+      <c r="B244" t="s">
+        <v>873</v>
+      </c>
+      <c r="C244" t="s">
+        <v>657</v>
+      </c>
+      <c r="E244" t="str">
+        <f t="shared" si="1"/>
+        <v>_properties.Add("A5477F61-7A82-4ECA-9DDE-98B69B2479B3/100", LanguageConsts._A5477F61-7A82-4ECA-9DDE-98B69B2479B3_100);</v>
+      </c>
+    </row>
+    <row r="245" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A245" t="s">
+        <v>766</v>
+      </c>
+      <c r="B245" t="s">
+        <v>874</v>
+      </c>
+      <c r="C245" t="s">
+        <v>658</v>
+      </c>
+      <c r="E245" t="str">
+        <f t="shared" si="1"/>
+        <v>_properties.Add("2CBAA8F5-D81F-47CA-B17A-F8D822300131/100", LanguageConsts._2CBAA8F5-D81F-47CA-B17A-F8D822300131_100);</v>
+      </c>
+    </row>
+    <row r="246" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A246" t="s">
+        <v>767</v>
+      </c>
+      <c r="B246" t="s">
+        <v>875</v>
+      </c>
+      <c r="C246" t="s">
+        <v>659</v>
+      </c>
+      <c r="E246" t="str">
+        <f t="shared" si="1"/>
+        <v>_properties.Add("43F8D7B7-A444-4F87-9383-52271C9B915C/100", LanguageConsts._43F8D7B7-A444-4F87-9383-52271C9B915C_100);</v>
+      </c>
+    </row>
+    <row r="247" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A247" t="s">
+        <v>768</v>
+      </c>
+      <c r="B247" t="s">
+        <v>876</v>
+      </c>
+      <c r="C247" t="s">
+        <v>660</v>
+      </c>
+      <c r="E247" t="str">
+        <f t="shared" si="1"/>
+        <v>_properties.Add("14B81DA1-0135-4D31-96D9-6CBFC9671A99/18258", LanguageConsts._14B81DA1-0135-4D31-96D9-6CBFC9671A99_18258);</v>
+      </c>
+    </row>
+    <row r="248" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A248" t="s">
+        <v>769</v>
+      </c>
+      <c r="B248" t="s">
+        <v>877</v>
+      </c>
+      <c r="C248" t="s">
+        <v>661</v>
+      </c>
+      <c r="E248" t="str">
+        <f t="shared" si="1"/>
+        <v>_properties.Add("72FAB781-ACDA-43E5-B155-B2434F85E678/100", LanguageConsts._72FAB781-ACDA-43E5-B155-B2434F85E678_100);</v>
+      </c>
+    </row>
+    <row r="249" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A249" t="s">
+        <v>770</v>
+      </c>
+      <c r="B249" t="s">
+        <v>878</v>
+      </c>
+      <c r="C249" t="s">
+        <v>662</v>
+      </c>
+      <c r="E249" t="str">
+        <f t="shared" si="1"/>
+        <v>_properties.Add("DE41CC29-6971-4290-B472-F59F2E2F31E2/100", LanguageConsts._DE41CC29-6971-4290-B472-F59F2E2F31E2_100);</v>
+      </c>
+    </row>
+    <row r="250" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A250" t="s">
+        <v>771</v>
+      </c>
+      <c r="B250" t="s">
+        <v>879</v>
+      </c>
+      <c r="C250" t="s">
+        <v>663</v>
+      </c>
+      <c r="E250" t="str">
+        <f t="shared" si="1"/>
+        <v>_properties.Add("5CBF2787-48CF-4208-B90E-EE5E5D420294/23", LanguageConsts._5CBF2787-48CF-4208-B90E-EE5E5D420294_23);</v>
+      </c>
+    </row>
+    <row r="251" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A251" t="s">
+        <v>772</v>
+      </c>
+      <c r="B251" t="s">
+        <v>880</v>
+      </c>
+      <c r="C251" t="s">
+        <v>664</v>
+      </c>
+      <c r="E251" t="str">
+        <f t="shared" si="1"/>
+        <v>_properties.Add("64440492-4C8B-11D1-8B70-080036B11A03/9", LanguageConsts._64440492-4C8B-11D1-8B70-080036B11A03_9);</v>
+      </c>
+    </row>
+    <row r="252" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A252" t="s">
+        <v>773</v>
+      </c>
+      <c r="B252" t="s">
+        <v>881</v>
+      </c>
+      <c r="C252" t="s">
+        <v>665</v>
+      </c>
+      <c r="E252" t="str">
+        <f t="shared" si="1"/>
+        <v>_properties.Add("000214A1-0000-0000-C000-000000000046/9", LanguageConsts._000214A1-0000-0000-C000-000000000046_9);</v>
+      </c>
+    </row>
+    <row r="253" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A253" t="s">
+        <v>774</v>
+      </c>
+      <c r="B253" t="s">
+        <v>882</v>
+      </c>
+      <c r="C253" t="s">
+        <v>666</v>
+      </c>
+      <c r="E253" t="str">
+        <f t="shared" si="1"/>
+        <v>_properties.Add("28636AA6-953D-11D2-B5D6-00C04FD918D0/14", LanguageConsts._28636AA6-953D-11D2-B5D6-00C04FD918D0_14);</v>
+      </c>
+    </row>
+    <row r="254" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A254" t="s">
+        <v>896</v>
+      </c>
+      <c r="B254" t="s">
+        <v>897</v>
+      </c>
+      <c r="C254" t="s">
+        <v>522</v>
+      </c>
+      <c r="E254" t="str">
+        <f t="shared" si="1"/>
+        <v>_properties.Add("D5CDD502-2E9C-101B-9397-08002B2CF9AE/8", LanguageConsts._D5CDD502-2E9C-101B-9397-08002B2CF9AE_8);</v>
+      </c>
+    </row>
+    <row r="255" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A255" t="s">
+        <v>898</v>
+      </c>
+      <c r="B255" t="s">
+        <v>899</v>
+      </c>
+      <c r="C255" t="s">
+        <v>523</v>
+      </c>
+      <c r="E255" t="str">
+        <f t="shared" si="1"/>
+        <v>_properties.Add("D5CDD502-2E9C-101B-9397-08002B2CF9AE/9", LanguageConsts._D5CDD502-2E9C-101B-9397-08002B2CF9AE_9);</v>
+      </c>
+    </row>
+    <row r="256" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A256" t="s">
+        <v>900</v>
+      </c>
+      <c r="B256" t="s">
+        <v>901</v>
+      </c>
+      <c r="C256" t="s">
+        <v>524</v>
+      </c>
+      <c r="E256" t="str">
+        <f t="shared" si="1"/>
+        <v>_properties.Add("D5CDD502-2E9C-101B-9397-08002B2CF9AE/10", LanguageConsts._D5CDD502-2E9C-101B-9397-08002B2CF9AE_10);</v>
+      </c>
+    </row>
+    <row r="257" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A257" t="s">
+        <v>902</v>
+      </c>
+      <c r="B257" t="s">
+        <v>903</v>
+      </c>
+      <c r="C257" t="s">
+        <v>525</v>
+      </c>
+      <c r="E257" t="str">
+        <f t="shared" si="1"/>
+        <v>_properties.Add("D5CDD502-2E9C-101B-9397-08002B2CF9AE/11", LanguageConsts._D5CDD502-2E9C-101B-9397-08002B2CF9AE_11);</v>
+      </c>
+    </row>
+    <row r="258" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A258" t="s">
+        <v>904</v>
+      </c>
+      <c r="B258" t="s">
+        <v>905</v>
+      </c>
+      <c r="C258" t="s">
+        <v>526</v>
+      </c>
+      <c r="E258" t="str">
+        <f t="shared" si="1"/>
+        <v>_properties.Add("D5CDD502-2E9C-101B-9397-08002B2CF9AE/12", LanguageConsts._D5CDD502-2E9C-101B-9397-08002B2CF9AE_12);</v>
+      </c>
+    </row>
+    <row r="259" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A259" t="s">
+        <v>906</v>
+      </c>
+      <c r="B259" t="s">
+        <v>907</v>
+      </c>
+      <c r="C259" t="s">
+        <v>527</v>
+      </c>
+      <c r="E259" t="str">
+        <f t="shared" si="1"/>
+        <v>_properties.Add("D5CDD502-2E9C-101B-9397-08002B2CF9AE/13", LanguageConsts._D5CDD502-2E9C-101B-9397-08002B2CF9AE_13);</v>
+      </c>
+    </row>
+    <row r="260" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A260" t="s">
+        <v>908</v>
+      </c>
+      <c r="B260" t="s">
+        <v>909</v>
+      </c>
+      <c r="C260" t="s">
+        <v>528</v>
+      </c>
+      <c r="E260" t="str">
+        <f t="shared" si="1"/>
+        <v>_properties.Add("D5CDD502-2E9C-101B-9397-08002B2CF9AE/16", LanguageConsts._D5CDD502-2E9C-101B-9397-08002B2CF9AE_16);</v>
+      </c>
+    </row>
+    <row r="261" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A261" t="s">
+        <v>910</v>
+      </c>
+      <c r="B261" t="s">
+        <v>911</v>
+      </c>
+      <c r="C261" t="s">
+        <v>529</v>
+      </c>
+      <c r="E261" t="str">
+        <f t="shared" si="1"/>
+        <v>_properties.Add("D5CDD502-2E9C-101B-9397-08002B2CF9AE/17", LanguageConsts._D5CDD502-2E9C-101B-9397-08002B2CF9AE_17);</v>
+      </c>
+    </row>
+    <row r="262" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A262" t="s">
+        <v>912</v>
+      </c>
+      <c r="B262" t="s">
+        <v>913</v>
+      </c>
+      <c r="C262" t="s">
+        <v>530</v>
+      </c>
+      <c r="E262" t="str">
+        <f t="shared" si="1"/>
+        <v>_properties.Add("D5CDD502-2E9C-101B-9397-08002B2CF9AE/18", LanguageConsts._D5CDD502-2E9C-101B-9397-08002B2CF9AE_18);</v>
+      </c>
+    </row>
+    <row r="263" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A263" t="s">
+        <v>914</v>
+      </c>
+      <c r="B263" t="s">
+        <v>915</v>
+      </c>
+      <c r="C263" t="s">
+        <v>531</v>
+      </c>
+      <c r="E263" t="str">
+        <f t="shared" si="1"/>
+        <v>_properties.Add("D5CDD502-2E9C-101B-9397-08002B2CF9AE/19", LanguageConsts._D5CDD502-2E9C-101B-9397-08002B2CF9AE_19);</v>
+      </c>
+    </row>
+    <row r="264" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A264" t="s">
+        <v>916</v>
+      </c>
+      <c r="B264" t="s">
+        <v>917</v>
+      </c>
+      <c r="C264" t="s">
+        <v>532</v>
+      </c>
+      <c r="E264" t="str">
+        <f t="shared" si="1"/>
+        <v>_properties.Add("D5CDD502-2E9C-101B-9397-08002B2CF9AE/22", LanguageConsts._D5CDD502-2E9C-101B-9397-08002B2CF9AE_22);</v>
+      </c>
+    </row>
+    <row r="265" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A265" t="s">
+        <v>918</v>
+      </c>
+      <c r="B265" t="s">
+        <v>919</v>
+      </c>
+      <c r="C265" t="s">
+        <v>533</v>
+      </c>
+      <c r="E265" t="str">
+        <f t="shared" ref="E265:E274" si="2">CONCATENATE("_properties.Add(""",A265,""", LanguageConsts.",B265,");")</f>
+        <v>_properties.Add("D5CDD502-2E9C-101B-9397-08002B2CF9AE/23", LanguageConsts._D5CDD502-2E9C-101B-9397-08002B2CF9AE_23);</v>
+      </c>
+    </row>
+    <row r="266" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A266" t="s">
+        <v>920</v>
+      </c>
+      <c r="B266" t="s">
+        <v>921</v>
+      </c>
+      <c r="C266" t="s">
+        <v>535</v>
+      </c>
+      <c r="E266" t="str">
         <f t="shared" si="2"/>
-        <v>_properties.Add("F29F85E0-4FF9-1068-AB91-08002B27B3D9/8", LanguageConsts._F29F85E0_4FF9_1068_AB91_08002B27B3D9_8);</v>
+        <v>_properties.Add("D5CDD502-2E9C-101B-9397-08002B2CF9AE/27", LanguageConsts._D5CDD502-2E9C-101B-9397-08002B2CF9AE_27);</v>
+      </c>
+    </row>
+    <row r="267" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A267" t="s">
+        <v>922</v>
+      </c>
+      <c r="B267" t="s">
+        <v>923</v>
+      </c>
+      <c r="C267" t="s">
+        <v>536</v>
+      </c>
+      <c r="E267" t="str">
+        <f t="shared" si="2"/>
+        <v>_properties.Add("D5CDD502-2E9C-101B-9397-08002B2CF9AE/28", LanguageConsts._D5CDD502-2E9C-101B-9397-08002B2CF9AE_28);</v>
+      </c>
+    </row>
+    <row r="268" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A268" t="s">
+        <v>924</v>
+      </c>
+      <c r="B268" t="s">
+        <v>925</v>
+      </c>
+      <c r="C268" t="s">
+        <v>537</v>
+      </c>
+      <c r="E268" t="str">
+        <f t="shared" si="2"/>
+        <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/_PID_HLINKS", LanguageConsts._D5CDD505-2E9C-101B-9397-08002B2CF9AE__PID_HLINKS);</v>
+      </c>
+    </row>
+    <row r="269" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A269" t="s">
+        <v>926</v>
+      </c>
+      <c r="B269" t="s">
+        <v>927</v>
+      </c>
+      <c r="C269" t="s">
+        <v>538</v>
+      </c>
+      <c r="E269" t="str">
+        <f t="shared" si="2"/>
+        <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/_SHAREDFILEINDEX", LanguageConsts._D5CDD505-2E9C-101B-9397-08002B2CF9AE__SHAREDFILEINDEX);</v>
+      </c>
+    </row>
+    <row r="270" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A270" t="s">
+        <v>928</v>
+      </c>
+      <c r="B270" t="s">
+        <v>929</v>
+      </c>
+      <c r="C270" t="s">
+        <v>539</v>
+      </c>
+      <c r="E270" t="str">
+        <f t="shared" si="2"/>
+        <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/_SOURCEURL", LanguageConsts._D5CDD505-2E9C-101B-9397-08002B2CF9AE__SOURCEURL);</v>
+      </c>
+    </row>
+    <row r="271" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A271" t="s">
+        <v>930</v>
+      </c>
+      <c r="B271" t="s">
+        <v>931</v>
+      </c>
+      <c r="C271" t="s">
+        <v>534</v>
+      </c>
+      <c r="E271" t="str">
+        <f t="shared" si="2"/>
+        <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/CONTENTTYPE", LanguageConsts._D5CDD505-2E9C-101B-9397-08002B2CF9AE_CONTENTTYPE);</v>
+      </c>
+    </row>
+    <row r="272" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A272" t="s">
+        <v>932</v>
+      </c>
+      <c r="B272" t="s">
+        <v>933</v>
+      </c>
+      <c r="C272" t="s">
+        <v>540</v>
+      </c>
+      <c r="E272" t="str">
+        <f t="shared" si="2"/>
+        <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/CONTENTTYPEID", LanguageConsts._D5CDD505-2E9C-101B-9397-08002B2CF9AE_CONTENTTYPEID);</v>
       </c>
     </row>
   </sheetData>
   <sortState ref="B1:D137">
     <sortCondition ref="B1:B137"/>
   </sortState>
+  <conditionalFormatting sqref="A1:A1048576">
+    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" copies="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated excel file with new properties
</commit_message>
<xml_diff>
--- a/IFilterTextReader/Properties.xlsx
+++ b/IFilterTextReader/Properties.xlsx
@@ -2081,9 +2081,6 @@
     <t>E3E0584C-B788-4A5A-BB20-7F5A44C9ACDD/6</t>
   </si>
   <si>
-    <t>49691C90-7E17-101A-A91C-08002B2ECDA9}/3</t>
-  </si>
-  <si>
     <t>64440490-4C8B-11D1-8B70-080036B11A03/7</t>
   </si>
   <si>
@@ -2204,9 +2201,6 @@
     <t>14B81DA1-0135-4D31-96D9-6CBFC9671A99/34850</t>
   </si>
   <si>
-    <t>14B81DA1-0135-4D31-96D9-6CBFC9671A99}/33437</t>
-  </si>
-  <si>
     <t>E6DDCAF7-29C5-4F0A-9A68-D19412EC7090/100</t>
   </si>
   <si>
@@ -2351,330 +2345,6 @@
     <t>28636AA6-953D-11D2-B5D6-00C04FD918D0/14</t>
   </si>
   <si>
-    <t>_F7DB74B4-4287-4103-AFBA-F1B13DCD75CF_100</t>
-  </si>
-  <si>
-    <t>_28636AA6-953D-11D2-B5D6-00C04FD918D0_11</t>
-  </si>
-  <si>
-    <t>_D5CDD502-2E9C-101B-9397-08002B2CF9AE_26</t>
-  </si>
-  <si>
-    <t>_1E3EE840-BC2B-476C-8237-2ACD1A839B22_3</t>
-  </si>
-  <si>
-    <t>_E4F10A3C-49E6-405D-8288-A23BD4EEAA6C_100</t>
-  </si>
-  <si>
-    <t>_28636AA6-953D-11D2-B5D6-00C04FD918D0_12</t>
-  </si>
-  <si>
-    <t>_EF884C5B-2BFE-41BB-AAE5-76EEDF4F9902_100</t>
-  </si>
-  <si>
-    <t>_EF884C5B-2BFE-41BB-AAE5-76EEDF4F9902_200</t>
-  </si>
-  <si>
-    <t>_EF884C5B-2BFE-41BB-AAE5-76EEDF4F9902_300</t>
-  </si>
-  <si>
-    <t>_B725F130-47EF-101A-A5F1-02608C9EEBAC_16</t>
-  </si>
-  <si>
-    <t>_B725F130-47EF-101A-A5F1-02608C9EEBAC_13</t>
-  </si>
-  <si>
-    <t>_9B174B34-40FF-11D2-A27E-00C04FC30871_4</t>
-  </si>
-  <si>
-    <t>_28636AA6-953D-11D2-B5D6-00C04FD918D0_5</t>
-  </si>
-  <si>
-    <t>_90E5E14E-648B-4826-B2AA-ACAF790E3513_10</t>
-  </si>
-  <si>
-    <t>_A94688B6-7D9F-4570-A648-E3DFC0AB2B3F_100</t>
-  </si>
-  <si>
-    <t>_6D24888F-4718-4BDA-AFED-EA0FB4386CD8_100</t>
-  </si>
-  <si>
-    <t>_B9B4B3FC-2B51-4A42-B5D8-324146AFCF25_2</t>
-  </si>
-  <si>
-    <t>_E3E0584C-B788-4A5A-BB20-7F5A44C9ACDD_6</t>
-  </si>
-  <si>
-    <t>_49691C90-7E17-101A-A91C-08002B2ECDA9}_3</t>
-  </si>
-  <si>
-    <t>_64440490-4C8B-11D1-8B70-080036B11A03_7</t>
-  </si>
-  <si>
-    <t>_64440490-4C8B-11D1-8B70-080036B11A03_5</t>
-  </si>
-  <si>
-    <t>_64440490-4C8B-11D1-8B70-080036B11A03_8</t>
-  </si>
-  <si>
-    <t>_56A3372E-CE9C-11D2-9F0E-006097C686F6_13</t>
-  </si>
-  <si>
-    <t>_56A3372E-CE9C-11D2-9F0E-006097C686F6_100</t>
-  </si>
-  <si>
-    <t>_FD122953-FA93-4EF7-92C3-04C946B2F7C8_100</t>
-  </si>
-  <si>
-    <t>_56A3372E-CE9C-11D2-9F0E-006097C686F6_35</t>
-  </si>
-  <si>
-    <t>_64440492-4C8B-11D1-8B70-080036B11A03_19</t>
-  </si>
-  <si>
-    <t>_56A3372E-CE9C-11D2-9F0E-006097C686F6_36</t>
-  </si>
-  <si>
-    <t>_56A3372E-CE9C-11D2-9F0E-006097C686F6_12</t>
-  </si>
-  <si>
-    <t>_56A3372E-CE9C-11D2-9F0E-006097C686F6_39</t>
-  </si>
-  <si>
-    <t>_56A3372E-CE9C-11D2-9F0E-006097C686F6_37</t>
-  </si>
-  <si>
-    <t>_D0A04F0A-462A-48A4-BB2F-3706E88DBD7D_100</t>
-  </si>
-  <si>
-    <t>_F334115E-DA1B-4509-9B3D-119504DC7ABB_15</t>
-  </si>
-  <si>
-    <t>_D5CDD502-2E9C-101B-9397-08002B2CF9AE_5</t>
-  </si>
-  <si>
-    <t>_D5CDD502-2E9C-101B-9397-08002B2CF9AE_6</t>
-  </si>
-  <si>
-    <t>_AEAC19E4-89AE-4508-B9B7-BB867ABEE2ED_2</t>
-  </si>
-  <si>
-    <t>_E08805C8-E395-40DF-80D2-54F0D6C43154_100</t>
-  </si>
-  <si>
-    <t>_6444048F-4C8B-11D1-8B70-080036B11A03_7</t>
-  </si>
-  <si>
-    <t>_14B81DA1-0135-4D31-96D9-6CBFC9671A99_259</t>
-  </si>
-  <si>
-    <t>_6444048F-4C8B-11D1-8B70-080036B11A03_3</t>
-  </si>
-  <si>
-    <t>_6444048F-4C8B-11D1-8B70-080036B11A03_4</t>
-  </si>
-  <si>
-    <t>_14B81DA1-0135-4D31-96D9-6CBFC9671A99_37378</t>
-  </si>
-  <si>
-    <t>_14B81DA1-0135-4D31-96D9-6CBFC9671A99_36867</t>
-  </si>
-  <si>
-    <t>_F85BF840-A925-4BC2-B0C4-8E36B598679E_100</t>
-  </si>
-  <si>
-    <t>_14B81DA1-0135-4D31-96D9-6CBFC9671A99_18248</t>
-  </si>
-  <si>
-    <t>_14B81DA1-0135-4D31-96D9-6CBFC9671A99_37380</t>
-  </si>
-  <si>
-    <t>_14B81DA1-0135-4D31-96D9-6CBFC9671A99_33434</t>
-  </si>
-  <si>
-    <t>_2D152B40-CA39-40DB-B2CC-573725B2FEC5_100</t>
-  </si>
-  <si>
-    <t>_14B81DA1-0135-4D31-96D9-6CBFC9671A99_37386</t>
-  </si>
-  <si>
-    <t>_14B81DA1-0135-4D31-96D9-6CBFC9671A99_34855</t>
-  </si>
-  <si>
-    <t>_14B81DA1-0135-4D31-96D9-6CBFC9671A99_37383</t>
-  </si>
-  <si>
-    <t>_E8309B6E-084C-49B4-B1FC-90A80331B638_100</t>
-  </si>
-  <si>
-    <t>_14B81DA1-0135-4D31-96D9-6CBFC9671A99_37377</t>
-  </si>
-  <si>
-    <t>_14B81DA1-0135-4D31-96D9-6CBFC9671A99_37382</t>
-  </si>
-  <si>
-    <t>_EE3D3D8A-5381-4CFA-B13B-AAF66B5F4EC9_100</t>
-  </si>
-  <si>
-    <t>_A0E74609-B84D-4F49-B860-462BD9971F98_100</t>
-  </si>
-  <si>
-    <t>_D35F743A-EB2E-47F2-A286-844132CB1427_100</t>
-  </si>
-  <si>
-    <t>_14B81DA1-0135-4D31-96D9-6CBFC9671A99_34850</t>
-  </si>
-  <si>
-    <t>_14B81DA1-0135-4D31-96D9-6CBFC9671A99}_33437</t>
-  </si>
-  <si>
-    <t>_E6DDCAF7-29C5-4F0A-9A68-D19412EC7090_100</t>
-  </si>
-  <si>
-    <t>_E1277516-2B5F-4869-89B1-2E585BD38B7A_100</t>
-  </si>
-  <si>
-    <t>_6D217F6D-3F6A-4825-B470-5F03CA2FBE9B_100</t>
-  </si>
-  <si>
-    <t>_49237325-A95A-4F67-B211-816B2D45D2E0_100</t>
-  </si>
-  <si>
-    <t>_64440492-4C8B-11D1-8B70-080036B11A03_27</t>
-  </si>
-  <si>
-    <t>_64440492-4C8B-11D1-8B70-080036B11A03_28</t>
-  </si>
-  <si>
-    <t>_2E4B640D-5019-46D8-8881-55414CC5CAA0_100</t>
-  </si>
-  <si>
-    <t>_64440490-4C8B-11D1-8B70-080036B11A03_3</t>
-  </si>
-  <si>
-    <t>_64440492-4C8B-11D1-8B70-080036B11A03_36</t>
-  </si>
-  <si>
-    <t>_6444048F-4C8B-11D1-8B70-080036B11A03_12</t>
-  </si>
-  <si>
-    <t>_64440492-4C8B-11D1-8B70-080036B11A03_22</t>
-  </si>
-  <si>
-    <t>_64440492-4C8B-11D1-8B70-080036B11A03_39</t>
-  </si>
-  <si>
-    <t>_64440492-4C8B-11D1-8B70-080036B11A03_30</t>
-  </si>
-  <si>
-    <t>_56A3372E-CE9C-11D2-9F0E-006097C686F6_38</t>
-  </si>
-  <si>
-    <t>_64440492-4C8B-11D1-8B70-080036B11A03_23</t>
-  </si>
-  <si>
-    <t>_64440492-4C8B-11D1-8B70-080036B11A03_21</t>
-  </si>
-  <si>
-    <t>_64440491-4C8B-11D1-8B70-080036B11A03_10</t>
-  </si>
-  <si>
-    <t>_64440492-4C8B-11D1-8B70-080036B11A03_20</t>
-  </si>
-  <si>
-    <t>_64440491-4C8B-11D1-8B70-080036B11A03_8</t>
-  </si>
-  <si>
-    <t>_64440491-4C8B-11D1-8B70-080036B11A03_44</t>
-  </si>
-  <si>
-    <t>_64440491-4C8B-11D1-8B70-080036B11A03_42</t>
-  </si>
-  <si>
-    <t>_64440491-4C8B-11D1-8B70-080036B11A03_45</t>
-  </si>
-  <si>
-    <t>_64440491-4C8B-11D1-8B70-080036B11A03_43</t>
-  </si>
-  <si>
-    <t>_0CEF7D53-FA64-11D1-A203-0000F81FEDEE_3</t>
-  </si>
-  <si>
-    <t>_0CEF7D53-FA64-11D1-A203-0000F81FEDEE_4</t>
-  </si>
-  <si>
-    <t>_841E4F90-FF59-4D16-8947-E81BBFFAB36D_16</t>
-  </si>
-  <si>
-    <t>_0CEF7D53-FA64-11D1-A203-0000F81FEDEE_7</t>
-  </si>
-  <si>
-    <t>_0CEF7D53-FA64-11D1-A203-0000F81FEDEE_8</t>
-  </si>
-  <si>
-    <t>_D5CDD502-2E9C-101B-9397-08002B2CF9AE_29</t>
-  </si>
-  <si>
-    <t>_64440492-4C8B-11D1-8B70-080036B11A03_11</t>
-  </si>
-  <si>
-    <t>_6D748DE2-8D38-4CC3-AC60-F009B057C557_7</t>
-  </si>
-  <si>
-    <t>_6D748DE2-8D38-4CC3-AC60-F009B057C557_2</t>
-  </si>
-  <si>
-    <t>_6D748DE2-8D38-4CC3-AC60-F009B057C557_12</t>
-  </si>
-  <si>
-    <t>_6D748DE2-8D38-4CC3-AC60-F009B057C557_17</t>
-  </si>
-  <si>
-    <t>_6D748DE2-8D38-4CC3-AC60-F009B057C557_18</t>
-  </si>
-  <si>
-    <t>_6D748DE2-8D38-4CC3-AC60-F009B057C557_13</t>
-  </si>
-  <si>
-    <t>_2C53C813-FB63-4E22-A1AB-0B331CA1E273_100</t>
-  </si>
-  <si>
-    <t>_4684FE97-8765-4842-9C13-F006447B178C_100</t>
-  </si>
-  <si>
-    <t>_6D748DE2-8D38-4CC3-AC60-F009B057C557_3</t>
-  </si>
-  <si>
-    <t>_A5477F61-7A82-4ECA-9DDE-98B69B2479B3_100</t>
-  </si>
-  <si>
-    <t>_2CBAA8F5-D81F-47CA-B17A-F8D822300131_100</t>
-  </si>
-  <si>
-    <t>_43F8D7B7-A444-4F87-9383-52271C9B915C_100</t>
-  </si>
-  <si>
-    <t>_14B81DA1-0135-4D31-96D9-6CBFC9671A99_18258</t>
-  </si>
-  <si>
-    <t>_72FAB781-ACDA-43E5-B155-B2434F85E678_100</t>
-  </si>
-  <si>
-    <t>_DE41CC29-6971-4290-B472-F59F2E2F31E2_100</t>
-  </si>
-  <si>
-    <t>_5CBF2787-48CF-4208-B90E-EE5E5D420294_23</t>
-  </si>
-  <si>
-    <t>_64440492-4C8B-11D1-8B70-080036B11A03_9</t>
-  </si>
-  <si>
-    <t>_000214A1-0000-0000-C000-000000000046_9</t>
-  </si>
-  <si>
-    <t>_28636AA6-953D-11D2-B5D6-00C04FD918D0_14</t>
-  </si>
-  <si>
     <t>Document last saved</t>
   </si>
   <si>
@@ -2717,115 +2387,445 @@
     <t>D5CDD502-2E9C-101B-9397-08002B2CF9AE/8</t>
   </si>
   <si>
-    <t>_D5CDD502-2E9C-101B-9397-08002B2CF9AE_8</t>
-  </si>
-  <si>
     <t>D5CDD502-2E9C-101B-9397-08002B2CF9AE/9</t>
   </si>
   <si>
-    <t>_D5CDD502-2E9C-101B-9397-08002B2CF9AE_9</t>
-  </si>
-  <si>
     <t>D5CDD502-2E9C-101B-9397-08002B2CF9AE/10</t>
   </si>
   <si>
-    <t>_D5CDD502-2E9C-101B-9397-08002B2CF9AE_10</t>
-  </si>
-  <si>
     <t>D5CDD502-2E9C-101B-9397-08002B2CF9AE/11</t>
   </si>
   <si>
-    <t>_D5CDD502-2E9C-101B-9397-08002B2CF9AE_11</t>
-  </si>
-  <si>
     <t>D5CDD502-2E9C-101B-9397-08002B2CF9AE/12</t>
   </si>
   <si>
-    <t>_D5CDD502-2E9C-101B-9397-08002B2CF9AE_12</t>
-  </si>
-  <si>
     <t>D5CDD502-2E9C-101B-9397-08002B2CF9AE/13</t>
   </si>
   <si>
-    <t>_D5CDD502-2E9C-101B-9397-08002B2CF9AE_13</t>
-  </si>
-  <si>
     <t>D5CDD502-2E9C-101B-9397-08002B2CF9AE/16</t>
   </si>
   <si>
-    <t>_D5CDD502-2E9C-101B-9397-08002B2CF9AE_16</t>
-  </si>
-  <si>
     <t>D5CDD502-2E9C-101B-9397-08002B2CF9AE/17</t>
   </si>
   <si>
-    <t>_D5CDD502-2E9C-101B-9397-08002B2CF9AE_17</t>
-  </si>
-  <si>
     <t>D5CDD502-2E9C-101B-9397-08002B2CF9AE/18</t>
   </si>
   <si>
-    <t>_D5CDD502-2E9C-101B-9397-08002B2CF9AE_18</t>
-  </si>
-  <si>
     <t>D5CDD502-2E9C-101B-9397-08002B2CF9AE/19</t>
   </si>
   <si>
-    <t>_D5CDD502-2E9C-101B-9397-08002B2CF9AE_19</t>
-  </si>
-  <si>
     <t>D5CDD502-2E9C-101B-9397-08002B2CF9AE/22</t>
   </si>
   <si>
-    <t>_D5CDD502-2E9C-101B-9397-08002B2CF9AE_22</t>
-  </si>
-  <si>
     <t>D5CDD502-2E9C-101B-9397-08002B2CF9AE/23</t>
   </si>
   <si>
-    <t>_D5CDD502-2E9C-101B-9397-08002B2CF9AE_23</t>
-  </si>
-  <si>
     <t>D5CDD502-2E9C-101B-9397-08002B2CF9AE/27</t>
   </si>
   <si>
-    <t>_D5CDD502-2E9C-101B-9397-08002B2CF9AE_27</t>
-  </si>
-  <si>
     <t>D5CDD502-2E9C-101B-9397-08002B2CF9AE/28</t>
   </si>
   <si>
-    <t>_D5CDD502-2E9C-101B-9397-08002B2CF9AE_28</t>
-  </si>
-  <si>
     <t>D5CDD505-2E9C-101B-9397-08002B2CF9AE/_PID_HLINKS</t>
   </si>
   <si>
-    <t>_D5CDD505-2E9C-101B-9397-08002B2CF9AE__PID_HLINKS</t>
-  </si>
-  <si>
     <t>D5CDD505-2E9C-101B-9397-08002B2CF9AE/_SHAREDFILEINDEX</t>
   </si>
   <si>
-    <t>_D5CDD505-2E9C-101B-9397-08002B2CF9AE__SHAREDFILEINDEX</t>
-  </si>
-  <si>
     <t>D5CDD505-2E9C-101B-9397-08002B2CF9AE/_SOURCEURL</t>
   </si>
   <si>
-    <t>_D5CDD505-2E9C-101B-9397-08002B2CF9AE__SOURCEURL</t>
-  </si>
-  <si>
     <t>D5CDD505-2E9C-101B-9397-08002B2CF9AE/CONTENTTYPE</t>
   </si>
   <si>
-    <t>_D5CDD505-2E9C-101B-9397-08002B2CF9AE_CONTENTTYPE</t>
-  </si>
-  <si>
     <t>D5CDD505-2E9C-101B-9397-08002B2CF9AE/CONTENTTYPEID</t>
   </si>
   <si>
-    <t>_D5CDD505-2E9C-101B-9397-08002B2CF9AE_CONTENTTYPEID</t>
+    <t>_F7DB74B4_4287_4103_AFBA_F1B13DCD75CF_100</t>
+  </si>
+  <si>
+    <t>_28636AA6_953D_11D2_B5D6_00C04FD918D0_11</t>
+  </si>
+  <si>
+    <t>_D5CDD502_2E9C_101B_9397_08002B2CF9AE_26</t>
+  </si>
+  <si>
+    <t>_1E3EE840_BC2B_476C_8237_2ACD1A839B22_3</t>
+  </si>
+  <si>
+    <t>_E4F10A3C_49E6_405D_8288_A23BD4EEAA6C_100</t>
+  </si>
+  <si>
+    <t>_28636AA6_953D_11D2_B5D6_00C04FD918D0_12</t>
+  </si>
+  <si>
+    <t>_EF884C5B_2BFE_41BB_AAE5_76EEDF4F9902_100</t>
+  </si>
+  <si>
+    <t>_EF884C5B_2BFE_41BB_AAE5_76EEDF4F9902_200</t>
+  </si>
+  <si>
+    <t>_EF884C5B_2BFE_41BB_AAE5_76EEDF4F9902_300</t>
+  </si>
+  <si>
+    <t>_B725F130_47EF_101A_A5F1_02608C9EEBAC_16</t>
+  </si>
+  <si>
+    <t>_B725F130_47EF_101A_A5F1_02608C9EEBAC_13</t>
+  </si>
+  <si>
+    <t>_9B174B34_40FF_11D2_A27E_00C04FC30871_4</t>
+  </si>
+  <si>
+    <t>_28636AA6_953D_11D2_B5D6_00C04FD918D0_5</t>
+  </si>
+  <si>
+    <t>_90E5E14E_648B_4826_B2AA_ACAF790E3513_10</t>
+  </si>
+  <si>
+    <t>_A94688B6_7D9F_4570_A648_E3DFC0AB2B3F_100</t>
+  </si>
+  <si>
+    <t>_6D24888F_4718_4BDA_AFED_EA0FB4386CD8_100</t>
+  </si>
+  <si>
+    <t>_B9B4B3FC_2B51_4A42_B5D8_324146AFCF25_2</t>
+  </si>
+  <si>
+    <t>_E3E0584C_B788_4A5A_BB20_7F5A44C9ACDD_6</t>
+  </si>
+  <si>
+    <t>_64440490_4C8B_11D1_8B70_080036B11A03_7</t>
+  </si>
+  <si>
+    <t>_64440490_4C8B_11D1_8B70_080036B11A03_5</t>
+  </si>
+  <si>
+    <t>_64440490_4C8B_11D1_8B70_080036B11A03_8</t>
+  </si>
+  <si>
+    <t>_56A3372E_CE9C_11D2_9F0E_006097C686F6_13</t>
+  </si>
+  <si>
+    <t>_56A3372E_CE9C_11D2_9F0E_006097C686F6_100</t>
+  </si>
+  <si>
+    <t>_FD122953_FA93_4EF7_92C3_04C946B2F7C8_100</t>
+  </si>
+  <si>
+    <t>_56A3372E_CE9C_11D2_9F0E_006097C686F6_35</t>
+  </si>
+  <si>
+    <t>_64440492_4C8B_11D1_8B70_080036B11A03_19</t>
+  </si>
+  <si>
+    <t>_56A3372E_CE9C_11D2_9F0E_006097C686F6_36</t>
+  </si>
+  <si>
+    <t>_56A3372E_CE9C_11D2_9F0E_006097C686F6_12</t>
+  </si>
+  <si>
+    <t>_56A3372E_CE9C_11D2_9F0E_006097C686F6_39</t>
+  </si>
+  <si>
+    <t>_56A3372E_CE9C_11D2_9F0E_006097C686F6_37</t>
+  </si>
+  <si>
+    <t>_D0A04F0A_462A_48A4_BB2F_3706E88DBD7D_100</t>
+  </si>
+  <si>
+    <t>_F334115E_DA1B_4509_9B3D_119504DC7ABB_15</t>
+  </si>
+  <si>
+    <t>_D5CDD502_2E9C_101B_9397_08002B2CF9AE_5</t>
+  </si>
+  <si>
+    <t>_D5CDD502_2E9C_101B_9397_08002B2CF9AE_6</t>
+  </si>
+  <si>
+    <t>_AEAC19E4_89AE_4508_B9B7_BB867ABEE2ED_2</t>
+  </si>
+  <si>
+    <t>_E08805C8_E395_40DF_80D2_54F0D6C43154_100</t>
+  </si>
+  <si>
+    <t>_6444048F_4C8B_11D1_8B70_080036B11A03_7</t>
+  </si>
+  <si>
+    <t>_14B81DA1_0135_4D31_96D9_6CBFC9671A99_259</t>
+  </si>
+  <si>
+    <t>_6444048F_4C8B_11D1_8B70_080036B11A03_3</t>
+  </si>
+  <si>
+    <t>_6444048F_4C8B_11D1_8B70_080036B11A03_4</t>
+  </si>
+  <si>
+    <t>_14B81DA1_0135_4D31_96D9_6CBFC9671A99_37378</t>
+  </si>
+  <si>
+    <t>_14B81DA1_0135_4D31_96D9_6CBFC9671A99_36867</t>
+  </si>
+  <si>
+    <t>_F85BF840_A925_4BC2_B0C4_8E36B598679E_100</t>
+  </si>
+  <si>
+    <t>_14B81DA1_0135_4D31_96D9_6CBFC9671A99_18248</t>
+  </si>
+  <si>
+    <t>_14B81DA1_0135_4D31_96D9_6CBFC9671A99_37380</t>
+  </si>
+  <si>
+    <t>_14B81DA1_0135_4D31_96D9_6CBFC9671A99_33434</t>
+  </si>
+  <si>
+    <t>_2D152B40_CA39_40DB_B2CC_573725B2FEC5_100</t>
+  </si>
+  <si>
+    <t>_14B81DA1_0135_4D31_96D9_6CBFC9671A99_37386</t>
+  </si>
+  <si>
+    <t>_14B81DA1_0135_4D31_96D9_6CBFC9671A99_34855</t>
+  </si>
+  <si>
+    <t>_14B81DA1_0135_4D31_96D9_6CBFC9671A99_37383</t>
+  </si>
+  <si>
+    <t>_E8309B6E_084C_49B4_B1FC_90A80331B638_100</t>
+  </si>
+  <si>
+    <t>_14B81DA1_0135_4D31_96D9_6CBFC9671A99_37377</t>
+  </si>
+  <si>
+    <t>_14B81DA1_0135_4D31_96D9_6CBFC9671A99_37382</t>
+  </si>
+  <si>
+    <t>_EE3D3D8A_5381_4CFA_B13B_AAF66B5F4EC9_100</t>
+  </si>
+  <si>
+    <t>_A0E74609_B84D_4F49_B860_462BD9971F98_100</t>
+  </si>
+  <si>
+    <t>_D35F743A_EB2E_47F2_A286_844132CB1427_100</t>
+  </si>
+  <si>
+    <t>_14B81DA1_0135_4D31_96D9_6CBFC9671A99_34850</t>
+  </si>
+  <si>
+    <t>_E6DDCAF7_29C5_4F0A_9A68_D19412EC7090_100</t>
+  </si>
+  <si>
+    <t>_E1277516_2B5F_4869_89B1_2E585BD38B7A_100</t>
+  </si>
+  <si>
+    <t>_6D217F6D_3F6A_4825_B470_5F03CA2FBE9B_100</t>
+  </si>
+  <si>
+    <t>_49237325_A95A_4F67_B211_816B2D45D2E0_100</t>
+  </si>
+  <si>
+    <t>_64440492_4C8B_11D1_8B70_080036B11A03_27</t>
+  </si>
+  <si>
+    <t>_64440492_4C8B_11D1_8B70_080036B11A03_28</t>
+  </si>
+  <si>
+    <t>_2E4B640D_5019_46D8_8881_55414CC5CAA0_100</t>
+  </si>
+  <si>
+    <t>_64440490_4C8B_11D1_8B70_080036B11A03_3</t>
+  </si>
+  <si>
+    <t>_64440492_4C8B_11D1_8B70_080036B11A03_36</t>
+  </si>
+  <si>
+    <t>_6444048F_4C8B_11D1_8B70_080036B11A03_12</t>
+  </si>
+  <si>
+    <t>_64440492_4C8B_11D1_8B70_080036B11A03_22</t>
+  </si>
+  <si>
+    <t>_64440492_4C8B_11D1_8B70_080036B11A03_39</t>
+  </si>
+  <si>
+    <t>_64440492_4C8B_11D1_8B70_080036B11A03_30</t>
+  </si>
+  <si>
+    <t>_56A3372E_CE9C_11D2_9F0E_006097C686F6_38</t>
+  </si>
+  <si>
+    <t>_64440492_4C8B_11D1_8B70_080036B11A03_23</t>
+  </si>
+  <si>
+    <t>_64440492_4C8B_11D1_8B70_080036B11A03_21</t>
+  </si>
+  <si>
+    <t>_64440491_4C8B_11D1_8B70_080036B11A03_10</t>
+  </si>
+  <si>
+    <t>_64440492_4C8B_11D1_8B70_080036B11A03_20</t>
+  </si>
+  <si>
+    <t>_64440491_4C8B_11D1_8B70_080036B11A03_8</t>
+  </si>
+  <si>
+    <t>_64440491_4C8B_11D1_8B70_080036B11A03_44</t>
+  </si>
+  <si>
+    <t>_64440491_4C8B_11D1_8B70_080036B11A03_42</t>
+  </si>
+  <si>
+    <t>_64440491_4C8B_11D1_8B70_080036B11A03_45</t>
+  </si>
+  <si>
+    <t>_64440491_4C8B_11D1_8B70_080036B11A03_43</t>
+  </si>
+  <si>
+    <t>_0CEF7D53_FA64_11D1_A203_0000F81FEDEE_3</t>
+  </si>
+  <si>
+    <t>_0CEF7D53_FA64_11D1_A203_0000F81FEDEE_4</t>
+  </si>
+  <si>
+    <t>_841E4F90_FF59_4D16_8947_E81BBFFAB36D_16</t>
+  </si>
+  <si>
+    <t>_0CEF7D53_FA64_11D1_A203_0000F81FEDEE_7</t>
+  </si>
+  <si>
+    <t>_0CEF7D53_FA64_11D1_A203_0000F81FEDEE_8</t>
+  </si>
+  <si>
+    <t>_D5CDD502_2E9C_101B_9397_08002B2CF9AE_29</t>
+  </si>
+  <si>
+    <t>_64440492_4C8B_11D1_8B70_080036B11A03_11</t>
+  </si>
+  <si>
+    <t>_6D748DE2_8D38_4CC3_AC60_F009B057C557_7</t>
+  </si>
+  <si>
+    <t>_6D748DE2_8D38_4CC3_AC60_F009B057C557_2</t>
+  </si>
+  <si>
+    <t>_6D748DE2_8D38_4CC3_AC60_F009B057C557_12</t>
+  </si>
+  <si>
+    <t>_6D748DE2_8D38_4CC3_AC60_F009B057C557_17</t>
+  </si>
+  <si>
+    <t>_6D748DE2_8D38_4CC3_AC60_F009B057C557_18</t>
+  </si>
+  <si>
+    <t>_6D748DE2_8D38_4CC3_AC60_F009B057C557_13</t>
+  </si>
+  <si>
+    <t>_2C53C813_FB63_4E22_A1AB_0B331CA1E273_100</t>
+  </si>
+  <si>
+    <t>_4684FE97_8765_4842_9C13_F006447B178C_100</t>
+  </si>
+  <si>
+    <t>_6D748DE2_8D38_4CC3_AC60_F009B057C557_3</t>
+  </si>
+  <si>
+    <t>_A5477F61_7A82_4ECA_9DDE_98B69B2479B3_100</t>
+  </si>
+  <si>
+    <t>_2CBAA8F5_D81F_47CA_B17A_F8D822300131_100</t>
+  </si>
+  <si>
+    <t>_43F8D7B7_A444_4F87_9383_52271C9B915C_100</t>
+  </si>
+  <si>
+    <t>_14B81DA1_0135_4D31_96D9_6CBFC9671A99_18258</t>
+  </si>
+  <si>
+    <t>_72FAB781_ACDA_43E5_B155_B2434F85E678_100</t>
+  </si>
+  <si>
+    <t>_DE41CC29_6971_4290_B472_F59F2E2F31E2_100</t>
+  </si>
+  <si>
+    <t>_5CBF2787_48CF_4208_B90E_EE5E5D420294_23</t>
+  </si>
+  <si>
+    <t>_64440492_4C8B_11D1_8B70_080036B11A03_9</t>
+  </si>
+  <si>
+    <t>_000214A1_0000_0000_C000_000000000046_9</t>
+  </si>
+  <si>
+    <t>_28636AA6_953D_11D2_B5D6_00C04FD918D0_14</t>
+  </si>
+  <si>
+    <t>_D5CDD502_2E9C_101B_9397_08002B2CF9AE_8</t>
+  </si>
+  <si>
+    <t>_D5CDD502_2E9C_101B_9397_08002B2CF9AE_9</t>
+  </si>
+  <si>
+    <t>_D5CDD502_2E9C_101B_9397_08002B2CF9AE_10</t>
+  </si>
+  <si>
+    <t>_D5CDD502_2E9C_101B_9397_08002B2CF9AE_11</t>
+  </si>
+  <si>
+    <t>_D5CDD502_2E9C_101B_9397_08002B2CF9AE_12</t>
+  </si>
+  <si>
+    <t>_D5CDD502_2E9C_101B_9397_08002B2CF9AE_13</t>
+  </si>
+  <si>
+    <t>_D5CDD502_2E9C_101B_9397_08002B2CF9AE_16</t>
+  </si>
+  <si>
+    <t>_D5CDD502_2E9C_101B_9397_08002B2CF9AE_17</t>
+  </si>
+  <si>
+    <t>_D5CDD502_2E9C_101B_9397_08002B2CF9AE_18</t>
+  </si>
+  <si>
+    <t>_D5CDD502_2E9C_101B_9397_08002B2CF9AE_19</t>
+  </si>
+  <si>
+    <t>_D5CDD502_2E9C_101B_9397_08002B2CF9AE_22</t>
+  </si>
+  <si>
+    <t>_D5CDD502_2E9C_101B_9397_08002B2CF9AE_23</t>
+  </si>
+  <si>
+    <t>_D5CDD502_2E9C_101B_9397_08002B2CF9AE_27</t>
+  </si>
+  <si>
+    <t>_D5CDD502_2E9C_101B_9397_08002B2CF9AE_28</t>
+  </si>
+  <si>
+    <t>_D5CDD505_2E9C_101B_9397_08002B2CF9AE__PID_HLINKS</t>
+  </si>
+  <si>
+    <t>_D5CDD505_2E9C_101B_9397_08002B2CF9AE__SHAREDFILEINDEX</t>
+  </si>
+  <si>
+    <t>_D5CDD505_2E9C_101B_9397_08002B2CF9AE__SOURCEURL</t>
+  </si>
+  <si>
+    <t>_D5CDD505_2E9C_101B_9397_08002B2CF9AE_CONTENTTYPE</t>
+  </si>
+  <si>
+    <t>_D5CDD505_2E9C_101B_9397_08002B2CF9AE_CONTENTTYPEID</t>
+  </si>
+  <si>
+    <t>49691C90-7E17-101A-A91C-08002B2ECDA9/3</t>
+  </si>
+  <si>
+    <t>_49691C90_7E17_101A_A91C_08002B2ECDA9_3</t>
+  </si>
+  <si>
+    <t>14B81DA1-0135-4D31-96D9-6CBFC9671A99/33437</t>
+  </si>
+  <si>
+    <t>_14B81DA1_0135_4D31_96D9_6CBFC9671A99_33437</t>
   </si>
 </sst>
 </file>
@@ -3156,8 +3156,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E272"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C250" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D272"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3182,7 +3182,7 @@
         <v>33</v>
       </c>
       <c r="E1" t="str">
-        <f>CONCATENATE("_properties.Add(""",A1,""", LanguageConsts.",B1,");")</f>
+        <f t="shared" ref="E1:E32" si="0">CONCATENATE("_properties.Add(""",A1,""", LanguageConsts.",B1,");")</f>
         <v>_properties.Add("0B63E350-9CCC-11D0-BCDB-00805FCCCE04/4", LanguageConsts._0B63E350_9CCC_11D0_BCDB_00805FCCCE04_4);</v>
       </c>
     </row>
@@ -3200,7 +3200,7 @@
         <v>243</v>
       </c>
       <c r="E2" t="str">
-        <f>CONCATENATE("_properties.Add(""",A2,""", LanguageConsts.",B2,");")</f>
+        <f t="shared" si="0"/>
         <v>_properties.Add("0B63E350-9CCC-11D0-BCDB-00805FCCCE04/5", LanguageConsts._0B63E350_9CCC_11D0_BCDB_00805FCCCE04_5);</v>
       </c>
     </row>
@@ -3218,7 +3218,7 @@
         <v>100</v>
       </c>
       <c r="E3" t="str">
-        <f>CONCATENATE("_properties.Add(""",A3,""", LanguageConsts.",B3,");")</f>
+        <f t="shared" si="0"/>
         <v>_properties.Add("14B81DA1-0135-4D31-96D9-6CBFC9671A99/271", LanguageConsts._14B81DA1_0135_4D31_96D9_6CBFC9671A99_271);</v>
       </c>
     </row>
@@ -3236,7 +3236,7 @@
         <v>101</v>
       </c>
       <c r="E4" t="str">
-        <f>CONCATENATE("_properties.Add(""",A4,""", LanguageConsts.",B4,");")</f>
+        <f t="shared" si="0"/>
         <v>_properties.Add("14B81DA1-0135-4D31-96D9-6CBFC9671A99/272", LanguageConsts._14B81DA1_0135_4D31_96D9_6CBFC9671A99_272);</v>
       </c>
     </row>
@@ -3254,7 +3254,7 @@
         <v>103</v>
       </c>
       <c r="E5" t="str">
-        <f>CONCATENATE("_properties.Add(""",A5,""", LanguageConsts.",B5,");")</f>
+        <f t="shared" si="0"/>
         <v>_properties.Add("14B81DA1-0135-4D31-96D9-6CBFC9671A99/274", LanguageConsts._14B81DA1_0135_4D31_96D9_6CBFC9671A99_274);</v>
       </c>
     </row>
@@ -3272,7 +3272,7 @@
         <v>240</v>
       </c>
       <c r="E6" t="str">
-        <f>CONCATENATE("_properties.Add(""",A6,""", LanguageConsts.",B6,");")</f>
+        <f t="shared" si="0"/>
         <v>_properties.Add("49691C90-7E17-101A-A91C-08002B2ECDA9/9", LanguageConsts._49691C90_7E17_101A_A91C_08002B2ECDA9_9);</v>
       </c>
     </row>
@@ -3290,7 +3290,7 @@
         <v>97</v>
       </c>
       <c r="E7" t="str">
-        <f>CONCATENATE("_properties.Add(""",A7,""", LanguageConsts.",B7,");")</f>
+        <f t="shared" si="0"/>
         <v>_properties.Add("56A3372E-CE9C-11D2-9F0E-006097C686F6/11", LanguageConsts._56A3372E_CE9C_11D2_9F0E_006097C686F6_11);</v>
       </c>
     </row>
@@ -3308,7 +3308,7 @@
         <v>96</v>
       </c>
       <c r="E8" t="str">
-        <f>CONCATENATE("_properties.Add(""",A8,""", LanguageConsts.",B8,");")</f>
+        <f t="shared" si="0"/>
         <v>_properties.Add("56A3372E-CE9C-11D2-9F0E-006097C686F6/2", LanguageConsts._56A3372E_CE9C_11D2_9F0E_006097C686F6_2);</v>
       </c>
     </row>
@@ -3326,7 +3326,7 @@
         <v>95</v>
       </c>
       <c r="E9" t="str">
-        <f>CONCATENATE("_properties.Add(""",A9,""", LanguageConsts.",B9,");")</f>
+        <f t="shared" si="0"/>
         <v>_properties.Add("56A3372E-CE9C-11D2-9F0E-006097C686F6/4", LanguageConsts._56A3372E_CE9C_11D2_9F0E_006097C686F6_4);</v>
       </c>
     </row>
@@ -3344,7 +3344,7 @@
         <v>99</v>
       </c>
       <c r="E10" t="str">
-        <f>CONCATENATE("_properties.Add(""",A10,""", LanguageConsts.",B10,");")</f>
+        <f t="shared" si="0"/>
         <v>_properties.Add("56A3372E-CE9C-11D2-9F0E-006097C686F6/5", LanguageConsts._56A3372E_CE9C_11D2_9F0E_006097C686F6_5);</v>
       </c>
     </row>
@@ -3362,7 +3362,7 @@
         <v>98</v>
       </c>
       <c r="E11" t="str">
-        <f>CONCATENATE("_properties.Add(""",A11,""", LanguageConsts.",B11,");")</f>
+        <f t="shared" si="0"/>
         <v>_properties.Add("56A3372E-CE9C-11D2-9F0E-006097C686F6/7", LanguageConsts._56A3372E_CE9C_11D2_9F0E_006097C686F6_7);</v>
       </c>
     </row>
@@ -3380,7 +3380,7 @@
         <v>94</v>
       </c>
       <c r="E12" t="str">
-        <f>CONCATENATE("_properties.Add(""",A12,""", LanguageConsts.",B12,");")</f>
+        <f t="shared" si="0"/>
         <v>_properties.Add("56A3372E-CE9C-11D2-9F0E-006097C686F6/8", LanguageConsts._56A3372E_CE9C_11D2_9F0E_006097C686F6_8);</v>
       </c>
     </row>
@@ -3398,7 +3398,7 @@
         <v>104</v>
       </c>
       <c r="E13" t="str">
-        <f>CONCATENATE("_properties.Add(""",A13,""", LanguageConsts.",B13,");")</f>
+        <f t="shared" si="0"/>
         <v>_properties.Add("6444048F-4C8B-11D1-8B70-080036B11A03/13", LanguageConsts._6444048F_4C8B_11D1_8B70_080036B11A03_13);</v>
       </c>
     </row>
@@ -3416,7 +3416,7 @@
         <v>105</v>
       </c>
       <c r="E14" t="str">
-        <f>CONCATENATE("_properties.Add(""",A14,""", LanguageConsts.",B14,");")</f>
+        <f t="shared" si="0"/>
         <v>_properties.Add("6444048F-4C8B-11D1-8B70-080036B11A03/5", LanguageConsts._6444048F_4C8B_11D1_8B70_080036B11A03_5);</v>
       </c>
     </row>
@@ -3434,7 +3434,7 @@
         <v>106</v>
       </c>
       <c r="E15" t="str">
-        <f>CONCATENATE("_properties.Add(""",A15,""", LanguageConsts.",B15,");")</f>
+        <f t="shared" si="0"/>
         <v>_properties.Add("6444048F-4C8B-11D1-8B70-080036B11A03/6", LanguageConsts._6444048F_4C8B_11D1_8B70_080036B11A03_6);</v>
       </c>
     </row>
@@ -3452,7 +3452,7 @@
         <v>93</v>
       </c>
       <c r="E16" t="str">
-        <f>CONCATENATE("_properties.Add(""",A16,""", LanguageConsts.",B16,");")</f>
+        <f t="shared" si="0"/>
         <v>_properties.Add("64440490-4C8B-11D1-8B70-080036B11A03/4", LanguageConsts._64440490_4C8B_11D1_8B70_080036B11A03_4);</v>
       </c>
     </row>
@@ -3470,7 +3470,7 @@
         <v>109</v>
       </c>
       <c r="E17" t="str">
-        <f>CONCATENATE("_properties.Add(""",A17,""", LanguageConsts.",B17,");")</f>
+        <f t="shared" si="0"/>
         <v>_properties.Add("64440491-4C8B-11D1-8B70-080036B11A03/3", LanguageConsts._64440491_4C8B_11D1_8B70_080036B11A03_3);</v>
       </c>
     </row>
@@ -3488,7 +3488,7 @@
         <v>107</v>
       </c>
       <c r="E18" t="str">
-        <f>CONCATENATE("_properties.Add(""",A18,""", LanguageConsts.",B18,");")</f>
+        <f t="shared" si="0"/>
         <v>_properties.Add("64440491-4C8B-11D1-8B70-080036B11A03/4", LanguageConsts._64440491_4C8B_11D1_8B70_080036B11A03_4);</v>
       </c>
     </row>
@@ -3506,7 +3506,7 @@
         <v>108</v>
       </c>
       <c r="E19" t="str">
-        <f>CONCATENATE("_properties.Add(""",A19,""", LanguageConsts.",B19,");")</f>
+        <f t="shared" si="0"/>
         <v>_properties.Add("64440491-4C8B-11D1-8B70-080036B11A03/6", LanguageConsts._64440491_4C8B_11D1_8B70_080036B11A03_6);</v>
       </c>
     </row>
@@ -3524,7 +3524,7 @@
         <v>111</v>
       </c>
       <c r="E20" t="str">
-        <f>CONCATENATE("_properties.Add(""",A20,""", LanguageConsts.",B20,");")</f>
+        <f t="shared" si="0"/>
         <v>_properties.Add("8DEE0300-16C2-101B-B121-08002B2ECDA9/CLASS", LanguageConsts._8DEE0300_16C2_101B_B121_08002B2ECDA9_class);</v>
       </c>
     </row>
@@ -3542,7 +3542,7 @@
         <v>133</v>
       </c>
       <c r="E21" t="str">
-        <f>CONCATENATE("_properties.Add(""",A21,""", LanguageConsts.",B21,");")</f>
+        <f t="shared" si="0"/>
         <v>_properties.Add("8DEE0300-16C2-101B-B121-08002B2ECDA9/COMPONENT", LanguageConsts._8DEE0300_16C2_101B_B121_08002B2ECDA9_component);</v>
       </c>
     </row>
@@ -3560,7 +3560,7 @@
         <v>125</v>
       </c>
       <c r="E22" t="str">
-        <f>CONCATENATE("_properties.Add(""",A22,""", LanguageConsts.",B22,");")</f>
+        <f t="shared" si="0"/>
         <v>_properties.Add("8DEE0300-16C2-101B-B121-08002B2ECDA9/CONST", LanguageConsts._8DEE0300_16C2_101B_B121_08002B2ECDA9_const);</v>
       </c>
     </row>
@@ -3578,7 +3578,7 @@
         <v>131</v>
       </c>
       <c r="E23" t="str">
-        <f>CONCATENATE("_properties.Add(""",A23,""", LanguageConsts.",B23,");")</f>
+        <f t="shared" si="0"/>
         <v>_properties.Add("8DEE0300-16C2-101B-B121-08002B2ECDA9/DEF", LanguageConsts._8DEE0300_16C2_101B_B121_08002B2ECDA9_def);</v>
       </c>
     </row>
@@ -3596,7 +3596,7 @@
         <v>119</v>
       </c>
       <c r="E24" t="str">
-        <f>CONCATENATE("_properties.Add(""",A24,""", LanguageConsts.",B24,");")</f>
+        <f t="shared" si="0"/>
         <v>_properties.Add("8DEE0300-16C2-101B-B121-08002B2ECDA9/DELEGATE", LanguageConsts._8DEE0300_16C2_101B_B121_08002B2ECDA9_delegate);</v>
       </c>
     </row>
@@ -3614,7 +3614,7 @@
         <v>123</v>
       </c>
       <c r="E25" t="str">
-        <f>CONCATENATE("_properties.Add(""",A25,""", LanguageConsts.",B25,");")</f>
+        <f t="shared" si="0"/>
         <v>_properties.Add("8DEE0300-16C2-101B-B121-08002B2ECDA9/ENUM", LanguageConsts._8DEE0300_16C2_101B_B121_08002B2ECDA9_enum);</v>
       </c>
     </row>
@@ -3632,7 +3632,7 @@
         <v>127</v>
       </c>
       <c r="E26" t="str">
-        <f>CONCATENATE("_properties.Add(""",A26,""", LanguageConsts.",B26,");")</f>
+        <f t="shared" si="0"/>
         <v>_properties.Add("8DEE0300-16C2-101B-B121-08002B2ECDA9/EVENT", LanguageConsts._8DEE0300_16C2_101B_B121_08002B2ECDA9_event);</v>
       </c>
     </row>
@@ -3650,7 +3650,7 @@
         <v>129</v>
       </c>
       <c r="E27" t="str">
-        <f>CONCATENATE("_properties.Add(""",A27,""", LanguageConsts.",B27,");")</f>
+        <f t="shared" si="0"/>
         <v>_properties.Add("8DEE0300-16C2-101B-B121-08002B2ECDA9/FIELD", LanguageConsts._8DEE0300_16C2_101B_B121_08002B2ECDA9_field);</v>
       </c>
     </row>
@@ -3668,7 +3668,7 @@
         <v>113</v>
       </c>
       <c r="E28" t="str">
-        <f>CONCATENATE("_properties.Add(""",A28,""", LanguageConsts.",B28,");")</f>
+        <f t="shared" si="0"/>
         <v>_properties.Add("8DEE0300-16C2-101B-B121-08002B2ECDA9/FUNC", LanguageConsts._8DEE0300_16C2_101B_B121_08002B2ECDA9_func);</v>
       </c>
     </row>
@@ -3686,7 +3686,7 @@
         <v>117</v>
       </c>
       <c r="E29" t="str">
-        <f>CONCATENATE("_properties.Add(""",A29,""", LanguageConsts.",B29,");")</f>
+        <f t="shared" si="0"/>
         <v>_properties.Add("8DEE0300-16C2-101B-B121-08002B2ECDA9/INTERFACE", LanguageConsts._8DEE0300_16C2_101B_B121_08002B2ECDA9_interface);</v>
       </c>
     </row>
@@ -3704,7 +3704,7 @@
         <v>135</v>
       </c>
       <c r="E30" t="str">
-        <f>CONCATENATE("_properties.Add(""",A30,""", LanguageConsts.",B30,");")</f>
+        <f t="shared" si="0"/>
         <v>_properties.Add("8DEE0300-16C2-101B-B121-08002B2ECDA9/PROJECT", LanguageConsts._8DEE0300_16C2_101B_B121_08002B2ECDA9_project);</v>
       </c>
     </row>
@@ -3722,7 +3722,7 @@
         <v>121</v>
       </c>
       <c r="E31" t="str">
-        <f>CONCATENATE("_properties.Add(""",A31,""", LanguageConsts.",B31,");")</f>
+        <f t="shared" si="0"/>
         <v>_properties.Add("8DEE0300-16C2-101B-B121-08002B2ECDA9/PROPERTY", LanguageConsts._8DEE0300_16C2_101B_B121_08002B2ECDA9_property);</v>
       </c>
     </row>
@@ -3740,7 +3740,7 @@
         <v>137</v>
       </c>
       <c r="E32" t="str">
-        <f>CONCATENATE("_properties.Add(""",A32,""", LanguageConsts.",B32,");")</f>
+        <f t="shared" si="0"/>
         <v>_properties.Add("8DEE0300-16C2-101B-B121-08002B2ECDA9/SOLUTION", LanguageConsts._8DEE0300_16C2_101B_B121_08002B2ECDA9_solution);</v>
       </c>
     </row>
@@ -3758,7 +3758,7 @@
         <v>115</v>
       </c>
       <c r="E33" t="str">
-        <f>CONCATENATE("_properties.Add(""",A33,""", LanguageConsts.",B33,");")</f>
+        <f t="shared" ref="E33:E64" si="1">CONCATENATE("_properties.Add(""",A33,""", LanguageConsts.",B33,");")</f>
         <v>_properties.Add("8DEE0300-16C2-101B-B121-08002B2ECDA9/STRUCT", LanguageConsts._8DEE0300_16C2_101B_B121_08002B2ECDA9_struct);</v>
       </c>
     </row>
@@ -3776,7 +3776,7 @@
         <v>37</v>
       </c>
       <c r="E34" t="str">
-        <f>CONCATENATE("_properties.Add(""",A34,""", LanguageConsts.",B34,");")</f>
+        <f t="shared" si="1"/>
         <v>_properties.Add("B725F130-47EF-101A-A5F1-02608C9EEBAC/10", LanguageConsts._B725F130_47EF_101A_A5F1_02608C9EEBAC_10);</v>
       </c>
     </row>
@@ -3794,7 +3794,7 @@
         <v>17</v>
       </c>
       <c r="E35" t="str">
-        <f>CONCATENATE("_properties.Add(""",A35,""", LanguageConsts.",B35,");")</f>
+        <f t="shared" si="1"/>
         <v>_properties.Add("B725F130-47EF-101A-A5F1-02608C9EEBAC/12", LanguageConsts._B725F130_47EF_101A_A5F1_02608C9EEBAC_12);</v>
       </c>
     </row>
@@ -3812,7 +3812,7 @@
         <v>21</v>
       </c>
       <c r="E36" t="str">
-        <f>CONCATENATE("_properties.Add(""",A36,""", LanguageConsts.",B36,");")</f>
+        <f t="shared" si="1"/>
         <v>_properties.Add("B725F130-47EF-101A-A5F1-02608C9EEBAC/14", LanguageConsts._B725F130_47EF_101A_A5F1_02608C9EEBAC_14);</v>
       </c>
     </row>
@@ -3830,7 +3830,7 @@
         <v>1</v>
       </c>
       <c r="E37" t="str">
-        <f>CONCATENATE("_properties.Add(""",A37,""", LanguageConsts.",B37,");")</f>
+        <f t="shared" si="1"/>
         <v>_properties.Add("B725F130-47EF-101A-A5F1-02608C9EEBAC/15", LanguageConsts._B725F130_47EF_101A_A5F1_02608C9EEBAC_15);</v>
       </c>
     </row>
@@ -3848,7 +3848,7 @@
         <v>38</v>
       </c>
       <c r="E38" t="str">
-        <f>CONCATENATE("_properties.Add(""",A38,""", LanguageConsts.",B38,");")</f>
+        <f t="shared" si="1"/>
         <v>_properties.Add("B725F130-47EF-101A-A5F1-02608C9EEBAC/20", LanguageConsts._B725F130_47EF_101A_A5F1_02608C9EEBAC_20);</v>
       </c>
     </row>
@@ -3866,7 +3866,7 @@
         <v>90</v>
       </c>
       <c r="E39" t="str">
-        <f>CONCATENATE("_properties.Add(""",A39,""", LanguageConsts.",B39,");")</f>
+        <f t="shared" si="1"/>
         <v>_properties.Add("D5CDD502-2E9C-101B-9397-08002B2CF9AE/14", LanguageConsts._D5CDD502_2E9C_101B_9397_08002B2CF9AE_14);</v>
       </c>
     </row>
@@ -3884,7 +3884,7 @@
         <v>88</v>
       </c>
       <c r="E40" t="str">
-        <f>CONCATENATE("_properties.Add(""",A40,""", LanguageConsts.",B40,");")</f>
+        <f t="shared" si="1"/>
         <v>_properties.Add("D5CDD502-2E9C-101B-9397-08002B2CF9AE/15", LanguageConsts._D5CDD502_2E9C_101B_9397_08002B2CF9AE_15);</v>
       </c>
     </row>
@@ -3902,7 +3902,7 @@
         <v>3</v>
       </c>
       <c r="E41" t="str">
-        <f>CONCATENATE("_properties.Add(""",A41,""", LanguageConsts.",B41,");")</f>
+        <f t="shared" si="1"/>
         <v>_properties.Add("D5CDD502-2E9C-101B-9397-08002B2CF9AE/2", LanguageConsts._D5CDD502_2E9C_101B_9397_08002B2CF9AE_2);</v>
       </c>
     </row>
@@ -3920,7 +3920,7 @@
         <v>91</v>
       </c>
       <c r="E42" t="str">
-        <f>CONCATENATE("_properties.Add(""",A42,""", LanguageConsts.",B42,");")</f>
+        <f t="shared" si="1"/>
         <v>_properties.Add("D5CDD502-2E9C-101B-9397-08002B2CF9AE/3", LanguageConsts._D5CDD502_2E9C_101B_9397_08002B2CF9AE_3);</v>
       </c>
     </row>
@@ -3938,7 +3938,7 @@
         <v>92</v>
       </c>
       <c r="E43" t="str">
-        <f>CONCATENATE("_properties.Add(""",A43,""", LanguageConsts.",B43,");")</f>
+        <f t="shared" si="1"/>
         <v>_properties.Add("D5CDD502-2E9C-101B-9397-08002B2CF9AE/7", LanguageConsts._D5CDD502_2E9C_101B_9397_08002B2CF9AE_7);</v>
       </c>
     </row>
@@ -3956,7 +3956,7 @@
         <v>59</v>
       </c>
       <c r="E44" t="str">
-        <f>CONCATENATE("_properties.Add(""",A44,""", LanguageConsts.",B44,");")</f>
+        <f t="shared" si="1"/>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/ANNIVERSARY", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_Anniversary);</v>
       </c>
     </row>
@@ -3974,7 +3974,7 @@
         <v>60</v>
       </c>
       <c r="E45" t="str">
-        <f>CONCATENATE("_properties.Add(""",A45,""", LanguageConsts.",B45,");")</f>
+        <f t="shared" si="1"/>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/ASSISTANTNAME", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_AssistantName);</v>
       </c>
     </row>
@@ -3992,7 +3992,7 @@
         <v>61</v>
       </c>
       <c r="E46" t="str">
-        <f>CONCATENATE("_properties.Add(""",A46,""", LanguageConsts.",B46,");")</f>
+        <f t="shared" si="1"/>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/ASSISTANTTELEPHONE", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_AssistantTelephone);</v>
       </c>
     </row>
@@ -4010,7 +4010,7 @@
         <v>39</v>
       </c>
       <c r="E47" t="str">
-        <f>CONCATENATE("_properties.Add(""",A47,""", LanguageConsts.",B47,");")</f>
+        <f t="shared" si="1"/>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/ATTACHMENTNAMES", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_AttachmentNames);</v>
       </c>
     </row>
@@ -4028,7 +4028,7 @@
         <v>40</v>
       </c>
       <c r="E48" t="str">
-        <f>CONCATENATE("_properties.Add(""",A48,""", LanguageConsts.",B48,");")</f>
+        <f t="shared" si="1"/>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/BCCADDRESS", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_BccAddress);</v>
       </c>
     </row>
@@ -4046,7 +4046,7 @@
         <v>41</v>
       </c>
       <c r="E49" t="str">
-        <f>CONCATENATE("_properties.Add(""",A49,""", LanguageConsts.",B49,");")</f>
+        <f t="shared" si="1"/>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/BCCNAME", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_BccName);</v>
       </c>
     </row>
@@ -4064,7 +4064,7 @@
         <v>63</v>
       </c>
       <c r="E50" t="str">
-        <f>CONCATENATE("_properties.Add(""",A50,""", LanguageConsts.",B50,");")</f>
+        <f t="shared" si="1"/>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/BIRTHDAY", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_Birthday);</v>
       </c>
     </row>
@@ -4082,7 +4082,7 @@
         <v>64</v>
       </c>
       <c r="E51" t="str">
-        <f>CONCATENATE("_properties.Add(""",A51,""", LanguageConsts.",B51,");")</f>
+        <f t="shared" si="1"/>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/BUSINESSADDRESSCITY", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_BusinessAddressCity);</v>
       </c>
     </row>
@@ -4100,7 +4100,7 @@
         <v>64</v>
       </c>
       <c r="E52" t="str">
-        <f>CONCATENATE("_properties.Add(""",A52,""", LanguageConsts.",B52,");")</f>
+        <f t="shared" si="1"/>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/BUSINESSADDRESSCOUNTRY", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_BusinessAddressCountry);</v>
       </c>
     </row>
@@ -4118,7 +4118,7 @@
         <v>64</v>
       </c>
       <c r="E53" t="str">
-        <f>CONCATENATE("_properties.Add(""",A53,""", LanguageConsts.",B53,");")</f>
+        <f t="shared" si="1"/>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/BUSINESSADDRESSPOSTALCODE", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_BusinessAddressPostalCode);</v>
       </c>
     </row>
@@ -4136,7 +4136,7 @@
         <v>64</v>
       </c>
       <c r="E54" t="str">
-        <f>CONCATENATE("_properties.Add(""",A54,""", LanguageConsts.",B54,");")</f>
+        <f t="shared" si="1"/>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/BUSINESSADDRESSPOSTOFFICEBOX", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_BusinessAddressPostOfficeBox);</v>
       </c>
     </row>
@@ -4154,7 +4154,7 @@
         <v>64</v>
       </c>
       <c r="E55" t="str">
-        <f>CONCATENATE("_properties.Add(""",A55,""", LanguageConsts.",B55,");")</f>
+        <f t="shared" si="1"/>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/BUSINESSADDRESSSTATE", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_BusinessAddressState);</v>
       </c>
     </row>
@@ -4172,7 +4172,7 @@
         <v>64</v>
       </c>
       <c r="E56" t="str">
-        <f>CONCATENATE("_properties.Add(""",A56,""", LanguageConsts.",B56,");")</f>
+        <f t="shared" si="1"/>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/BUSINESSADDRESSSTREET", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_BusinessAddressStreet);</v>
       </c>
     </row>
@@ -4190,7 +4190,7 @@
         <v>77</v>
       </c>
       <c r="E57" t="str">
-        <f>CONCATENATE("_properties.Add(""",A57,""", LanguageConsts.",B57,");")</f>
+        <f t="shared" si="1"/>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/BUSINESSFAXNUMBER", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_BusinessFaxNumber);</v>
       </c>
     </row>
@@ -4208,7 +4208,7 @@
         <v>65</v>
       </c>
       <c r="E58" t="str">
-        <f>CONCATENATE("_properties.Add(""",A58,""", LanguageConsts.",B58,");")</f>
+        <f t="shared" si="1"/>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/CALLBACKTELEPHONE", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_CallbackTelephone);</v>
       </c>
     </row>
@@ -4226,7 +4226,7 @@
         <v>66</v>
       </c>
       <c r="E59" t="str">
-        <f>CONCATENATE("_properties.Add(""",A59,""", LanguageConsts.",B59,");")</f>
+        <f t="shared" si="1"/>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/CARTELEPHONE", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_CarTelephone);</v>
       </c>
     </row>
@@ -4244,7 +4244,7 @@
         <v>42</v>
       </c>
       <c r="E60" t="str">
-        <f>CONCATENATE("_properties.Add(""",A60,""", LanguageConsts.",B60,");")</f>
+        <f t="shared" si="1"/>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/CCADDRESS", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_CcAddress);</v>
       </c>
     </row>
@@ -4262,7 +4262,7 @@
         <v>43</v>
       </c>
       <c r="E61" t="str">
-        <f>CONCATENATE("_properties.Add(""",A61,""", LanguageConsts.",B61,");")</f>
+        <f t="shared" si="1"/>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/CCNAME", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_CcName);</v>
       </c>
     </row>
@@ -4280,7 +4280,7 @@
         <v>68</v>
       </c>
       <c r="E62" t="str">
-        <f>CONCATENATE("_properties.Add(""",A62,""", LanguageConsts.",B62,");")</f>
+        <f t="shared" si="1"/>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/CHILDREN", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_Children);</v>
       </c>
     </row>
@@ -4298,7 +4298,7 @@
         <v>66</v>
       </c>
       <c r="E63" t="str">
-        <f>CONCATENATE("_properties.Add(""",A63,""", LanguageConsts.",B63,");")</f>
+        <f t="shared" si="1"/>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/COMPANYMAINTELEPHONE", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_CompanyMainTelephone);</v>
       </c>
     </row>
@@ -4316,7 +4316,7 @@
         <v>32</v>
       </c>
       <c r="E64" t="str">
-        <f>CONCATENATE("_properties.Add(""",A64,""", LanguageConsts.",B64,");")</f>
+        <f t="shared" si="1"/>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/CONTAINERHASH", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_ContainerHash);</v>
       </c>
     </row>
@@ -4334,7 +4334,7 @@
         <v>44</v>
       </c>
       <c r="E65" t="str">
-        <f>CONCATENATE("_properties.Add(""",A65,""", LanguageConsts.",B65,");")</f>
+        <f t="shared" ref="E65:E96" si="2">CONCATENATE("_properties.Add(""",A65,""", LanguageConsts.",B65,");")</f>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/CONVERSATIONID", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_ConversationID);</v>
       </c>
     </row>
@@ -4352,7 +4352,7 @@
         <v>102</v>
       </c>
       <c r="E66" t="str">
-        <f>CONCATENATE("_properties.Add(""",A66,""", LanguageConsts.",B66,");")</f>
+        <f t="shared" si="2"/>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/DATETAKEN", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_DateTaken);</v>
       </c>
     </row>
@@ -4370,7 +4370,7 @@
         <v>241</v>
       </c>
       <c r="E67" t="str">
-        <f>CONCATENATE("_properties.Add(""",A67,""", LanguageConsts.",B67,");")</f>
+        <f t="shared" si="2"/>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/DISPLAYFOLDER", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_DisplayFolder);</v>
       </c>
     </row>
@@ -4388,7 +4388,7 @@
         <v>5</v>
       </c>
       <c r="E68" t="str">
-        <f>CONCATENATE("_properties.Add(""",A68,""", LanguageConsts.",B68,");")</f>
+        <f t="shared" si="2"/>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/DOCTITLEPREFIX", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_DocTitlePrefix);</v>
       </c>
     </row>
@@ -4406,7 +4406,7 @@
         <v>22</v>
       </c>
       <c r="E69" t="str">
-        <f>CONCATENATE("_properties.Add(""",A69,""", LanguageConsts.",B69,");")</f>
+        <f t="shared" si="2"/>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/DUEDATE", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_DueDate);</v>
       </c>
     </row>
@@ -4424,7 +4424,7 @@
         <v>55</v>
       </c>
       <c r="E70" t="str">
-        <f>CONCATENATE("_properties.Add(""",A70,""", LanguageConsts.",B70,");")</f>
+        <f t="shared" si="2"/>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/DURATION", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_Duration);</v>
       </c>
     </row>
@@ -4442,7 +4442,7 @@
         <v>69</v>
       </c>
       <c r="E71" t="str">
-        <f>CONCATENATE("_properties.Add(""",A71,""", LanguageConsts.",B71,");")</f>
+        <f t="shared" si="2"/>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/EMAILADDRESS", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_EmailAddress);</v>
       </c>
     </row>
@@ -4460,7 +4460,7 @@
         <v>70</v>
       </c>
       <c r="E72" t="str">
-        <f>CONCATENATE("_properties.Add(""",A72,""", LanguageConsts.",B72,");")</f>
+        <f t="shared" si="2"/>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/EMAILNAME", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_EmailName);</v>
       </c>
     </row>
@@ -4478,7 +4478,7 @@
         <v>244</v>
       </c>
       <c r="E73" t="str">
-        <f>CONCATENATE("_properties.Add(""",A73,""", LanguageConsts.",B73,");")</f>
+        <f t="shared" si="2"/>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/ENDDATE", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_EndDate);</v>
       </c>
     </row>
@@ -4496,7 +4496,7 @@
         <v>36</v>
       </c>
       <c r="E74" t="str">
-        <f>CONCATENATE("_properties.Add(""",A74,""", LanguageConsts.",B74,");")</f>
+        <f t="shared" si="2"/>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/FILEEXT", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_FileExt);</v>
       </c>
     </row>
@@ -4514,7 +4514,7 @@
         <v>242</v>
       </c>
       <c r="E75" t="str">
-        <f>CONCATENATE("_properties.Add(""",A75,""", LanguageConsts.",B75,");")</f>
+        <f t="shared" si="2"/>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/FILEEXTDESC", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_FileExtDesc);</v>
       </c>
     </row>
@@ -4532,7 +4532,7 @@
         <v>71</v>
       </c>
       <c r="E76" t="str">
-        <f>CONCATENATE("_properties.Add(""",A76,""", LanguageConsts.",B76,");")</f>
+        <f t="shared" si="2"/>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/FIRSTNAME", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_FirstName);</v>
       </c>
     </row>
@@ -4550,7 +4550,7 @@
         <v>26</v>
       </c>
       <c r="E77" t="str">
-        <f>CONCATENATE("_properties.Add(""",A77,""", LanguageConsts.",B77,");")</f>
+        <f t="shared" si="2"/>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/FLAGTEXT", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_FlagText);</v>
       </c>
     </row>
@@ -4568,7 +4568,7 @@
         <v>7</v>
       </c>
       <c r="E78" t="str">
-        <f>CONCATENATE("_properties.Add(""",A78,""", LanguageConsts.",B78,");")</f>
+        <f t="shared" si="2"/>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/FOLDERNAME", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_FolderName);</v>
       </c>
     </row>
@@ -4586,7 +4586,7 @@
         <v>45</v>
       </c>
       <c r="E79" t="str">
-        <f>CONCATENATE("_properties.Add(""",A79,""", LanguageConsts.",B79,");")</f>
+        <f t="shared" si="2"/>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/FROMADDRESS", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_FromAddress);</v>
       </c>
     </row>
@@ -4604,7 +4604,7 @@
         <v>46</v>
       </c>
       <c r="E80" t="str">
-        <f>CONCATENATE("_properties.Add(""",A80,""", LanguageConsts.",B80,");")</f>
+        <f t="shared" si="2"/>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/FROMNAME", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_FromName);</v>
       </c>
     </row>
@@ -4622,7 +4622,7 @@
         <v>72</v>
       </c>
       <c r="E81" t="str">
-        <f>CONCATENATE("_properties.Add(""",A81,""", LanguageConsts.",B81,");")</f>
+        <f t="shared" si="2"/>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/FULLNAME", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_FullName);</v>
       </c>
     </row>
@@ -4640,7 +4640,7 @@
         <v>47</v>
       </c>
       <c r="E82" t="str">
-        <f>CONCATENATE("_properties.Add(""",A82,""", LanguageConsts.",B82,");")</f>
+        <f t="shared" si="2"/>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/FWDRPLY", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_FwdRply);</v>
       </c>
     </row>
@@ -4658,7 +4658,7 @@
         <v>245</v>
       </c>
       <c r="E83" t="str">
-        <f>CONCATENATE("_properties.Add(""",A83,""", LanguageConsts.",B83,");")</f>
+        <f t="shared" si="2"/>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/GENDER", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_Gender);</v>
       </c>
     </row>
@@ -4676,7 +4676,7 @@
         <v>48</v>
       </c>
       <c r="E84" t="str">
-        <f>CONCATENATE("_properties.Add(""",A84,""", LanguageConsts.",B84,");")</f>
+        <f t="shared" si="2"/>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/HASATTACH", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_HasAttach);</v>
       </c>
     </row>
@@ -4694,7 +4694,7 @@
         <v>75</v>
       </c>
       <c r="E85" t="str">
-        <f>CONCATENATE("_properties.Add(""",A85,""", LanguageConsts.",B85,");")</f>
+        <f t="shared" si="2"/>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/HOBBY", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_Hobby);</v>
       </c>
     </row>
@@ -4712,7 +4712,7 @@
         <v>76</v>
       </c>
       <c r="E86" t="str">
-        <f>CONCATENATE("_properties.Add(""",A86,""", LanguageConsts.",B86,");")</f>
+        <f t="shared" si="2"/>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/HOMEADDRESSCITY", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_HomeAddressCity);</v>
       </c>
     </row>
@@ -4730,7 +4730,7 @@
         <v>76</v>
       </c>
       <c r="E87" t="str">
-        <f>CONCATENATE("_properties.Add(""",A87,""", LanguageConsts.",B87,");")</f>
+        <f t="shared" si="2"/>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/HOMEADDRESSCOUNTRY", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_HomeAddressCountry);</v>
       </c>
     </row>
@@ -4748,7 +4748,7 @@
         <v>76</v>
       </c>
       <c r="E88" t="str">
-        <f>CONCATENATE("_properties.Add(""",A88,""", LanguageConsts.",B88,");")</f>
+        <f t="shared" si="2"/>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/HOMEADDRESSPOSTALCODE", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_HomeAddressPostalCode);</v>
       </c>
     </row>
@@ -4766,7 +4766,7 @@
         <v>76</v>
       </c>
       <c r="E89" t="str">
-        <f>CONCATENATE("_properties.Add(""",A89,""", LanguageConsts.",B89,");")</f>
+        <f t="shared" si="2"/>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/HOMEADDRESSSTATE", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_HomeAddressState);</v>
       </c>
     </row>
@@ -4784,7 +4784,7 @@
         <v>76</v>
       </c>
       <c r="E90" t="str">
-        <f>CONCATENATE("_properties.Add(""",A90,""", LanguageConsts.",B90,");")</f>
+        <f t="shared" si="2"/>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/HOMEADDRESSSTREET", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_HomeAddressStreet);</v>
       </c>
     </row>
@@ -4802,7 +4802,7 @@
         <v>77</v>
       </c>
       <c r="E91" t="str">
-        <f>CONCATENATE("_properties.Add(""",A91,""", LanguageConsts.",B91,");")</f>
+        <f t="shared" si="2"/>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/HOMEFAXNUMBER", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_HomeFaxNumber);</v>
       </c>
     </row>
@@ -4820,7 +4820,7 @@
         <v>66</v>
       </c>
       <c r="E92" t="str">
-        <f>CONCATENATE("_properties.Add(""",A92,""", LanguageConsts.",B92,");")</f>
+        <f t="shared" si="2"/>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/HOMETELEPHONE", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_HomeTelephone);</v>
       </c>
     </row>
@@ -4838,7 +4838,7 @@
         <v>28</v>
       </c>
       <c r="E93" t="str">
-        <f>CONCATENATE("_properties.Add(""",A93,""", LanguageConsts.",B93,");")</f>
+        <f t="shared" si="2"/>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/IDENTITY", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_Identity);</v>
       </c>
     </row>
@@ -4856,7 +4856,7 @@
         <v>78</v>
       </c>
       <c r="E94" t="str">
-        <f>CONCATENATE("_properties.Add(""",A94,""", LanguageConsts.",B94,");")</f>
+        <f t="shared" si="2"/>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/IMADDRESS", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_IMAddress);</v>
       </c>
     </row>
@@ -4874,7 +4874,7 @@
         <v>31</v>
       </c>
       <c r="E95" t="str">
-        <f>CONCATENATE("_properties.Add(""",A95,""", LanguageConsts.",B95,");")</f>
+        <f t="shared" si="2"/>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/IMPORTANCE", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_Importance);</v>
       </c>
     </row>
@@ -4892,7 +4892,7 @@
         <v>8</v>
       </c>
       <c r="E96" t="str">
-        <f>CONCATENATE("_properties.Add(""",A96,""", LanguageConsts.",B96,");")</f>
+        <f t="shared" si="2"/>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/ISATTACHMENT", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_IsAttachment);</v>
       </c>
     </row>
@@ -4910,7 +4910,7 @@
         <v>9</v>
       </c>
       <c r="E97" t="str">
-        <f>CONCATENATE("_properties.Add(""",A97,""", LanguageConsts.",B97,");")</f>
+        <f t="shared" ref="E97:E128" si="3">CONCATENATE("_properties.Add(""",A97,""", LanguageConsts.",B97,");")</f>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/ISDELETED", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_IsDeleted);</v>
       </c>
     </row>
@@ -4928,7 +4928,7 @@
         <v>25</v>
       </c>
       <c r="E98" t="str">
-        <f>CONCATENATE("_properties.Add(""",A98,""", LanguageConsts.",B98,");")</f>
+        <f t="shared" si="3"/>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/ISFLAGGED", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_IsFlagged);</v>
       </c>
     </row>
@@ -4946,7 +4946,7 @@
         <v>24</v>
       </c>
       <c r="E99" t="str">
-        <f>CONCATENATE("_properties.Add(""",A99,""", LanguageConsts.",B99,");")</f>
+        <f t="shared" si="3"/>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/ISFLAGGEDCOMPLETED", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_IsFlaggedCompleted);</v>
       </c>
     </row>
@@ -4964,7 +4964,7 @@
         <v>23</v>
       </c>
       <c r="E100" t="str">
-        <f>CONCATENATE("_properties.Add(""",A100,""", LanguageConsts.",B100,");")</f>
+        <f t="shared" si="3"/>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/ISINCOMPLETE", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_IsIncomplete);</v>
       </c>
     </row>
@@ -4982,7 +4982,7 @@
         <v>29</v>
       </c>
       <c r="E101" t="str">
-        <f>CONCATENATE("_properties.Add(""",A101,""", LanguageConsts.",B101,");")</f>
+        <f t="shared" si="3"/>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/ISREAD", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_IsRead);</v>
       </c>
     </row>
@@ -5000,7 +5000,7 @@
         <v>53</v>
       </c>
       <c r="E102" t="str">
-        <f>CONCATENATE("_properties.Add(""",A102,""", LanguageConsts.",B102,");")</f>
+        <f t="shared" si="3"/>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/ISRECURRING", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_IsRecurring);</v>
       </c>
     </row>
@@ -5018,7 +5018,7 @@
         <v>79</v>
       </c>
       <c r="E103" t="str">
-        <f>CONCATENATE("_properties.Add(""",A103,""", LanguageConsts.",B103,");")</f>
+        <f t="shared" si="3"/>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/JOBTITLE", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_JobTitle);</v>
       </c>
     </row>
@@ -5036,7 +5036,7 @@
         <v>75</v>
       </c>
       <c r="E104" t="str">
-        <f>CONCATENATE("_properties.Add(""",A104,""", LanguageConsts.",B104,");")</f>
+        <f t="shared" si="3"/>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/LASTNAME", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_LastName);</v>
       </c>
     </row>
@@ -5054,7 +5054,7 @@
         <v>10</v>
       </c>
       <c r="E105" t="str">
-        <f>CONCATENATE("_properties.Add(""",A105,""", LanguageConsts.",B105,");")</f>
+        <f t="shared" si="3"/>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/LASTVIEWED", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_LastViewed);</v>
       </c>
     </row>
@@ -5072,7 +5072,7 @@
         <v>57</v>
       </c>
       <c r="E106" t="str">
-        <f>CONCATENATE("_properties.Add(""",A106,""", LanguageConsts.",B106,");")</f>
+        <f t="shared" si="3"/>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/LOCATION", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_Location);</v>
       </c>
     </row>
@@ -5090,7 +5090,7 @@
         <v>75</v>
       </c>
       <c r="E107" t="str">
-        <f>CONCATENATE("_properties.Add(""",A107,""", LanguageConsts.",B107,");")</f>
+        <f t="shared" si="3"/>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/MIDDLENAME", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_MiddleName);</v>
       </c>
     </row>
@@ -5108,7 +5108,7 @@
         <v>66</v>
       </c>
       <c r="E108" t="str">
-        <f>CONCATENATE("_properties.Add(""",A108,""", LanguageConsts.",B108,");")</f>
+        <f t="shared" si="3"/>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/MOBILETELEPHONE", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_MobileTelephone);</v>
       </c>
     </row>
@@ -5126,7 +5126,7 @@
         <v>75</v>
       </c>
       <c r="E109" t="str">
-        <f>CONCATENATE("_properties.Add(""",A109,""", LanguageConsts.",B109,");")</f>
+        <f t="shared" si="3"/>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/NICKNAME", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_NickName);</v>
       </c>
     </row>
@@ -5144,7 +5144,7 @@
         <v>75</v>
       </c>
       <c r="E110" t="str">
-        <f>CONCATENATE("_properties.Add(""",A110,""", LanguageConsts.",B110,");")</f>
+        <f t="shared" si="3"/>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/OFFICE", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_Office);</v>
       </c>
     </row>
@@ -5162,7 +5162,7 @@
         <v>66</v>
       </c>
       <c r="E111" t="str">
-        <f>CONCATENATE("_properties.Add(""",A111,""", LanguageConsts.",B111,");")</f>
+        <f t="shared" si="3"/>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/OFFICETELEPHONE", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_OfficeTelephone);</v>
       </c>
     </row>
@@ -5180,7 +5180,7 @@
         <v>66</v>
       </c>
       <c r="E112" t="str">
-        <f>CONCATENATE("_properties.Add(""",A112,""", LanguageConsts.",B112,");")</f>
+        <f t="shared" si="3"/>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/PAGERTELEPHONE", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_PagerTelephone);</v>
       </c>
     </row>
@@ -5198,7 +5198,7 @@
         <v>12</v>
       </c>
       <c r="E113" t="str">
-        <f>CONCATENATE("_properties.Add(""",A113,""", LanguageConsts.",B113,");")</f>
+        <f t="shared" si="3"/>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/PEOPLE", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_People);</v>
       </c>
     </row>
@@ -5216,7 +5216,7 @@
         <v>13</v>
       </c>
       <c r="E114" t="str">
-        <f>CONCATENATE("_properties.Add(""",A114,""", LanguageConsts.",B114,");")</f>
+        <f t="shared" si="3"/>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/PERCEIVEDTYPE", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_PerceivedType);</v>
       </c>
     </row>
@@ -5234,7 +5234,7 @@
         <v>14</v>
       </c>
       <c r="E115" t="str">
-        <f>CONCATENATE("_properties.Add(""",A115,""", LanguageConsts.",B115,");")</f>
+        <f t="shared" si="3"/>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/PERCEIVEDTYPENAME", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_PerceivedTypeName);</v>
       </c>
     </row>
@@ -5252,7 +5252,7 @@
         <v>81</v>
       </c>
       <c r="E116" t="str">
-        <f>CONCATENATE("_properties.Add(""",A116,""", LanguageConsts.",B116,");")</f>
+        <f t="shared" si="3"/>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/PERSONALTITLE", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_PersonalTitle);</v>
       </c>
     </row>
@@ -5270,7 +5270,7 @@
         <v>15</v>
       </c>
       <c r="E117" t="str">
-        <f>CONCATENATE("_properties.Add(""",A117,""", LanguageConsts.",B117,");")</f>
+        <f t="shared" si="3"/>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/PRIMARYDATE", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_PrimaryDate);</v>
       </c>
     </row>
@@ -5288,7 +5288,7 @@
         <v>66</v>
       </c>
       <c r="E118" t="str">
-        <f>CONCATENATE("_properties.Add(""",A118,""", LanguageConsts.",B118,");")</f>
+        <f t="shared" si="3"/>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/PRIMARYTELEPHONE", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_PrimaryTelephone);</v>
       </c>
     </row>
@@ -5306,7 +5306,7 @@
         <v>75</v>
       </c>
       <c r="E119" t="str">
-        <f>CONCATENATE("_properties.Add(""",A119,""", LanguageConsts.",B119,");")</f>
+        <f t="shared" si="3"/>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/PROFESSION", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_Profession);</v>
       </c>
     </row>
@@ -5324,7 +5324,7 @@
         <v>49</v>
       </c>
       <c r="E120" t="str">
-        <f>CONCATENATE("_properties.Add(""",A120,""", LanguageConsts.",B120,");")</f>
+        <f t="shared" si="3"/>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/RECEIVEDDATE", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_ReceivedDate);</v>
       </c>
     </row>
@@ -5342,7 +5342,7 @@
         <v>75</v>
       </c>
       <c r="E121" t="str">
-        <f>CONCATENATE("_properties.Add(""",A121,""", LanguageConsts.",B121,");")</f>
+        <f t="shared" si="3"/>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/SPOUSE", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_Spouse);</v>
       </c>
     </row>
@@ -5360,7 +5360,7 @@
         <v>246</v>
       </c>
       <c r="E122" t="str">
-        <f>CONCATENATE("_properties.Add(""",A122,""", LanguageConsts.",B122,");")</f>
+        <f t="shared" si="3"/>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/STARTDATE", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_StartDate);</v>
       </c>
     </row>
@@ -5378,7 +5378,7 @@
         <v>35</v>
       </c>
       <c r="E123" t="str">
-        <f>CONCATENATE("_properties.Add(""",A123,""", LanguageConsts.",B123,");")</f>
+        <f t="shared" si="3"/>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/STORE", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_Store);</v>
       </c>
     </row>
@@ -5396,7 +5396,7 @@
         <v>75</v>
       </c>
       <c r="E124" t="str">
-        <f>CONCATENATE("_properties.Add(""",A124,""", LanguageConsts.",B124,");")</f>
+        <f t="shared" si="3"/>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/SUFFIX", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_Suffix);</v>
       </c>
     </row>
@@ -5414,7 +5414,7 @@
         <v>52</v>
       </c>
       <c r="E125" t="str">
-        <f>CONCATENATE("_properties.Add(""",A125,""", LanguageConsts.",B125,");")</f>
+        <f t="shared" si="3"/>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/TASKSTATUS", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_TaskStatus);</v>
       </c>
     </row>
@@ -5432,7 +5432,7 @@
         <v>85</v>
       </c>
       <c r="E126" t="str">
-        <f>CONCATENATE("_properties.Add(""",A126,""", LanguageConsts.",B126,");")</f>
+        <f t="shared" si="3"/>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/TELEXNUMBER", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_TelexNumber);</v>
       </c>
     </row>
@@ -5450,7 +5450,7 @@
         <v>50</v>
       </c>
       <c r="E127" t="str">
-        <f>CONCATENATE("_properties.Add(""",A127,""", LanguageConsts.",B127,");")</f>
+        <f t="shared" si="3"/>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/TOADDRESS", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_ToAddress);</v>
       </c>
     </row>
@@ -5468,7 +5468,7 @@
         <v>51</v>
       </c>
       <c r="E128" t="str">
-        <f>CONCATENATE("_properties.Add(""",A128,""", LanguageConsts.",B128,");")</f>
+        <f t="shared" si="3"/>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/TONAME", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_ToName);</v>
       </c>
     </row>
@@ -5486,7 +5486,7 @@
         <v>247</v>
       </c>
       <c r="E129" t="str">
-        <f>CONCATENATE("_properties.Add(""",A129,""", LanguageConsts.",B129,");")</f>
+        <f t="shared" ref="E129:E136" si="4">CONCATENATE("_properties.Add(""",A129,""", LanguageConsts.",B129,");")</f>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/TTYTDDTELEPHONE", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_TTYTDDTelephone);</v>
       </c>
     </row>
@@ -5504,7 +5504,7 @@
         <v>87</v>
       </c>
       <c r="E130" t="str">
-        <f>CONCATENATE("_properties.Add(""",A130,""", LanguageConsts.",B130,");")</f>
+        <f t="shared" si="4"/>
         <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/WEBPAGE", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_WebPage);</v>
       </c>
     </row>
@@ -5522,7 +5522,7 @@
         <v>6</v>
       </c>
       <c r="E131" t="str">
-        <f>CONCATENATE("_properties.Add(""",A131,""", LanguageConsts.",B131,");")</f>
+        <f t="shared" si="4"/>
         <v>_properties.Add("F29F85E0-4FF9-1068-AB91-08002B27B3D9/2", LanguageConsts._F29F85E0_4FF9_1068_AB91_08002B27B3D9_2);</v>
       </c>
     </row>
@@ -5540,7 +5540,7 @@
         <v>18</v>
       </c>
       <c r="E132" t="str">
-        <f>CONCATENATE("_properties.Add(""",A132,""", LanguageConsts.",B132,");")</f>
+        <f t="shared" si="4"/>
         <v>_properties.Add("F29F85E0-4FF9-1068-AB91-08002B27B3D9/3", LanguageConsts._F29F85E0_4FF9_1068_AB91_08002B27B3D9_3);</v>
       </c>
     </row>
@@ -5558,7 +5558,7 @@
         <v>2</v>
       </c>
       <c r="E133" t="str">
-        <f>CONCATENATE("_properties.Add(""",A133,""", LanguageConsts.",B133,");")</f>
+        <f t="shared" si="4"/>
         <v>_properties.Add("F29F85E0-4FF9-1068-AB91-08002B27B3D9/4", LanguageConsts._F29F85E0_4FF9_1068_AB91_08002B27B3D9_4);</v>
       </c>
     </row>
@@ -5576,7 +5576,7 @@
         <v>4</v>
       </c>
       <c r="E134" t="str">
-        <f>CONCATENATE("_properties.Add(""",A134,""", LanguageConsts.",B134,");")</f>
+        <f t="shared" si="4"/>
         <v>_properties.Add("F29F85E0-4FF9-1068-AB91-08002B27B3D9/5", LanguageConsts._F29F85E0_4FF9_1068_AB91_08002B27B3D9_5);</v>
       </c>
     </row>
@@ -5594,7 +5594,7 @@
         <v>0</v>
       </c>
       <c r="E135" t="str">
-        <f>CONCATENATE("_properties.Add(""",A135,""", LanguageConsts.",B135,");")</f>
+        <f t="shared" si="4"/>
         <v>_properties.Add("F29F85E0-4FF9-1068-AB91-08002B27B3D9/6", LanguageConsts._F29F85E0_4FF9_1068_AB91_08002B27B3D9_6);</v>
       </c>
     </row>
@@ -5612,7 +5612,7 @@
         <v>239</v>
       </c>
       <c r="E136" t="str">
-        <f>CONCATENATE("_properties.Add(""",A136,""", LanguageConsts.",B136,");")</f>
+        <f t="shared" si="4"/>
         <v>_properties.Add("F29F85E0-4FF9-1068-AB91-08002B27B3D9/8", LanguageConsts._F29F85E0_4FF9_1068_AB91_08002B27B3D9_8);</v>
       </c>
     </row>
@@ -5624,13 +5624,13 @@
         <v>551</v>
       </c>
       <c r="C137" t="s">
-        <v>886</v>
+        <v>776</v>
       </c>
       <c r="D137" t="s">
-        <v>885</v>
+        <v>775</v>
       </c>
       <c r="E137" t="str">
-        <f t="shared" ref="E137:E200" si="0">CONCATENATE("_properties.Add(""",A137,""", LanguageConsts.",B137,");")</f>
+        <f t="shared" ref="E137:E200" si="5">CONCATENATE("_properties.Add(""",A137,""", LanguageConsts.",B137,");")</f>
         <v>_properties.Add("F29F85E0-4FF9-1068-AB91-08002B27B3D9/10", LanguageConsts._F29F85E0_4FF9_1068_AB91_08002B27B3D9_10);</v>
       </c>
     </row>
@@ -5648,7 +5648,7 @@
         <v>89</v>
       </c>
       <c r="E138" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>_properties.Add("F29F85E0-4FF9-1068-AB91-08002B27B3D9/11", LanguageConsts._F29F85E0_4FF9_1068_AB91_08002B27B3D9_11);</v>
       </c>
     </row>
@@ -5660,13 +5660,13 @@
         <v>552</v>
       </c>
       <c r="C139" t="s">
-        <v>888</v>
+        <v>778</v>
       </c>
       <c r="D139" t="s">
-        <v>887</v>
+        <v>777</v>
       </c>
       <c r="E139" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>_properties.Add("F29F85E0-4FF9-1068-AB91-08002B27B3D9/12", LanguageConsts._F29F85E0_4FF9_1068_AB91_08002B27B3D9_12);</v>
       </c>
     </row>
@@ -5678,13 +5678,13 @@
         <v>553</v>
       </c>
       <c r="C140" t="s">
-        <v>883</v>
+        <v>773</v>
       </c>
       <c r="D140" t="s">
-        <v>884</v>
+        <v>774</v>
       </c>
       <c r="E140" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>_properties.Add("F29F85E0-4FF9-1068-AB91-08002B27B3D9/13", LanguageConsts._F29F85E0_4FF9_1068_AB91_08002B27B3D9_13);</v>
       </c>
     </row>
@@ -5696,13 +5696,13 @@
         <v>554</v>
       </c>
       <c r="C141" t="s">
-        <v>890</v>
+        <v>780</v>
       </c>
       <c r="D141" t="s">
-        <v>889</v>
+        <v>779</v>
       </c>
       <c r="E141" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>_properties.Add("F29F85E0-4FF9-1068-AB91-08002B27B3D9/14", LanguageConsts._F29F85E0_4FF9_1068_AB91_08002B27B3D9_14);</v>
       </c>
     </row>
@@ -5714,13 +5714,13 @@
         <v>555</v>
       </c>
       <c r="C142" t="s">
-        <v>894</v>
+        <v>784</v>
       </c>
       <c r="D142" t="s">
-        <v>893</v>
+        <v>783</v>
       </c>
       <c r="E142" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>_properties.Add("F29F85E0-4FF9-1068-AB91-08002B27B3D9/15", LanguageConsts._F29F85E0_4FF9_1068_AB91_08002B27B3D9_15);</v>
       </c>
     </row>
@@ -5732,13 +5732,13 @@
         <v>556</v>
       </c>
       <c r="C143" t="s">
-        <v>892</v>
+        <v>782</v>
       </c>
       <c r="D143" t="s">
-        <v>891</v>
+        <v>781</v>
       </c>
       <c r="E143" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>_properties.Add("F29F85E0-4FF9-1068-AB91-08002B27B3D9/16", LanguageConsts._F29F85E0_4FF9_1068_AB91_08002B27B3D9_16);</v>
       </c>
     </row>
@@ -5753,7 +5753,7 @@
         <v>541</v>
       </c>
       <c r="E144" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>_properties.Add("F29F85E0-4FF9-1068-AB91-08002B27B3D9/18", LanguageConsts._F29F85E0_4FF9_1068_AB91_08002B27B3D9_18);</v>
       </c>
     </row>
@@ -5768,10 +5768,10 @@
         <v>542</v>
       </c>
       <c r="D145" t="s">
-        <v>895</v>
+        <v>785</v>
       </c>
       <c r="E145" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>_properties.Add("F29F85E0-4FF9-1068-AB91-08002B27B3D9/19", LanguageConsts._F29F85E0_4FF9_1068_AB91_08002B27B3D9_19);</v>
       </c>
     </row>
@@ -5780,14 +5780,14 @@
         <v>667</v>
       </c>
       <c r="B146" t="s">
-        <v>775</v>
+        <v>805</v>
       </c>
       <c r="C146" t="s">
         <v>559</v>
       </c>
       <c r="E146" t="str">
-        <f t="shared" si="0"/>
-        <v>_properties.Add("F7DB74B4-4287-4103-AFBA-F1B13DCD75CF/100", LanguageConsts._F7DB74B4-4287-4103-AFBA-F1B13DCD75CF_100);</v>
+        <f t="shared" si="5"/>
+        <v>_properties.Add("F7DB74B4-4287-4103-AFBA-F1B13DCD75CF/100", LanguageConsts._F7DB74B4_4287_4103_AFBA_F1B13DCD75CF_100);</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.45">
@@ -5795,14 +5795,14 @@
         <v>668</v>
       </c>
       <c r="B147" t="s">
-        <v>776</v>
+        <v>806</v>
       </c>
       <c r="C147" t="s">
         <v>560</v>
       </c>
       <c r="E147" t="str">
-        <f t="shared" si="0"/>
-        <v>_properties.Add("28636AA6-953D-11D2-B5D6-00C04FD918D0/11", LanguageConsts._28636AA6-953D-11D2-B5D6-00C04FD918D0_11);</v>
+        <f t="shared" si="5"/>
+        <v>_properties.Add("28636AA6-953D-11D2-B5D6-00C04FD918D0/11", LanguageConsts._28636AA6_953D_11D2_B5D6_00C04FD918D0_11);</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.45">
@@ -5810,14 +5810,14 @@
         <v>669</v>
       </c>
       <c r="B148" t="s">
-        <v>777</v>
+        <v>807</v>
       </c>
       <c r="C148" t="s">
         <v>561</v>
       </c>
       <c r="E148" t="str">
-        <f t="shared" si="0"/>
-        <v>_properties.Add("D5CDD502-2E9C-101B-9397-08002B2CF9AE/26", LanguageConsts._D5CDD502-2E9C-101B-9397-08002B2CF9AE_26);</v>
+        <f t="shared" si="5"/>
+        <v>_properties.Add("D5CDD502-2E9C-101B-9397-08002B2CF9AE/26", LanguageConsts._D5CDD502_2E9C_101B_9397_08002B2CF9AE_26);</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.45">
@@ -5825,14 +5825,14 @@
         <v>670</v>
       </c>
       <c r="B149" t="s">
-        <v>778</v>
+        <v>808</v>
       </c>
       <c r="C149" t="s">
         <v>562</v>
       </c>
       <c r="E149" t="str">
-        <f t="shared" si="0"/>
-        <v>_properties.Add("1E3EE840-BC2B-476C-8237-2ACD1A839B22/3", LanguageConsts._1E3EE840-BC2B-476C-8237-2ACD1A839B22_3);</v>
+        <f t="shared" si="5"/>
+        <v>_properties.Add("1E3EE840-BC2B-476C-8237-2ACD1A839B22/3", LanguageConsts._1E3EE840_BC2B_476C_8237_2ACD1A839B22_3);</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.45">
@@ -5840,14 +5840,14 @@
         <v>671</v>
       </c>
       <c r="B150" t="s">
-        <v>779</v>
+        <v>809</v>
       </c>
       <c r="C150" t="s">
         <v>563</v>
       </c>
       <c r="E150" t="str">
-        <f t="shared" si="0"/>
-        <v>_properties.Add("E4F10A3C-49E6-405D-8288-A23BD4EEAA6C/100", LanguageConsts._E4F10A3C-49E6-405D-8288-A23BD4EEAA6C_100);</v>
+        <f t="shared" si="5"/>
+        <v>_properties.Add("E4F10A3C-49E6-405D-8288-A23BD4EEAA6C/100", LanguageConsts._E4F10A3C_49E6_405D_8288_A23BD4EEAA6C_100);</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.45">
@@ -5855,14 +5855,14 @@
         <v>672</v>
       </c>
       <c r="B151" t="s">
-        <v>780</v>
+        <v>810</v>
       </c>
       <c r="C151" t="s">
         <v>564</v>
       </c>
       <c r="E151" t="str">
-        <f t="shared" si="0"/>
-        <v>_properties.Add("28636AA6-953D-11D2-B5D6-00C04FD918D0/12", LanguageConsts._28636AA6-953D-11D2-B5D6-00C04FD918D0_12);</v>
+        <f t="shared" si="5"/>
+        <v>_properties.Add("28636AA6-953D-11D2-B5D6-00C04FD918D0/12", LanguageConsts._28636AA6_953D_11D2_B5D6_00C04FD918D0_12);</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.45">
@@ -5870,14 +5870,14 @@
         <v>673</v>
       </c>
       <c r="B152" t="s">
-        <v>781</v>
+        <v>811</v>
       </c>
       <c r="C152" t="s">
         <v>565</v>
       </c>
       <c r="E152" t="str">
-        <f t="shared" si="0"/>
-        <v>_properties.Add("EF884C5B-2BFE-41BB-AAE5-76EEDF4F9902/100", LanguageConsts._EF884C5B-2BFE-41BB-AAE5-76EEDF4F9902_100);</v>
+        <f t="shared" si="5"/>
+        <v>_properties.Add("EF884C5B-2BFE-41BB-AAE5-76EEDF4F9902/100", LanguageConsts._EF884C5B_2BFE_41BB_AAE5_76EEDF4F9902_100);</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.45">
@@ -5885,14 +5885,14 @@
         <v>674</v>
       </c>
       <c r="B153" t="s">
-        <v>782</v>
+        <v>812</v>
       </c>
       <c r="C153" t="s">
         <v>566</v>
       </c>
       <c r="E153" t="str">
-        <f t="shared" si="0"/>
-        <v>_properties.Add("EF884C5B-2BFE-41BB-AAE5-76EEDF4F9902/200", LanguageConsts._EF884C5B-2BFE-41BB-AAE5-76EEDF4F9902_200);</v>
+        <f t="shared" si="5"/>
+        <v>_properties.Add("EF884C5B-2BFE-41BB-AAE5-76EEDF4F9902/200", LanguageConsts._EF884C5B_2BFE_41BB_AAE5_76EEDF4F9902_200);</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.45">
@@ -5900,14 +5900,14 @@
         <v>675</v>
       </c>
       <c r="B154" t="s">
-        <v>783</v>
+        <v>813</v>
       </c>
       <c r="C154" t="s">
         <v>567</v>
       </c>
       <c r="E154" t="str">
-        <f t="shared" si="0"/>
-        <v>_properties.Add("EF884C5B-2BFE-41BB-AAE5-76EEDF4F9902/300", LanguageConsts._EF884C5B-2BFE-41BB-AAE5-76EEDF4F9902_300);</v>
+        <f t="shared" si="5"/>
+        <v>_properties.Add("EF884C5B-2BFE-41BB-AAE5-76EEDF4F9902/300", LanguageConsts._EF884C5B_2BFE_41BB_AAE5_76EEDF4F9902_300);</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.45">
@@ -5915,14 +5915,14 @@
         <v>676</v>
       </c>
       <c r="B155" t="s">
-        <v>784</v>
+        <v>814</v>
       </c>
       <c r="C155" t="s">
         <v>568</v>
       </c>
       <c r="E155" t="str">
-        <f t="shared" si="0"/>
-        <v>_properties.Add("B725F130-47EF-101A-A5F1-02608C9EEBAC/16", LanguageConsts._B725F130-47EF-101A-A5F1-02608C9EEBAC_16);</v>
+        <f t="shared" si="5"/>
+        <v>_properties.Add("B725F130-47EF-101A-A5F1-02608C9EEBAC/16", LanguageConsts._B725F130_47EF_101A_A5F1_02608C9EEBAC_16);</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.45">
@@ -5930,14 +5930,14 @@
         <v>677</v>
       </c>
       <c r="B156" t="s">
-        <v>785</v>
+        <v>815</v>
       </c>
       <c r="C156" t="s">
         <v>569</v>
       </c>
       <c r="E156" t="str">
-        <f t="shared" si="0"/>
-        <v>_properties.Add("B725F130-47EF-101A-A5F1-02608C9EEBAC/13", LanguageConsts._B725F130-47EF-101A-A5F1-02608C9EEBAC_13);</v>
+        <f t="shared" si="5"/>
+        <v>_properties.Add("B725F130-47EF-101A-A5F1-02608C9EEBAC/13", LanguageConsts._B725F130_47EF_101A_A5F1_02608C9EEBAC_13);</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.45">
@@ -5945,14 +5945,14 @@
         <v>678</v>
       </c>
       <c r="B157" t="s">
-        <v>786</v>
+        <v>816</v>
       </c>
       <c r="C157" t="s">
         <v>570</v>
       </c>
       <c r="E157" t="str">
-        <f t="shared" si="0"/>
-        <v>_properties.Add("9B174B34-40FF-11D2-A27E-00C04FC30871/4", LanguageConsts._9B174B34-40FF-11D2-A27E-00C04FC30871_4);</v>
+        <f t="shared" si="5"/>
+        <v>_properties.Add("9B174B34-40FF-11D2-A27E-00C04FC30871/4", LanguageConsts._9B174B34_40FF_11D2_A27E_00C04FC30871_4);</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.45">
@@ -5960,14 +5960,14 @@
         <v>679</v>
       </c>
       <c r="B158" t="s">
-        <v>787</v>
+        <v>817</v>
       </c>
       <c r="C158" t="s">
         <v>571</v>
       </c>
       <c r="E158" t="str">
-        <f t="shared" si="0"/>
-        <v>_properties.Add("28636AA6-953D-11D2-B5D6-00C04FD918D0/5", LanguageConsts._28636AA6-953D-11D2-B5D6-00C04FD918D0_5);</v>
+        <f t="shared" si="5"/>
+        <v>_properties.Add("28636AA6-953D-11D2-B5D6-00C04FD918D0/5", LanguageConsts._28636AA6_953D_11D2_B5D6_00C04FD918D0_5);</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.45">
@@ -5975,14 +5975,14 @@
         <v>680</v>
       </c>
       <c r="B159" t="s">
-        <v>788</v>
+        <v>818</v>
       </c>
       <c r="C159" t="s">
         <v>572</v>
       </c>
       <c r="E159" t="str">
-        <f t="shared" si="0"/>
-        <v>_properties.Add("90E5E14E-648B-4826-B2AA-ACAF790E3513/10", LanguageConsts._90E5E14E-648B-4826-B2AA-ACAF790E3513_10);</v>
+        <f t="shared" si="5"/>
+        <v>_properties.Add("90E5E14E-648B-4826-B2AA-ACAF790E3513/10", LanguageConsts._90E5E14E_648B_4826_B2AA_ACAF790E3513_10);</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.45">
@@ -5990,14 +5990,14 @@
         <v>681</v>
       </c>
       <c r="B160" t="s">
-        <v>789</v>
+        <v>819</v>
       </c>
       <c r="C160" t="s">
         <v>573</v>
       </c>
       <c r="E160" t="str">
-        <f t="shared" si="0"/>
-        <v>_properties.Add("A94688B6-7D9F-4570-A648-E3DFC0AB2B3F/100", LanguageConsts._A94688B6-7D9F-4570-A648-E3DFC0AB2B3F_100);</v>
+        <f t="shared" si="5"/>
+        <v>_properties.Add("A94688B6-7D9F-4570-A648-E3DFC0AB2B3F/100", LanguageConsts._A94688B6_7D9F_4570_A648_E3DFC0AB2B3F_100);</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.45">
@@ -6005,14 +6005,14 @@
         <v>682</v>
       </c>
       <c r="B161" t="s">
-        <v>790</v>
+        <v>820</v>
       </c>
       <c r="C161" t="s">
         <v>574</v>
       </c>
       <c r="E161" t="str">
-        <f t="shared" si="0"/>
-        <v>_properties.Add("6D24888F-4718-4BDA-AFED-EA0FB4386CD8/100", LanguageConsts._6D24888F-4718-4BDA-AFED-EA0FB4386CD8_100);</v>
+        <f t="shared" si="5"/>
+        <v>_properties.Add("6D24888F-4718-4BDA-AFED-EA0FB4386CD8/100", LanguageConsts._6D24888F_4718_4BDA_AFED_EA0FB4386CD8_100);</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.45">
@@ -6020,14 +6020,14 @@
         <v>683</v>
       </c>
       <c r="B162" t="s">
-        <v>791</v>
+        <v>821</v>
       </c>
       <c r="C162" t="s">
         <v>575</v>
       </c>
       <c r="E162" t="str">
-        <f t="shared" si="0"/>
-        <v>_properties.Add("B9B4B3FC-2B51-4A42-B5D8-324146AFCF25/2", LanguageConsts._B9B4B3FC-2B51-4A42-B5D8-324146AFCF25_2);</v>
+        <f t="shared" si="5"/>
+        <v>_properties.Add("B9B4B3FC-2B51-4A42-B5D8-324146AFCF25/2", LanguageConsts._B9B4B3FC_2B51_4A42_B5D8_324146AFCF25_2);</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.45">
@@ -6035,1579 +6035,1579 @@
         <v>684</v>
       </c>
       <c r="B163" t="s">
-        <v>792</v>
+        <v>822</v>
       </c>
       <c r="C163" t="s">
         <v>576</v>
       </c>
       <c r="E163" t="str">
-        <f t="shared" si="0"/>
-        <v>_properties.Add("E3E0584C-B788-4A5A-BB20-7F5A44C9ACDD/6", LanguageConsts._E3E0584C-B788-4A5A-BB20-7F5A44C9ACDD_6);</v>
+        <f t="shared" si="5"/>
+        <v>_properties.Add("E3E0584C-B788-4A5A-BB20-7F5A44C9ACDD/6", LanguageConsts._E3E0584C_B788_4A5A_BB20_7F5A44C9ACDD_6);</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A164" t="s">
-        <v>685</v>
+        <v>930</v>
       </c>
       <c r="B164" t="s">
-        <v>793</v>
+        <v>931</v>
       </c>
       <c r="C164" t="s">
         <v>577</v>
       </c>
       <c r="E164" t="str">
-        <f t="shared" si="0"/>
-        <v>_properties.Add("49691C90-7E17-101A-A91C-08002B2ECDA9}/3", LanguageConsts._49691C90-7E17-101A-A91C-08002B2ECDA9}_3);</v>
+        <f t="shared" si="5"/>
+        <v>_properties.Add("49691C90-7E17-101A-A91C-08002B2ECDA9/3", LanguageConsts._49691C90_7E17_101A_A91C_08002B2ECDA9_3);</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A165" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="B165" t="s">
-        <v>794</v>
+        <v>823</v>
       </c>
       <c r="C165" t="s">
         <v>578</v>
       </c>
       <c r="E165" t="str">
-        <f t="shared" si="0"/>
-        <v>_properties.Add("64440490-4C8B-11D1-8B70-080036B11A03/7", LanguageConsts._64440490-4C8B-11D1-8B70-080036B11A03_7);</v>
+        <f t="shared" si="5"/>
+        <v>_properties.Add("64440490-4C8B-11D1-8B70-080036B11A03/7", LanguageConsts._64440490_4C8B_11D1_8B70_080036B11A03_7);</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A166" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="B166" t="s">
-        <v>795</v>
+        <v>824</v>
       </c>
       <c r="C166" t="s">
         <v>579</v>
       </c>
       <c r="E166" t="str">
-        <f t="shared" si="0"/>
-        <v>_properties.Add("64440490-4C8B-11D1-8B70-080036B11A03/5", LanguageConsts._64440490-4C8B-11D1-8B70-080036B11A03_5);</v>
+        <f t="shared" si="5"/>
+        <v>_properties.Add("64440490-4C8B-11D1-8B70-080036B11A03/5", LanguageConsts._64440490_4C8B_11D1_8B70_080036B11A03_5);</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A167" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="B167" t="s">
-        <v>796</v>
+        <v>825</v>
       </c>
       <c r="C167" t="s">
         <v>580</v>
       </c>
       <c r="E167" t="str">
-        <f t="shared" si="0"/>
-        <v>_properties.Add("64440490-4C8B-11D1-8B70-080036B11A03/8", LanguageConsts._64440490-4C8B-11D1-8B70-080036B11A03_8);</v>
+        <f t="shared" si="5"/>
+        <v>_properties.Add("64440490-4C8B-11D1-8B70-080036B11A03/8", LanguageConsts._64440490_4C8B_11D1_8B70_080036B11A03_8);</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A168" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="B168" t="s">
-        <v>797</v>
+        <v>826</v>
       </c>
       <c r="C168" t="s">
         <v>581</v>
       </c>
       <c r="E168" t="str">
-        <f t="shared" si="0"/>
-        <v>_properties.Add("56A3372E-CE9C-11D2-9F0E-006097C686F6/13", LanguageConsts._56A3372E-CE9C-11D2-9F0E-006097C686F6_13);</v>
+        <f t="shared" si="5"/>
+        <v>_properties.Add("56A3372E-CE9C-11D2-9F0E-006097C686F6/13", LanguageConsts._56A3372E_CE9C_11D2_9F0E_006097C686F6_13);</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A169" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="B169" t="s">
-        <v>798</v>
+        <v>827</v>
       </c>
       <c r="C169" t="s">
         <v>582</v>
       </c>
       <c r="E169" t="str">
-        <f t="shared" si="0"/>
-        <v>_properties.Add("56A3372E-CE9C-11D2-9F0E-006097C686F6/100", LanguageConsts._56A3372E-CE9C-11D2-9F0E-006097C686F6_100);</v>
+        <f t="shared" si="5"/>
+        <v>_properties.Add("56A3372E-CE9C-11D2-9F0E-006097C686F6/100", LanguageConsts._56A3372E_CE9C_11D2_9F0E_006097C686F6_100);</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A170" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="B170" t="s">
-        <v>799</v>
+        <v>828</v>
       </c>
       <c r="C170" t="s">
         <v>583</v>
       </c>
       <c r="E170" t="str">
-        <f t="shared" si="0"/>
-        <v>_properties.Add("FD122953-FA93-4EF7-92C3-04C946B2F7C8/100", LanguageConsts._FD122953-FA93-4EF7-92C3-04C946B2F7C8_100);</v>
+        <f t="shared" si="5"/>
+        <v>_properties.Add("FD122953-FA93-4EF7-92C3-04C946B2F7C8/100", LanguageConsts._FD122953_FA93_4EF7_92C3_04C946B2F7C8_100);</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A171" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="B171" t="s">
-        <v>800</v>
+        <v>829</v>
       </c>
       <c r="C171" t="s">
         <v>584</v>
       </c>
       <c r="E171" t="str">
-        <f t="shared" si="0"/>
-        <v>_properties.Add("56A3372E-CE9C-11D2-9F0E-006097C686F6/35", LanguageConsts._56A3372E-CE9C-11D2-9F0E-006097C686F6_35);</v>
+        <f t="shared" si="5"/>
+        <v>_properties.Add("56A3372E-CE9C-11D2-9F0E-006097C686F6/35", LanguageConsts._56A3372E_CE9C_11D2_9F0E_006097C686F6_35);</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A172" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="B172" t="s">
-        <v>801</v>
+        <v>830</v>
       </c>
       <c r="C172" t="s">
         <v>585</v>
       </c>
       <c r="E172" t="str">
-        <f t="shared" si="0"/>
-        <v>_properties.Add("64440492-4C8B-11D1-8B70-080036B11A03/19", LanguageConsts._64440492-4C8B-11D1-8B70-080036B11A03_19);</v>
+        <f t="shared" si="5"/>
+        <v>_properties.Add("64440492-4C8B-11D1-8B70-080036B11A03/19", LanguageConsts._64440492_4C8B_11D1_8B70_080036B11A03_19);</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A173" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="B173" t="s">
-        <v>802</v>
+        <v>831</v>
       </c>
       <c r="C173" t="s">
         <v>586</v>
       </c>
       <c r="E173" t="str">
-        <f t="shared" si="0"/>
-        <v>_properties.Add("56A3372E-CE9C-11D2-9F0E-006097C686F6/36", LanguageConsts._56A3372E-CE9C-11D2-9F0E-006097C686F6_36);</v>
+        <f t="shared" si="5"/>
+        <v>_properties.Add("56A3372E-CE9C-11D2-9F0E-006097C686F6/36", LanguageConsts._56A3372E_CE9C_11D2_9F0E_006097C686F6_36);</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A174" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="B174" t="s">
-        <v>803</v>
+        <v>832</v>
       </c>
       <c r="C174" t="s">
         <v>587</v>
       </c>
       <c r="E174" t="str">
-        <f t="shared" si="0"/>
-        <v>_properties.Add("56A3372E-CE9C-11D2-9F0E-006097C686F6/12", LanguageConsts._56A3372E-CE9C-11D2-9F0E-006097C686F6_12);</v>
+        <f t="shared" si="5"/>
+        <v>_properties.Add("56A3372E-CE9C-11D2-9F0E-006097C686F6/12", LanguageConsts._56A3372E_CE9C_11D2_9F0E_006097C686F6_12);</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A175" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="B175" t="s">
-        <v>804</v>
+        <v>833</v>
       </c>
       <c r="C175" t="s">
         <v>588</v>
       </c>
       <c r="E175" t="str">
-        <f t="shared" si="0"/>
-        <v>_properties.Add("56A3372E-CE9C-11D2-9F0E-006097C686F6/39", LanguageConsts._56A3372E-CE9C-11D2-9F0E-006097C686F6_39);</v>
+        <f t="shared" si="5"/>
+        <v>_properties.Add("56A3372E-CE9C-11D2-9F0E-006097C686F6/39", LanguageConsts._56A3372E_CE9C_11D2_9F0E_006097C686F6_39);</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A176" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="B176" t="s">
-        <v>805</v>
+        <v>834</v>
       </c>
       <c r="C176" t="s">
         <v>590</v>
       </c>
       <c r="E176" t="str">
-        <f t="shared" si="0"/>
-        <v>_properties.Add("56A3372E-CE9C-11D2-9F0E-006097C686F6/37", LanguageConsts._56A3372E-CE9C-11D2-9F0E-006097C686F6_37);</v>
+        <f t="shared" si="5"/>
+        <v>_properties.Add("56A3372E-CE9C-11D2-9F0E-006097C686F6/37", LanguageConsts._56A3372E_CE9C_11D2_9F0E_006097C686F6_37);</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A177" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="B177" t="s">
-        <v>806</v>
+        <v>835</v>
       </c>
       <c r="C177" t="s">
         <v>591</v>
       </c>
       <c r="E177" t="str">
-        <f t="shared" si="0"/>
-        <v>_properties.Add("D0A04F0A-462A-48A4-BB2F-3706E88DBD7D/100", LanguageConsts._D0A04F0A-462A-48A4-BB2F-3706E88DBD7D_100);</v>
+        <f t="shared" si="5"/>
+        <v>_properties.Add("D0A04F0A-462A-48A4-BB2F-3706E88DBD7D/100", LanguageConsts._D0A04F0A_462A_48A4_BB2F_3706E88DBD7D_100);</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A178" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="B178" t="s">
-        <v>807</v>
+        <v>836</v>
       </c>
       <c r="C178" t="s">
         <v>592</v>
       </c>
       <c r="E178" t="str">
-        <f t="shared" si="0"/>
-        <v>_properties.Add("F334115E-DA1B-4509-9B3D-119504DC7ABB/15", LanguageConsts._F334115E-DA1B-4509-9B3D-119504DC7ABB_15);</v>
+        <f t="shared" si="5"/>
+        <v>_properties.Add("F334115E-DA1B-4509-9B3D-119504DC7ABB/15", LanguageConsts._F334115E_DA1B_4509_9B3D_119504DC7ABB_15);</v>
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A179" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="B179" t="s">
-        <v>808</v>
+        <v>837</v>
       </c>
       <c r="C179" t="s">
         <v>593</v>
       </c>
       <c r="E179" t="str">
-        <f t="shared" si="0"/>
-        <v>_properties.Add("D5CDD502-2E9C-101B-9397-08002B2CF9AE/5", LanguageConsts._D5CDD502-2E9C-101B-9397-08002B2CF9AE_5);</v>
+        <f t="shared" si="5"/>
+        <v>_properties.Add("D5CDD502-2E9C-101B-9397-08002B2CF9AE/5", LanguageConsts._D5CDD502_2E9C_101B_9397_08002B2CF9AE_5);</v>
       </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A180" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="B180" t="s">
-        <v>809</v>
+        <v>838</v>
       </c>
       <c r="C180" t="s">
         <v>594</v>
       </c>
       <c r="E180" t="str">
-        <f t="shared" si="0"/>
-        <v>_properties.Add("D5CDD502-2E9C-101B-9397-08002B2CF9AE/6", LanguageConsts._D5CDD502-2E9C-101B-9397-08002B2CF9AE_6);</v>
+        <f t="shared" si="5"/>
+        <v>_properties.Add("D5CDD502-2E9C-101B-9397-08002B2CF9AE/6", LanguageConsts._D5CDD502_2E9C_101B_9397_08002B2CF9AE_6);</v>
       </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A181" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="B181" t="s">
-        <v>810</v>
+        <v>839</v>
       </c>
       <c r="C181" t="s">
         <v>595</v>
       </c>
       <c r="E181" t="str">
-        <f t="shared" si="0"/>
-        <v>_properties.Add("AEAC19E4-89AE-4508-B9B7-BB867ABEE2ED/2", LanguageConsts._AEAC19E4-89AE-4508-B9B7-BB867ABEE2ED_2);</v>
+        <f t="shared" si="5"/>
+        <v>_properties.Add("AEAC19E4-89AE-4508-B9B7-BB867ABEE2ED/2", LanguageConsts._AEAC19E4_89AE_4508_B9B7_BB867ABEE2ED_2);</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A182" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="B182" t="s">
-        <v>811</v>
+        <v>840</v>
       </c>
       <c r="C182" t="s">
         <v>597</v>
       </c>
       <c r="E182" t="str">
-        <f t="shared" si="0"/>
-        <v>_properties.Add("E08805C8-E395-40DF-80D2-54F0D6C43154/100", LanguageConsts._E08805C8-E395-40DF-80D2-54F0D6C43154_100);</v>
+        <f t="shared" si="5"/>
+        <v>_properties.Add("E08805C8-E395-40DF-80D2-54F0D6C43154/100", LanguageConsts._E08805C8_E395_40DF_80D2_54F0D6C43154_100);</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A183" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="B183" t="s">
-        <v>812</v>
+        <v>841</v>
       </c>
       <c r="C183" t="s">
         <v>598</v>
       </c>
       <c r="E183" t="str">
-        <f t="shared" si="0"/>
-        <v>_properties.Add("6444048F-4C8B-11D1-8B70-080036B11A03/7", LanguageConsts._6444048F-4C8B-11D1-8B70-080036B11A03_7);</v>
+        <f t="shared" si="5"/>
+        <v>_properties.Add("6444048F-4C8B-11D1-8B70-080036B11A03/7", LanguageConsts._6444048F_4C8B_11D1_8B70_080036B11A03_7);</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A184" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="B184" t="s">
-        <v>813</v>
+        <v>842</v>
       </c>
       <c r="C184" t="s">
         <v>599</v>
       </c>
       <c r="E184" t="str">
-        <f t="shared" si="0"/>
-        <v>_properties.Add("14B81DA1-0135-4D31-96D9-6CBFC9671A99/259", LanguageConsts._14B81DA1-0135-4D31-96D9-6CBFC9671A99_259);</v>
+        <f t="shared" si="5"/>
+        <v>_properties.Add("14B81DA1-0135-4D31-96D9-6CBFC9671A99/259", LanguageConsts._14B81DA1_0135_4D31_96D9_6CBFC9671A99_259);</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A185" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="B185" t="s">
-        <v>814</v>
+        <v>843</v>
       </c>
       <c r="C185" t="s">
         <v>600</v>
       </c>
       <c r="E185" t="str">
-        <f t="shared" si="0"/>
-        <v>_properties.Add("6444048F-4C8B-11D1-8B70-080036B11A03/3", LanguageConsts._6444048F-4C8B-11D1-8B70-080036B11A03_3);</v>
+        <f t="shared" si="5"/>
+        <v>_properties.Add("6444048F-4C8B-11D1-8B70-080036B11A03/3", LanguageConsts._6444048F_4C8B_11D1_8B70_080036B11A03_3);</v>
       </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A186" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="B186" t="s">
-        <v>815</v>
+        <v>844</v>
       </c>
       <c r="C186" t="s">
         <v>601</v>
       </c>
       <c r="E186" t="str">
-        <f t="shared" si="0"/>
-        <v>_properties.Add("6444048F-4C8B-11D1-8B70-080036B11A03/4", LanguageConsts._6444048F-4C8B-11D1-8B70-080036B11A03_4);</v>
+        <f t="shared" si="5"/>
+        <v>_properties.Add("6444048F-4C8B-11D1-8B70-080036B11A03/4", LanguageConsts._6444048F_4C8B_11D1_8B70_080036B11A03_4);</v>
       </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A187" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="B187" t="s">
-        <v>816</v>
+        <v>845</v>
       </c>
       <c r="C187" t="s">
         <v>602</v>
       </c>
       <c r="E187" t="str">
-        <f t="shared" si="0"/>
-        <v>_properties.Add("14B81DA1-0135-4D31-96D9-6CBFC9671A99/37378", LanguageConsts._14B81DA1-0135-4D31-96D9-6CBFC9671A99_37378);</v>
+        <f t="shared" si="5"/>
+        <v>_properties.Add("14B81DA1-0135-4D31-96D9-6CBFC9671A99/37378", LanguageConsts._14B81DA1_0135_4D31_96D9_6CBFC9671A99_37378);</v>
       </c>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A188" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="B188" t="s">
-        <v>817</v>
+        <v>846</v>
       </c>
       <c r="C188" t="s">
         <v>603</v>
       </c>
       <c r="E188" t="str">
-        <f t="shared" si="0"/>
-        <v>_properties.Add("14B81DA1-0135-4D31-96D9-6CBFC9671A99/36867", LanguageConsts._14B81DA1-0135-4D31-96D9-6CBFC9671A99_36867);</v>
+        <f t="shared" si="5"/>
+        <v>_properties.Add("14B81DA1-0135-4D31-96D9-6CBFC9671A99/36867", LanguageConsts._14B81DA1_0135_4D31_96D9_6CBFC9671A99_36867);</v>
       </c>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A189" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="B189" t="s">
-        <v>818</v>
+        <v>847</v>
       </c>
       <c r="C189" t="s">
         <v>604</v>
       </c>
       <c r="E189" t="str">
-        <f t="shared" si="0"/>
-        <v>_properties.Add("F85BF840-A925-4BC2-B0C4-8E36B598679E/100", LanguageConsts._F85BF840-A925-4BC2-B0C4-8E36B598679E_100);</v>
+        <f t="shared" si="5"/>
+        <v>_properties.Add("F85BF840-A925-4BC2-B0C4-8E36B598679E/100", LanguageConsts._F85BF840_A925_4BC2_B0C4_8E36B598679E_100);</v>
       </c>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A190" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="B190" t="s">
-        <v>819</v>
+        <v>848</v>
       </c>
       <c r="C190" t="s">
         <v>605</v>
       </c>
       <c r="E190" t="str">
-        <f t="shared" si="0"/>
-        <v>_properties.Add("14B81DA1-0135-4D31-96D9-6CBFC9671A99/18248", LanguageConsts._14B81DA1-0135-4D31-96D9-6CBFC9671A99_18248);</v>
+        <f t="shared" si="5"/>
+        <v>_properties.Add("14B81DA1-0135-4D31-96D9-6CBFC9671A99/18248", LanguageConsts._14B81DA1_0135_4D31_96D9_6CBFC9671A99_18248);</v>
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A191" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="B191" t="s">
-        <v>820</v>
+        <v>849</v>
       </c>
       <c r="C191" t="s">
         <v>606</v>
       </c>
       <c r="E191" t="str">
-        <f t="shared" si="0"/>
-        <v>_properties.Add("14B81DA1-0135-4D31-96D9-6CBFC9671A99/37380", LanguageConsts._14B81DA1-0135-4D31-96D9-6CBFC9671A99_37380);</v>
+        <f t="shared" si="5"/>
+        <v>_properties.Add("14B81DA1-0135-4D31-96D9-6CBFC9671A99/37380", LanguageConsts._14B81DA1_0135_4D31_96D9_6CBFC9671A99_37380);</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A192" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="B192" t="s">
-        <v>821</v>
+        <v>850</v>
       </c>
       <c r="C192" t="s">
         <v>607</v>
       </c>
       <c r="E192" t="str">
-        <f t="shared" si="0"/>
-        <v>_properties.Add("14B81DA1-0135-4D31-96D9-6CBFC9671A99/33434", LanguageConsts._14B81DA1-0135-4D31-96D9-6CBFC9671A99_33434);</v>
+        <f t="shared" si="5"/>
+        <v>_properties.Add("14B81DA1-0135-4D31-96D9-6CBFC9671A99/33434", LanguageConsts._14B81DA1_0135_4D31_96D9_6CBFC9671A99_33434);</v>
       </c>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A193" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="B193" t="s">
-        <v>822</v>
+        <v>851</v>
       </c>
       <c r="C193" t="s">
         <v>608</v>
       </c>
       <c r="E193" t="str">
-        <f t="shared" si="0"/>
-        <v>_properties.Add("2D152B40-CA39-40DB-B2CC-573725B2FEC5/100", LanguageConsts._2D152B40-CA39-40DB-B2CC-573725B2FEC5_100);</v>
+        <f t="shared" si="5"/>
+        <v>_properties.Add("2D152B40-CA39-40DB-B2CC-573725B2FEC5/100", LanguageConsts._2D152B40_CA39_40DB_B2CC_573725B2FEC5_100);</v>
       </c>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A194" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="B194" t="s">
-        <v>823</v>
+        <v>852</v>
       </c>
       <c r="C194" t="s">
         <v>609</v>
       </c>
       <c r="E194" t="str">
-        <f t="shared" si="0"/>
-        <v>_properties.Add("14B81DA1-0135-4D31-96D9-6CBFC9671A99/37386", LanguageConsts._14B81DA1-0135-4D31-96D9-6CBFC9671A99_37386);</v>
+        <f t="shared" si="5"/>
+        <v>_properties.Add("14B81DA1-0135-4D31-96D9-6CBFC9671A99/37386", LanguageConsts._14B81DA1_0135_4D31_96D9_6CBFC9671A99_37386);</v>
       </c>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A195" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="B195" t="s">
-        <v>824</v>
+        <v>853</v>
       </c>
       <c r="C195" t="s">
         <v>610</v>
       </c>
       <c r="E195" t="str">
-        <f t="shared" si="0"/>
-        <v>_properties.Add("14B81DA1-0135-4D31-96D9-6CBFC9671A99/34855", LanguageConsts._14B81DA1-0135-4D31-96D9-6CBFC9671A99_34855);</v>
+        <f t="shared" si="5"/>
+        <v>_properties.Add("14B81DA1-0135-4D31-96D9-6CBFC9671A99/34855", LanguageConsts._14B81DA1_0135_4D31_96D9_6CBFC9671A99_34855);</v>
       </c>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A196" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="B196" t="s">
-        <v>825</v>
+        <v>854</v>
       </c>
       <c r="C196" t="s">
         <v>611</v>
       </c>
       <c r="E196" t="str">
-        <f t="shared" si="0"/>
-        <v>_properties.Add("14B81DA1-0135-4D31-96D9-6CBFC9671A99/37383", LanguageConsts._14B81DA1-0135-4D31-96D9-6CBFC9671A99_37383);</v>
+        <f t="shared" si="5"/>
+        <v>_properties.Add("14B81DA1-0135-4D31-96D9-6CBFC9671A99/37383", LanguageConsts._14B81DA1_0135_4D31_96D9_6CBFC9671A99_37383);</v>
       </c>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A197" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="B197" t="s">
-        <v>826</v>
+        <v>855</v>
       </c>
       <c r="C197" t="s">
         <v>612</v>
       </c>
       <c r="E197" t="str">
-        <f t="shared" si="0"/>
-        <v>_properties.Add("E8309B6E-084C-49B4-B1FC-90A80331B638/100", LanguageConsts._E8309B6E-084C-49B4-B1FC-90A80331B638_100);</v>
+        <f t="shared" si="5"/>
+        <v>_properties.Add("E8309B6E-084C-49B4-B1FC-90A80331B638/100", LanguageConsts._E8309B6E_084C_49B4_B1FC_90A80331B638_100);</v>
       </c>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A198" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B198" t="s">
-        <v>827</v>
+        <v>856</v>
       </c>
       <c r="C198" t="s">
         <v>613</v>
       </c>
       <c r="E198" t="str">
-        <f t="shared" si="0"/>
-        <v>_properties.Add("14B81DA1-0135-4D31-96D9-6CBFC9671A99/37377", LanguageConsts._14B81DA1-0135-4D31-96D9-6CBFC9671A99_37377);</v>
+        <f t="shared" si="5"/>
+        <v>_properties.Add("14B81DA1-0135-4D31-96D9-6CBFC9671A99/37377", LanguageConsts._14B81DA1_0135_4D31_96D9_6CBFC9671A99_37377);</v>
       </c>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A199" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="B199" t="s">
-        <v>828</v>
+        <v>857</v>
       </c>
       <c r="C199" t="s">
         <v>614</v>
       </c>
       <c r="E199" t="str">
-        <f t="shared" si="0"/>
-        <v>_properties.Add("14B81DA1-0135-4D31-96D9-6CBFC9671A99/37382", LanguageConsts._14B81DA1-0135-4D31-96D9-6CBFC9671A99_37382);</v>
+        <f t="shared" si="5"/>
+        <v>_properties.Add("14B81DA1-0135-4D31-96D9-6CBFC9671A99/37382", LanguageConsts._14B81DA1_0135_4D31_96D9_6CBFC9671A99_37382);</v>
       </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A200" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="B200" t="s">
-        <v>829</v>
+        <v>858</v>
       </c>
       <c r="C200" t="s">
         <v>615</v>
       </c>
       <c r="E200" t="str">
-        <f t="shared" si="0"/>
-        <v>_properties.Add("EE3D3D8A-5381-4CFA-B13B-AAF66B5F4EC9/100", LanguageConsts._EE3D3D8A-5381-4CFA-B13B-AAF66B5F4EC9_100);</v>
+        <f t="shared" si="5"/>
+        <v>_properties.Add("EE3D3D8A-5381-4CFA-B13B-AAF66B5F4EC9/100", LanguageConsts._EE3D3D8A_5381_4CFA_B13B_AAF66B5F4EC9_100);</v>
       </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A201" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="B201" t="s">
-        <v>830</v>
+        <v>859</v>
       </c>
       <c r="C201" t="s">
         <v>616</v>
       </c>
       <c r="E201" t="str">
-        <f t="shared" ref="E201:E264" si="1">CONCATENATE("_properties.Add(""",A201,""", LanguageConsts.",B201,");")</f>
-        <v>_properties.Add("A0E74609-B84D-4F49-B860-462BD9971F98/100", LanguageConsts._A0E74609-B84D-4F49-B860-462BD9971F98_100);</v>
+        <f t="shared" ref="E201:E264" si="6">CONCATENATE("_properties.Add(""",A201,""", LanguageConsts.",B201,");")</f>
+        <v>_properties.Add("A0E74609-B84D-4F49-B860-462BD9971F98/100", LanguageConsts._A0E74609_B84D_4F49_B860_462BD9971F98_100);</v>
       </c>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A202" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="B202" t="s">
-        <v>831</v>
+        <v>860</v>
       </c>
       <c r="C202" t="s">
         <v>617</v>
       </c>
       <c r="E202" t="str">
-        <f t="shared" si="1"/>
-        <v>_properties.Add("D35F743A-EB2E-47F2-A286-844132CB1427/100", LanguageConsts._D35F743A-EB2E-47F2-A286-844132CB1427_100);</v>
+        <f t="shared" si="6"/>
+        <v>_properties.Add("D35F743A-EB2E-47F2-A286-844132CB1427/100", LanguageConsts._D35F743A_EB2E_47F2_A286_844132CB1427_100);</v>
       </c>
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A203" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="B203" t="s">
-        <v>832</v>
+        <v>861</v>
       </c>
       <c r="C203" t="s">
         <v>618</v>
       </c>
       <c r="E203" t="str">
-        <f t="shared" si="1"/>
-        <v>_properties.Add("14B81DA1-0135-4D31-96D9-6CBFC9671A99/34850", LanguageConsts._14B81DA1-0135-4D31-96D9-6CBFC9671A99_34850);</v>
+        <f t="shared" si="6"/>
+        <v>_properties.Add("14B81DA1-0135-4D31-96D9-6CBFC9671A99/34850", LanguageConsts._14B81DA1_0135_4D31_96D9_6CBFC9671A99_34850);</v>
       </c>
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A204" t="s">
-        <v>726</v>
+        <v>932</v>
       </c>
       <c r="B204" t="s">
-        <v>833</v>
+        <v>933</v>
       </c>
       <c r="C204" t="s">
         <v>619</v>
       </c>
       <c r="E204" t="str">
-        <f t="shared" si="1"/>
-        <v>_properties.Add("14B81DA1-0135-4D31-96D9-6CBFC9671A99}/33437", LanguageConsts._14B81DA1-0135-4D31-96D9-6CBFC9671A99}_33437);</v>
+        <f t="shared" si="6"/>
+        <v>_properties.Add("14B81DA1-0135-4D31-96D9-6CBFC9671A99/33437", LanguageConsts._14B81DA1_0135_4D31_96D9_6CBFC9671A99_33437);</v>
       </c>
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A205" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="B205" t="s">
-        <v>834</v>
+        <v>862</v>
       </c>
       <c r="C205" t="s">
         <v>620</v>
       </c>
       <c r="E205" t="str">
-        <f t="shared" si="1"/>
-        <v>_properties.Add("E6DDCAF7-29C5-4F0A-9A68-D19412EC7090/100", LanguageConsts._E6DDCAF7-29C5-4F0A-9A68-D19412EC7090_100);</v>
+        <f t="shared" si="6"/>
+        <v>_properties.Add("E6DDCAF7-29C5-4F0A-9A68-D19412EC7090/100", LanguageConsts._E6DDCAF7_29C5_4F0A_9A68_D19412EC7090_100);</v>
       </c>
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A206" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="B206" t="s">
-        <v>835</v>
+        <v>863</v>
       </c>
       <c r="C206" t="s">
         <v>621</v>
       </c>
       <c r="E206" t="str">
-        <f t="shared" si="1"/>
-        <v>_properties.Add("E1277516-2B5F-4869-89B1-2E585BD38B7A/100", LanguageConsts._E1277516-2B5F-4869-89B1-2E585BD38B7A_100);</v>
+        <f t="shared" si="6"/>
+        <v>_properties.Add("E1277516-2B5F-4869-89B1-2E585BD38B7A/100", LanguageConsts._E1277516_2B5F_4869_89B1_2E585BD38B7A_100);</v>
       </c>
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A207" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="B207" t="s">
-        <v>836</v>
+        <v>864</v>
       </c>
       <c r="C207" t="s">
         <v>622</v>
       </c>
       <c r="E207" t="str">
-        <f t="shared" si="1"/>
-        <v>_properties.Add("6D217F6D-3F6A-4825-B470-5F03CA2FBE9B/100", LanguageConsts._6D217F6D-3F6A-4825-B470-5F03CA2FBE9B_100);</v>
+        <f t="shared" si="6"/>
+        <v>_properties.Add("6D217F6D-3F6A-4825-B470-5F03CA2FBE9B/100", LanguageConsts._6D217F6D_3F6A_4825_B470_5F03CA2FBE9B_100);</v>
       </c>
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A208" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="B208" t="s">
-        <v>837</v>
+        <v>865</v>
       </c>
       <c r="C208" t="s">
         <v>623</v>
       </c>
       <c r="E208" t="str">
-        <f t="shared" si="1"/>
-        <v>_properties.Add("49237325-A95A-4F67-B211-816B2D45D2E0/100", LanguageConsts._49237325-A95A-4F67-B211-816B2D45D2E0_100);</v>
+        <f t="shared" si="6"/>
+        <v>_properties.Add("49237325-A95A-4F67-B211-816B2D45D2E0/100", LanguageConsts._49237325_A95A_4F67_B211_816B2D45D2E0_100);</v>
       </c>
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A209" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="B209" t="s">
-        <v>838</v>
+        <v>866</v>
       </c>
       <c r="C209" t="s">
         <v>624</v>
       </c>
       <c r="E209" t="str">
-        <f t="shared" si="1"/>
-        <v>_properties.Add("64440492-4C8B-11D1-8B70-080036B11A03/27", LanguageConsts._64440492-4C8B-11D1-8B70-080036B11A03_27);</v>
+        <f t="shared" si="6"/>
+        <v>_properties.Add("64440492-4C8B-11D1-8B70-080036B11A03/27", LanguageConsts._64440492_4C8B_11D1_8B70_080036B11A03_27);</v>
       </c>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A210" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="B210" t="s">
-        <v>839</v>
+        <v>867</v>
       </c>
       <c r="C210" t="s">
         <v>625</v>
       </c>
       <c r="E210" t="str">
-        <f t="shared" si="1"/>
-        <v>_properties.Add("64440492-4C8B-11D1-8B70-080036B11A03/28", LanguageConsts._64440492-4C8B-11D1-8B70-080036B11A03_28);</v>
+        <f t="shared" si="6"/>
+        <v>_properties.Add("64440492-4C8B-11D1-8B70-080036B11A03/28", LanguageConsts._64440492_4C8B_11D1_8B70_080036B11A03_28);</v>
       </c>
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A211" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="B211" t="s">
-        <v>840</v>
+        <v>868</v>
       </c>
       <c r="C211" t="s">
         <v>626</v>
       </c>
       <c r="E211" t="str">
-        <f t="shared" si="1"/>
-        <v>_properties.Add("2E4B640D-5019-46D8-8881-55414CC5CAA0/100", LanguageConsts._2E4B640D-5019-46D8-8881-55414CC5CAA0_100);</v>
+        <f t="shared" si="6"/>
+        <v>_properties.Add("2E4B640D-5019-46D8-8881-55414CC5CAA0/100", LanguageConsts._2E4B640D_5019_46D8_8881_55414CC5CAA0_100);</v>
       </c>
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A212" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="B212" t="s">
-        <v>841</v>
+        <v>869</v>
       </c>
       <c r="C212" t="s">
         <v>627</v>
       </c>
       <c r="E212" t="str">
-        <f t="shared" si="1"/>
-        <v>_properties.Add("64440490-4C8B-11D1-8B70-080036B11A03/3", LanguageConsts._64440490-4C8B-11D1-8B70-080036B11A03_3);</v>
+        <f t="shared" si="6"/>
+        <v>_properties.Add("64440490-4C8B-11D1-8B70-080036B11A03/3", LanguageConsts._64440490_4C8B_11D1_8B70_080036B11A03_3);</v>
       </c>
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A213" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="B213" t="s">
-        <v>842</v>
+        <v>870</v>
       </c>
       <c r="C213" t="s">
         <v>628</v>
       </c>
       <c r="E213" t="str">
-        <f t="shared" si="1"/>
-        <v>_properties.Add("64440492-4C8B-11D1-8B70-080036B11A03/36", LanguageConsts._64440492-4C8B-11D1-8B70-080036B11A03_36);</v>
+        <f t="shared" si="6"/>
+        <v>_properties.Add("64440492-4C8B-11D1-8B70-080036B11A03/36", LanguageConsts._64440492_4C8B_11D1_8B70_080036B11A03_36);</v>
       </c>
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A214" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="B214" t="s">
-        <v>843</v>
+        <v>871</v>
       </c>
       <c r="C214" t="s">
         <v>629</v>
       </c>
       <c r="E214" t="str">
-        <f t="shared" si="1"/>
-        <v>_properties.Add("6444048F-4C8B-11D1-8B70-080036B11A03/12", LanguageConsts._6444048F-4C8B-11D1-8B70-080036B11A03_12);</v>
+        <f t="shared" si="6"/>
+        <v>_properties.Add("6444048F-4C8B-11D1-8B70-080036B11A03/12", LanguageConsts._6444048F_4C8B_11D1_8B70_080036B11A03_12);</v>
       </c>
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A215" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="B215" t="s">
-        <v>844</v>
+        <v>872</v>
       </c>
       <c r="C215" t="s">
         <v>630</v>
       </c>
       <c r="E215" t="str">
-        <f t="shared" si="1"/>
-        <v>_properties.Add("64440492-4C8B-11D1-8B70-080036B11A03/22", LanguageConsts._64440492-4C8B-11D1-8B70-080036B11A03_22);</v>
+        <f t="shared" si="6"/>
+        <v>_properties.Add("64440492-4C8B-11D1-8B70-080036B11A03/22", LanguageConsts._64440492_4C8B_11D1_8B70_080036B11A03_22);</v>
       </c>
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A216" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="B216" t="s">
-        <v>845</v>
+        <v>873</v>
       </c>
       <c r="C216" t="s">
         <v>631</v>
       </c>
       <c r="E216" t="str">
-        <f t="shared" si="1"/>
-        <v>_properties.Add("64440492-4C8B-11D1-8B70-080036B11A03/39", LanguageConsts._64440492-4C8B-11D1-8B70-080036B11A03_39);</v>
+        <f t="shared" si="6"/>
+        <v>_properties.Add("64440492-4C8B-11D1-8B70-080036B11A03/39", LanguageConsts._64440492_4C8B_11D1_8B70_080036B11A03_39);</v>
       </c>
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A217" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="B217" t="s">
-        <v>846</v>
+        <v>874</v>
       </c>
       <c r="C217" t="s">
         <v>632</v>
       </c>
       <c r="E217" t="str">
-        <f t="shared" si="1"/>
-        <v>_properties.Add("64440492-4C8B-11D1-8B70-080036B11A03/30", LanguageConsts._64440492-4C8B-11D1-8B70-080036B11A03_30);</v>
+        <f t="shared" si="6"/>
+        <v>_properties.Add("64440492-4C8B-11D1-8B70-080036B11A03/30", LanguageConsts._64440492_4C8B_11D1_8B70_080036B11A03_30);</v>
       </c>
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A218" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="B218" t="s">
-        <v>847</v>
+        <v>875</v>
       </c>
       <c r="C218" t="s">
         <v>633</v>
       </c>
       <c r="E218" t="str">
-        <f t="shared" si="1"/>
-        <v>_properties.Add("56A3372E-CE9C-11D2-9F0E-006097C686F6/38", LanguageConsts._56A3372E-CE9C-11D2-9F0E-006097C686F6_38);</v>
+        <f t="shared" si="6"/>
+        <v>_properties.Add("56A3372E-CE9C-11D2-9F0E-006097C686F6/38", LanguageConsts._56A3372E_CE9C_11D2_9F0E_006097C686F6_38);</v>
       </c>
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A219" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="B219" t="s">
-        <v>848</v>
+        <v>876</v>
       </c>
       <c r="C219" t="s">
         <v>634</v>
       </c>
       <c r="E219" t="str">
-        <f t="shared" si="1"/>
-        <v>_properties.Add("64440492-4C8B-11D1-8B70-080036B11A03/23", LanguageConsts._64440492-4C8B-11D1-8B70-080036B11A03_23);</v>
+        <f t="shared" si="6"/>
+        <v>_properties.Add("64440492-4C8B-11D1-8B70-080036B11A03/23", LanguageConsts._64440492_4C8B_11D1_8B70_080036B11A03_23);</v>
       </c>
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A220" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="B220" t="s">
-        <v>849</v>
+        <v>877</v>
       </c>
       <c r="C220" t="s">
         <v>589</v>
       </c>
       <c r="E220" t="str">
-        <f t="shared" si="1"/>
-        <v>_properties.Add("64440492-4C8B-11D1-8B70-080036B11A03/21", LanguageConsts._64440492-4C8B-11D1-8B70-080036B11A03_21);</v>
+        <f t="shared" si="6"/>
+        <v>_properties.Add("64440492-4C8B-11D1-8B70-080036B11A03/21", LanguageConsts._64440492_4C8B_11D1_8B70_080036B11A03_21);</v>
       </c>
     </row>
     <row r="221" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A221" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="B221" t="s">
-        <v>850</v>
+        <v>878</v>
       </c>
       <c r="C221" t="s">
         <v>635</v>
       </c>
       <c r="E221" t="str">
-        <f t="shared" si="1"/>
-        <v>_properties.Add("64440491-4C8B-11D1-8B70-080036B11A03/10", LanguageConsts._64440491-4C8B-11D1-8B70-080036B11A03_10);</v>
+        <f t="shared" si="6"/>
+        <v>_properties.Add("64440491-4C8B-11D1-8B70-080036B11A03/10", LanguageConsts._64440491_4C8B_11D1_8B70_080036B11A03_10);</v>
       </c>
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A222" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="B222" t="s">
-        <v>851</v>
+        <v>879</v>
       </c>
       <c r="C222" t="s">
         <v>636</v>
       </c>
       <c r="E222" t="str">
-        <f t="shared" si="1"/>
-        <v>_properties.Add("64440492-4C8B-11D1-8B70-080036B11A03/20", LanguageConsts._64440492-4C8B-11D1-8B70-080036B11A03_20);</v>
+        <f t="shared" si="6"/>
+        <v>_properties.Add("64440492-4C8B-11D1-8B70-080036B11A03/20", LanguageConsts._64440492_4C8B_11D1_8B70_080036B11A03_20);</v>
       </c>
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A223" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="B223" t="s">
-        <v>852</v>
+        <v>880</v>
       </c>
       <c r="C223" t="s">
         <v>637</v>
       </c>
       <c r="E223" t="str">
-        <f t="shared" si="1"/>
-        <v>_properties.Add("64440491-4C8B-11D1-8B70-080036B11A03/8", LanguageConsts._64440491-4C8B-11D1-8B70-080036B11A03_8);</v>
+        <f t="shared" si="6"/>
+        <v>_properties.Add("64440491-4C8B-11D1-8B70-080036B11A03/8", LanguageConsts._64440491_4C8B_11D1_8B70_080036B11A03_8);</v>
       </c>
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A224" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="B224" t="s">
-        <v>853</v>
+        <v>881</v>
       </c>
       <c r="C224" t="s">
         <v>638</v>
       </c>
       <c r="E224" t="str">
-        <f t="shared" si="1"/>
-        <v>_properties.Add("64440491-4C8B-11D1-8B70-080036B11A03/44", LanguageConsts._64440491-4C8B-11D1-8B70-080036B11A03_44);</v>
+        <f t="shared" si="6"/>
+        <v>_properties.Add("64440491-4C8B-11D1-8B70-080036B11A03/44", LanguageConsts._64440491_4C8B_11D1_8B70_080036B11A03_44);</v>
       </c>
     </row>
     <row r="225" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A225" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="B225" t="s">
-        <v>854</v>
+        <v>882</v>
       </c>
       <c r="C225" t="s">
         <v>639</v>
       </c>
       <c r="E225" t="str">
-        <f t="shared" si="1"/>
-        <v>_properties.Add("64440491-4C8B-11D1-8B70-080036B11A03/42", LanguageConsts._64440491-4C8B-11D1-8B70-080036B11A03_42);</v>
+        <f t="shared" si="6"/>
+        <v>_properties.Add("64440491-4C8B-11D1-8B70-080036B11A03/42", LanguageConsts._64440491_4C8B_11D1_8B70_080036B11A03_42);</v>
       </c>
     </row>
     <row r="226" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A226" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="B226" t="s">
-        <v>855</v>
+        <v>883</v>
       </c>
       <c r="C226" t="s">
         <v>640</v>
       </c>
       <c r="E226" t="str">
-        <f t="shared" si="1"/>
-        <v>_properties.Add("64440491-4C8B-11D1-8B70-080036B11A03/45", LanguageConsts._64440491-4C8B-11D1-8B70-080036B11A03_45);</v>
+        <f t="shared" si="6"/>
+        <v>_properties.Add("64440491-4C8B-11D1-8B70-080036B11A03/45", LanguageConsts._64440491_4C8B_11D1_8B70_080036B11A03_45);</v>
       </c>
     </row>
     <row r="227" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A227" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="B227" t="s">
-        <v>856</v>
+        <v>884</v>
       </c>
       <c r="C227" t="s">
         <v>641</v>
       </c>
       <c r="E227" t="str">
-        <f t="shared" si="1"/>
-        <v>_properties.Add("64440491-4C8B-11D1-8B70-080036B11A03/43", LanguageConsts._64440491-4C8B-11D1-8B70-080036B11A03_43);</v>
+        <f t="shared" si="6"/>
+        <v>_properties.Add("64440491-4C8B-11D1-8B70-080036B11A03/43", LanguageConsts._64440491_4C8B_11D1_8B70_080036B11A03_43);</v>
       </c>
     </row>
     <row r="228" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A228" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="B228" t="s">
-        <v>857</v>
+        <v>885</v>
       </c>
       <c r="C228" t="s">
         <v>642</v>
       </c>
       <c r="E228" t="str">
-        <f t="shared" si="1"/>
-        <v>_properties.Add("0CEF7D53-FA64-11D1-A203-0000F81FEDEE/3", LanguageConsts._0CEF7D53-FA64-11D1-A203-0000F81FEDEE_3);</v>
+        <f t="shared" si="6"/>
+        <v>_properties.Add("0CEF7D53-FA64-11D1-A203-0000F81FEDEE/3", LanguageConsts._0CEF7D53_FA64_11D1_A203_0000F81FEDEE_3);</v>
       </c>
     </row>
     <row r="229" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A229" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="B229" t="s">
-        <v>858</v>
+        <v>886</v>
       </c>
       <c r="C229" t="s">
         <v>643</v>
       </c>
       <c r="E229" t="str">
-        <f t="shared" si="1"/>
-        <v>_properties.Add("0CEF7D53-FA64-11D1-A203-0000F81FEDEE/4", LanguageConsts._0CEF7D53-FA64-11D1-A203-0000F81FEDEE_4);</v>
+        <f t="shared" si="6"/>
+        <v>_properties.Add("0CEF7D53-FA64-11D1-A203-0000F81FEDEE/4", LanguageConsts._0CEF7D53_FA64_11D1_A203_0000F81FEDEE_4);</v>
       </c>
     </row>
     <row r="230" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A230" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="B230" t="s">
-        <v>859</v>
+        <v>887</v>
       </c>
       <c r="C230" t="s">
         <v>644</v>
       </c>
       <c r="E230" t="str">
-        <f t="shared" si="1"/>
-        <v>_properties.Add("841E4F90-FF59-4D16-8947-E81BBFFAB36D/16", LanguageConsts._841E4F90-FF59-4D16-8947-E81BBFFAB36D_16);</v>
+        <f t="shared" si="6"/>
+        <v>_properties.Add("841E4F90-FF59-4D16-8947-E81BBFFAB36D/16", LanguageConsts._841E4F90_FF59_4D16_8947_E81BBFFAB36D_16);</v>
       </c>
     </row>
     <row r="231" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A231" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="B231" t="s">
-        <v>860</v>
+        <v>888</v>
       </c>
       <c r="C231" t="s">
         <v>645</v>
       </c>
       <c r="E231" t="str">
-        <f t="shared" si="1"/>
-        <v>_properties.Add("0CEF7D53-FA64-11D1-A203-0000F81FEDEE/7", LanguageConsts._0CEF7D53-FA64-11D1-A203-0000F81FEDEE_7);</v>
+        <f t="shared" si="6"/>
+        <v>_properties.Add("0CEF7D53-FA64-11D1-A203-0000F81FEDEE/7", LanguageConsts._0CEF7D53_FA64_11D1_A203_0000F81FEDEE_7);</v>
       </c>
     </row>
     <row r="232" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A232" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="B232" t="s">
-        <v>861</v>
+        <v>889</v>
       </c>
       <c r="C232" t="s">
         <v>646</v>
       </c>
       <c r="E232" t="str">
-        <f t="shared" si="1"/>
-        <v>_properties.Add("0CEF7D53-FA64-11D1-A203-0000F81FEDEE/8", LanguageConsts._0CEF7D53-FA64-11D1-A203-0000F81FEDEE_8);</v>
+        <f t="shared" si="6"/>
+        <v>_properties.Add("0CEF7D53-FA64-11D1-A203-0000F81FEDEE/8", LanguageConsts._0CEF7D53_FA64_11D1_A203_0000F81FEDEE_8);</v>
       </c>
     </row>
     <row r="233" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A233" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="B233" t="s">
-        <v>862</v>
+        <v>890</v>
       </c>
       <c r="C233" t="s">
         <v>647</v>
       </c>
       <c r="E233" t="str">
-        <f t="shared" si="1"/>
-        <v>_properties.Add("D5CDD502-2E9C-101B-9397-08002B2CF9AE/29", LanguageConsts._D5CDD502-2E9C-101B-9397-08002B2CF9AE_29);</v>
+        <f t="shared" si="6"/>
+        <v>_properties.Add("D5CDD502-2E9C-101B-9397-08002B2CF9AE/29", LanguageConsts._D5CDD502_2E9C_101B_9397_08002B2CF9AE_29);</v>
       </c>
     </row>
     <row r="234" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A234" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="B234" t="s">
-        <v>863</v>
+        <v>891</v>
       </c>
       <c r="C234" t="s">
         <v>596</v>
       </c>
       <c r="E234" t="str">
-        <f t="shared" si="1"/>
-        <v>_properties.Add("64440492-4C8B-11D1-8B70-080036B11A03/11", LanguageConsts._64440492-4C8B-11D1-8B70-080036B11A03_11);</v>
+        <f t="shared" si="6"/>
+        <v>_properties.Add("64440492-4C8B-11D1-8B70-080036B11A03/11", LanguageConsts._64440492_4C8B_11D1_8B70_080036B11A03_11);</v>
       </c>
     </row>
     <row r="235" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A235" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="B235" t="s">
-        <v>864</v>
+        <v>892</v>
       </c>
       <c r="C235" t="s">
         <v>648</v>
       </c>
       <c r="E235" t="str">
-        <f t="shared" si="1"/>
-        <v>_properties.Add("6D748DE2-8D38-4CC3-AC60-F009B057C557/7", LanguageConsts._6D748DE2-8D38-4CC3-AC60-F009B057C557_7);</v>
+        <f t="shared" si="6"/>
+        <v>_properties.Add("6D748DE2-8D38-4CC3-AC60-F009B057C557/7", LanguageConsts._6D748DE2_8D38_4CC3_AC60_F009B057C557_7);</v>
       </c>
     </row>
     <row r="236" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A236" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="B236" t="s">
-        <v>865</v>
+        <v>893</v>
       </c>
       <c r="C236" t="s">
         <v>649</v>
       </c>
       <c r="E236" t="str">
-        <f t="shared" si="1"/>
-        <v>_properties.Add("6D748DE2-8D38-4CC3-AC60-F009B057C557/2", LanguageConsts._6D748DE2-8D38-4CC3-AC60-F009B057C557_2);</v>
+        <f t="shared" si="6"/>
+        <v>_properties.Add("6D748DE2-8D38-4CC3-AC60-F009B057C557/2", LanguageConsts._6D748DE2_8D38_4CC3_AC60_F009B057C557_2);</v>
       </c>
     </row>
     <row r="237" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A237" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="B237" t="s">
-        <v>866</v>
+        <v>894</v>
       </c>
       <c r="C237" t="s">
         <v>650</v>
       </c>
       <c r="E237" t="str">
-        <f t="shared" si="1"/>
-        <v>_properties.Add("6D748DE2-8D38-4CC3-AC60-F009B057C557/12", LanguageConsts._6D748DE2-8D38-4CC3-AC60-F009B057C557_12);</v>
+        <f t="shared" si="6"/>
+        <v>_properties.Add("6D748DE2-8D38-4CC3-AC60-F009B057C557/12", LanguageConsts._6D748DE2_8D38_4CC3_AC60_F009B057C557_12);</v>
       </c>
     </row>
     <row r="238" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A238" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="B238" t="s">
-        <v>867</v>
+        <v>895</v>
       </c>
       <c r="C238" t="s">
         <v>651</v>
       </c>
       <c r="E238" t="str">
-        <f t="shared" si="1"/>
-        <v>_properties.Add("6D748DE2-8D38-4CC3-AC60-F009B057C557/17", LanguageConsts._6D748DE2-8D38-4CC3-AC60-F009B057C557_17);</v>
+        <f t="shared" si="6"/>
+        <v>_properties.Add("6D748DE2-8D38-4CC3-AC60-F009B057C557/17", LanguageConsts._6D748DE2_8D38_4CC3_AC60_F009B057C557_17);</v>
       </c>
     </row>
     <row r="239" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A239" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="B239" t="s">
-        <v>868</v>
+        <v>896</v>
       </c>
       <c r="C239" t="s">
         <v>652</v>
       </c>
       <c r="E239" t="str">
-        <f t="shared" si="1"/>
-        <v>_properties.Add("6D748DE2-8D38-4CC3-AC60-F009B057C557/18", LanguageConsts._6D748DE2-8D38-4CC3-AC60-F009B057C557_18);</v>
+        <f t="shared" si="6"/>
+        <v>_properties.Add("6D748DE2-8D38-4CC3-AC60-F009B057C557/18", LanguageConsts._6D748DE2_8D38_4CC3_AC60_F009B057C557_18);</v>
       </c>
     </row>
     <row r="240" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A240" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="B240" t="s">
-        <v>869</v>
+        <v>897</v>
       </c>
       <c r="C240" t="s">
         <v>653</v>
       </c>
       <c r="E240" t="str">
-        <f t="shared" si="1"/>
-        <v>_properties.Add("6D748DE2-8D38-4CC3-AC60-F009B057C557/13", LanguageConsts._6D748DE2-8D38-4CC3-AC60-F009B057C557_13);</v>
+        <f t="shared" si="6"/>
+        <v>_properties.Add("6D748DE2-8D38-4CC3-AC60-F009B057C557/13", LanguageConsts._6D748DE2_8D38_4CC3_AC60_F009B057C557_13);</v>
       </c>
     </row>
     <row r="241" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A241" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="B241" t="s">
-        <v>870</v>
+        <v>898</v>
       </c>
       <c r="C241" t="s">
         <v>654</v>
       </c>
       <c r="E241" t="str">
-        <f t="shared" si="1"/>
-        <v>_properties.Add("2C53C813-FB63-4E22-A1AB-0B331CA1E273/100", LanguageConsts._2C53C813-FB63-4E22-A1AB-0B331CA1E273_100);</v>
+        <f t="shared" si="6"/>
+        <v>_properties.Add("2C53C813-FB63-4E22-A1AB-0B331CA1E273/100", LanguageConsts._2C53C813_FB63_4E22_A1AB_0B331CA1E273_100);</v>
       </c>
     </row>
     <row r="242" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A242" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="B242" t="s">
-        <v>871</v>
+        <v>899</v>
       </c>
       <c r="C242" t="s">
         <v>655</v>
       </c>
       <c r="E242" t="str">
-        <f t="shared" si="1"/>
-        <v>_properties.Add("4684FE97-8765-4842-9C13-F006447B178C/100", LanguageConsts._4684FE97-8765-4842-9C13-F006447B178C_100);</v>
+        <f t="shared" si="6"/>
+        <v>_properties.Add("4684FE97-8765-4842-9C13-F006447B178C/100", LanguageConsts._4684FE97_8765_4842_9C13_F006447B178C_100);</v>
       </c>
     </row>
     <row r="243" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A243" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
       <c r="B243" t="s">
-        <v>872</v>
+        <v>900</v>
       </c>
       <c r="C243" t="s">
         <v>656</v>
       </c>
       <c r="E243" t="str">
-        <f t="shared" si="1"/>
-        <v>_properties.Add("6D748DE2-8D38-4CC3-AC60-F009B057C557/3", LanguageConsts._6D748DE2-8D38-4CC3-AC60-F009B057C557_3);</v>
+        <f t="shared" si="6"/>
+        <v>_properties.Add("6D748DE2-8D38-4CC3-AC60-F009B057C557/3", LanguageConsts._6D748DE2_8D38_4CC3_AC60_F009B057C557_3);</v>
       </c>
     </row>
     <row r="244" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A244" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="B244" t="s">
-        <v>873</v>
+        <v>901</v>
       </c>
       <c r="C244" t="s">
         <v>657</v>
       </c>
       <c r="E244" t="str">
-        <f t="shared" si="1"/>
-        <v>_properties.Add("A5477F61-7A82-4ECA-9DDE-98B69B2479B3/100", LanguageConsts._A5477F61-7A82-4ECA-9DDE-98B69B2479B3_100);</v>
+        <f t="shared" si="6"/>
+        <v>_properties.Add("A5477F61-7A82-4ECA-9DDE-98B69B2479B3/100", LanguageConsts._A5477F61_7A82_4ECA_9DDE_98B69B2479B3_100);</v>
       </c>
     </row>
     <row r="245" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A245" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="B245" t="s">
-        <v>874</v>
+        <v>902</v>
       </c>
       <c r="C245" t="s">
         <v>658</v>
       </c>
       <c r="E245" t="str">
-        <f t="shared" si="1"/>
-        <v>_properties.Add("2CBAA8F5-D81F-47CA-B17A-F8D822300131/100", LanguageConsts._2CBAA8F5-D81F-47CA-B17A-F8D822300131_100);</v>
+        <f t="shared" si="6"/>
+        <v>_properties.Add("2CBAA8F5-D81F-47CA-B17A-F8D822300131/100", LanguageConsts._2CBAA8F5_D81F_47CA_B17A_F8D822300131_100);</v>
       </c>
     </row>
     <row r="246" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A246" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="B246" t="s">
-        <v>875</v>
+        <v>903</v>
       </c>
       <c r="C246" t="s">
         <v>659</v>
       </c>
       <c r="E246" t="str">
-        <f t="shared" si="1"/>
-        <v>_properties.Add("43F8D7B7-A444-4F87-9383-52271C9B915C/100", LanguageConsts._43F8D7B7-A444-4F87-9383-52271C9B915C_100);</v>
+        <f t="shared" si="6"/>
+        <v>_properties.Add("43F8D7B7-A444-4F87-9383-52271C9B915C/100", LanguageConsts._43F8D7B7_A444_4F87_9383_52271C9B915C_100);</v>
       </c>
     </row>
     <row r="247" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A247" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="B247" t="s">
-        <v>876</v>
+        <v>904</v>
       </c>
       <c r="C247" t="s">
         <v>660</v>
       </c>
       <c r="E247" t="str">
-        <f t="shared" si="1"/>
-        <v>_properties.Add("14B81DA1-0135-4D31-96D9-6CBFC9671A99/18258", LanguageConsts._14B81DA1-0135-4D31-96D9-6CBFC9671A99_18258);</v>
+        <f t="shared" si="6"/>
+        <v>_properties.Add("14B81DA1-0135-4D31-96D9-6CBFC9671A99/18258", LanguageConsts._14B81DA1_0135_4D31_96D9_6CBFC9671A99_18258);</v>
       </c>
     </row>
     <row r="248" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A248" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="B248" t="s">
-        <v>877</v>
+        <v>905</v>
       </c>
       <c r="C248" t="s">
         <v>661</v>
       </c>
       <c r="E248" t="str">
-        <f t="shared" si="1"/>
-        <v>_properties.Add("72FAB781-ACDA-43E5-B155-B2434F85E678/100", LanguageConsts._72FAB781-ACDA-43E5-B155-B2434F85E678_100);</v>
+        <f t="shared" si="6"/>
+        <v>_properties.Add("72FAB781-ACDA-43E5-B155-B2434F85E678/100", LanguageConsts._72FAB781_ACDA_43E5_B155_B2434F85E678_100);</v>
       </c>
     </row>
     <row r="249" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A249" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="B249" t="s">
-        <v>878</v>
+        <v>906</v>
       </c>
       <c r="C249" t="s">
         <v>662</v>
       </c>
       <c r="E249" t="str">
-        <f t="shared" si="1"/>
-        <v>_properties.Add("DE41CC29-6971-4290-B472-F59F2E2F31E2/100", LanguageConsts._DE41CC29-6971-4290-B472-F59F2E2F31E2_100);</v>
+        <f t="shared" si="6"/>
+        <v>_properties.Add("DE41CC29-6971-4290-B472-F59F2E2F31E2/100", LanguageConsts._DE41CC29_6971_4290_B472_F59F2E2F31E2_100);</v>
       </c>
     </row>
     <row r="250" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A250" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="B250" t="s">
-        <v>879</v>
+        <v>907</v>
       </c>
       <c r="C250" t="s">
         <v>663</v>
       </c>
       <c r="E250" t="str">
-        <f t="shared" si="1"/>
-        <v>_properties.Add("5CBF2787-48CF-4208-B90E-EE5E5D420294/23", LanguageConsts._5CBF2787-48CF-4208-B90E-EE5E5D420294_23);</v>
+        <f t="shared" si="6"/>
+        <v>_properties.Add("5CBF2787-48CF-4208-B90E-EE5E5D420294/23", LanguageConsts._5CBF2787_48CF_4208_B90E_EE5E5D420294_23);</v>
       </c>
     </row>
     <row r="251" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A251" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="B251" t="s">
-        <v>880</v>
+        <v>908</v>
       </c>
       <c r="C251" t="s">
         <v>664</v>
       </c>
       <c r="E251" t="str">
-        <f t="shared" si="1"/>
-        <v>_properties.Add("64440492-4C8B-11D1-8B70-080036B11A03/9", LanguageConsts._64440492-4C8B-11D1-8B70-080036B11A03_9);</v>
+        <f t="shared" si="6"/>
+        <v>_properties.Add("64440492-4C8B-11D1-8B70-080036B11A03/9", LanguageConsts._64440492_4C8B_11D1_8B70_080036B11A03_9);</v>
       </c>
     </row>
     <row r="252" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A252" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="B252" t="s">
-        <v>881</v>
+        <v>909</v>
       </c>
       <c r="C252" t="s">
         <v>665</v>
       </c>
       <c r="E252" t="str">
-        <f t="shared" si="1"/>
-        <v>_properties.Add("000214A1-0000-0000-C000-000000000046/9", LanguageConsts._000214A1-0000-0000-C000-000000000046_9);</v>
+        <f t="shared" si="6"/>
+        <v>_properties.Add("000214A1-0000-0000-C000-000000000046/9", LanguageConsts._000214A1_0000_0000_C000_000000000046_9);</v>
       </c>
     </row>
     <row r="253" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A253" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="B253" t="s">
-        <v>882</v>
+        <v>910</v>
       </c>
       <c r="C253" t="s">
         <v>666</v>
       </c>
       <c r="E253" t="str">
-        <f t="shared" si="1"/>
-        <v>_properties.Add("28636AA6-953D-11D2-B5D6-00C04FD918D0/14", LanguageConsts._28636AA6-953D-11D2-B5D6-00C04FD918D0_14);</v>
+        <f t="shared" si="6"/>
+        <v>_properties.Add("28636AA6-953D-11D2-B5D6-00C04FD918D0/14", LanguageConsts._28636AA6_953D_11D2_B5D6_00C04FD918D0_14);</v>
       </c>
     </row>
     <row r="254" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A254" t="s">
-        <v>896</v>
+        <v>786</v>
       </c>
       <c r="B254" t="s">
-        <v>897</v>
+        <v>911</v>
       </c>
       <c r="C254" t="s">
         <v>522</v>
       </c>
       <c r="E254" t="str">
-        <f t="shared" si="1"/>
-        <v>_properties.Add("D5CDD502-2E9C-101B-9397-08002B2CF9AE/8", LanguageConsts._D5CDD502-2E9C-101B-9397-08002B2CF9AE_8);</v>
+        <f t="shared" si="6"/>
+        <v>_properties.Add("D5CDD502-2E9C-101B-9397-08002B2CF9AE/8", LanguageConsts._D5CDD502_2E9C_101B_9397_08002B2CF9AE_8);</v>
       </c>
     </row>
     <row r="255" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A255" t="s">
-        <v>898</v>
+        <v>787</v>
       </c>
       <c r="B255" t="s">
-        <v>899</v>
+        <v>912</v>
       </c>
       <c r="C255" t="s">
         <v>523</v>
       </c>
       <c r="E255" t="str">
-        <f t="shared" si="1"/>
-        <v>_properties.Add("D5CDD502-2E9C-101B-9397-08002B2CF9AE/9", LanguageConsts._D5CDD502-2E9C-101B-9397-08002B2CF9AE_9);</v>
+        <f t="shared" si="6"/>
+        <v>_properties.Add("D5CDD502-2E9C-101B-9397-08002B2CF9AE/9", LanguageConsts._D5CDD502_2E9C_101B_9397_08002B2CF9AE_9);</v>
       </c>
     </row>
     <row r="256" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A256" t="s">
-        <v>900</v>
+        <v>788</v>
       </c>
       <c r="B256" t="s">
-        <v>901</v>
+        <v>913</v>
       </c>
       <c r="C256" t="s">
         <v>524</v>
       </c>
       <c r="E256" t="str">
-        <f t="shared" si="1"/>
-        <v>_properties.Add("D5CDD502-2E9C-101B-9397-08002B2CF9AE/10", LanguageConsts._D5CDD502-2E9C-101B-9397-08002B2CF9AE_10);</v>
+        <f t="shared" si="6"/>
+        <v>_properties.Add("D5CDD502-2E9C-101B-9397-08002B2CF9AE/10", LanguageConsts._D5CDD502_2E9C_101B_9397_08002B2CF9AE_10);</v>
       </c>
     </row>
     <row r="257" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A257" t="s">
-        <v>902</v>
+        <v>789</v>
       </c>
       <c r="B257" t="s">
-        <v>903</v>
+        <v>914</v>
       </c>
       <c r="C257" t="s">
         <v>525</v>
       </c>
       <c r="E257" t="str">
-        <f t="shared" si="1"/>
-        <v>_properties.Add("D5CDD502-2E9C-101B-9397-08002B2CF9AE/11", LanguageConsts._D5CDD502-2E9C-101B-9397-08002B2CF9AE_11);</v>
+        <f t="shared" si="6"/>
+        <v>_properties.Add("D5CDD502-2E9C-101B-9397-08002B2CF9AE/11", LanguageConsts._D5CDD502_2E9C_101B_9397_08002B2CF9AE_11);</v>
       </c>
     </row>
     <row r="258" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A258" t="s">
-        <v>904</v>
+        <v>790</v>
       </c>
       <c r="B258" t="s">
-        <v>905</v>
+        <v>915</v>
       </c>
       <c r="C258" t="s">
         <v>526</v>
       </c>
       <c r="E258" t="str">
-        <f t="shared" si="1"/>
-        <v>_properties.Add("D5CDD502-2E9C-101B-9397-08002B2CF9AE/12", LanguageConsts._D5CDD502-2E9C-101B-9397-08002B2CF9AE_12);</v>
+        <f t="shared" si="6"/>
+        <v>_properties.Add("D5CDD502-2E9C-101B-9397-08002B2CF9AE/12", LanguageConsts._D5CDD502_2E9C_101B_9397_08002B2CF9AE_12);</v>
       </c>
     </row>
     <row r="259" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A259" t="s">
-        <v>906</v>
+        <v>791</v>
       </c>
       <c r="B259" t="s">
-        <v>907</v>
+        <v>916</v>
       </c>
       <c r="C259" t="s">
         <v>527</v>
       </c>
       <c r="E259" t="str">
-        <f t="shared" si="1"/>
-        <v>_properties.Add("D5CDD502-2E9C-101B-9397-08002B2CF9AE/13", LanguageConsts._D5CDD502-2E9C-101B-9397-08002B2CF9AE_13);</v>
+        <f t="shared" si="6"/>
+        <v>_properties.Add("D5CDD502-2E9C-101B-9397-08002B2CF9AE/13", LanguageConsts._D5CDD502_2E9C_101B_9397_08002B2CF9AE_13);</v>
       </c>
     </row>
     <row r="260" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A260" t="s">
-        <v>908</v>
+        <v>792</v>
       </c>
       <c r="B260" t="s">
-        <v>909</v>
+        <v>917</v>
       </c>
       <c r="C260" t="s">
         <v>528</v>
       </c>
       <c r="E260" t="str">
-        <f t="shared" si="1"/>
-        <v>_properties.Add("D5CDD502-2E9C-101B-9397-08002B2CF9AE/16", LanguageConsts._D5CDD502-2E9C-101B-9397-08002B2CF9AE_16);</v>
+        <f t="shared" si="6"/>
+        <v>_properties.Add("D5CDD502-2E9C-101B-9397-08002B2CF9AE/16", LanguageConsts._D5CDD502_2E9C_101B_9397_08002B2CF9AE_16);</v>
       </c>
     </row>
     <row r="261" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A261" t="s">
-        <v>910</v>
+        <v>793</v>
       </c>
       <c r="B261" t="s">
-        <v>911</v>
+        <v>918</v>
       </c>
       <c r="C261" t="s">
         <v>529</v>
       </c>
       <c r="E261" t="str">
-        <f t="shared" si="1"/>
-        <v>_properties.Add("D5CDD502-2E9C-101B-9397-08002B2CF9AE/17", LanguageConsts._D5CDD502-2E9C-101B-9397-08002B2CF9AE_17);</v>
+        <f t="shared" si="6"/>
+        <v>_properties.Add("D5CDD502-2E9C-101B-9397-08002B2CF9AE/17", LanguageConsts._D5CDD502_2E9C_101B_9397_08002B2CF9AE_17);</v>
       </c>
     </row>
     <row r="262" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A262" t="s">
-        <v>912</v>
+        <v>794</v>
       </c>
       <c r="B262" t="s">
-        <v>913</v>
+        <v>919</v>
       </c>
       <c r="C262" t="s">
         <v>530</v>
       </c>
       <c r="E262" t="str">
-        <f t="shared" si="1"/>
-        <v>_properties.Add("D5CDD502-2E9C-101B-9397-08002B2CF9AE/18", LanguageConsts._D5CDD502-2E9C-101B-9397-08002B2CF9AE_18);</v>
+        <f t="shared" si="6"/>
+        <v>_properties.Add("D5CDD502-2E9C-101B-9397-08002B2CF9AE/18", LanguageConsts._D5CDD502_2E9C_101B_9397_08002B2CF9AE_18);</v>
       </c>
     </row>
     <row r="263" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A263" t="s">
-        <v>914</v>
+        <v>795</v>
       </c>
       <c r="B263" t="s">
-        <v>915</v>
+        <v>920</v>
       </c>
       <c r="C263" t="s">
         <v>531</v>
       </c>
       <c r="E263" t="str">
-        <f t="shared" si="1"/>
-        <v>_properties.Add("D5CDD502-2E9C-101B-9397-08002B2CF9AE/19", LanguageConsts._D5CDD502-2E9C-101B-9397-08002B2CF9AE_19);</v>
+        <f t="shared" si="6"/>
+        <v>_properties.Add("D5CDD502-2E9C-101B-9397-08002B2CF9AE/19", LanguageConsts._D5CDD502_2E9C_101B_9397_08002B2CF9AE_19);</v>
       </c>
     </row>
     <row r="264" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A264" t="s">
-        <v>916</v>
+        <v>796</v>
       </c>
       <c r="B264" t="s">
-        <v>917</v>
+        <v>921</v>
       </c>
       <c r="C264" t="s">
         <v>532</v>
       </c>
       <c r="E264" t="str">
-        <f t="shared" si="1"/>
-        <v>_properties.Add("D5CDD502-2E9C-101B-9397-08002B2CF9AE/22", LanguageConsts._D5CDD502-2E9C-101B-9397-08002B2CF9AE_22);</v>
+        <f t="shared" si="6"/>
+        <v>_properties.Add("D5CDD502-2E9C-101B-9397-08002B2CF9AE/22", LanguageConsts._D5CDD502_2E9C_101B_9397_08002B2CF9AE_22);</v>
       </c>
     </row>
     <row r="265" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A265" t="s">
-        <v>918</v>
+        <v>797</v>
       </c>
       <c r="B265" t="s">
-        <v>919</v>
+        <v>922</v>
       </c>
       <c r="C265" t="s">
         <v>533</v>
       </c>
       <c r="E265" t="str">
-        <f t="shared" ref="E265:E274" si="2">CONCATENATE("_properties.Add(""",A265,""", LanguageConsts.",B265,");")</f>
-        <v>_properties.Add("D5CDD502-2E9C-101B-9397-08002B2CF9AE/23", LanguageConsts._D5CDD502-2E9C-101B-9397-08002B2CF9AE_23);</v>
+        <f t="shared" ref="E265:E272" si="7">CONCATENATE("_properties.Add(""",A265,""", LanguageConsts.",B265,");")</f>
+        <v>_properties.Add("D5CDD502-2E9C-101B-9397-08002B2CF9AE/23", LanguageConsts._D5CDD502_2E9C_101B_9397_08002B2CF9AE_23);</v>
       </c>
     </row>
     <row r="266" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A266" t="s">
-        <v>920</v>
+        <v>798</v>
       </c>
       <c r="B266" t="s">
-        <v>921</v>
+        <v>923</v>
       </c>
       <c r="C266" t="s">
         <v>535</v>
       </c>
       <c r="E266" t="str">
-        <f t="shared" si="2"/>
-        <v>_properties.Add("D5CDD502-2E9C-101B-9397-08002B2CF9AE/27", LanguageConsts._D5CDD502-2E9C-101B-9397-08002B2CF9AE_27);</v>
+        <f t="shared" si="7"/>
+        <v>_properties.Add("D5CDD502-2E9C-101B-9397-08002B2CF9AE/27", LanguageConsts._D5CDD502_2E9C_101B_9397_08002B2CF9AE_27);</v>
       </c>
     </row>
     <row r="267" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A267" t="s">
-        <v>922</v>
+        <v>799</v>
       </c>
       <c r="B267" t="s">
-        <v>923</v>
+        <v>924</v>
       </c>
       <c r="C267" t="s">
         <v>536</v>
       </c>
       <c r="E267" t="str">
-        <f t="shared" si="2"/>
-        <v>_properties.Add("D5CDD502-2E9C-101B-9397-08002B2CF9AE/28", LanguageConsts._D5CDD502-2E9C-101B-9397-08002B2CF9AE_28);</v>
+        <f t="shared" si="7"/>
+        <v>_properties.Add("D5CDD502-2E9C-101B-9397-08002B2CF9AE/28", LanguageConsts._D5CDD502_2E9C_101B_9397_08002B2CF9AE_28);</v>
       </c>
     </row>
     <row r="268" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A268" t="s">
-        <v>924</v>
+        <v>800</v>
       </c>
       <c r="B268" t="s">
         <v>925</v>
@@ -7616,68 +7616,68 @@
         <v>537</v>
       </c>
       <c r="E268" t="str">
-        <f t="shared" si="2"/>
-        <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/_PID_HLINKS", LanguageConsts._D5CDD505-2E9C-101B-9397-08002B2CF9AE__PID_HLINKS);</v>
+        <f t="shared" si="7"/>
+        <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/_PID_HLINKS", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE__PID_HLINKS);</v>
       </c>
     </row>
     <row r="269" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A269" t="s">
+        <v>801</v>
+      </c>
+      <c r="B269" t="s">
         <v>926</v>
-      </c>
-      <c r="B269" t="s">
-        <v>927</v>
       </c>
       <c r="C269" t="s">
         <v>538</v>
       </c>
       <c r="E269" t="str">
-        <f t="shared" si="2"/>
-        <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/_SHAREDFILEINDEX", LanguageConsts._D5CDD505-2E9C-101B-9397-08002B2CF9AE__SHAREDFILEINDEX);</v>
+        <f t="shared" si="7"/>
+        <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/_SHAREDFILEINDEX", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE__SHAREDFILEINDEX);</v>
       </c>
     </row>
     <row r="270" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A270" t="s">
-        <v>928</v>
+        <v>802</v>
       </c>
       <c r="B270" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
       <c r="C270" t="s">
         <v>539</v>
       </c>
       <c r="E270" t="str">
-        <f t="shared" si="2"/>
-        <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/_SOURCEURL", LanguageConsts._D5CDD505-2E9C-101B-9397-08002B2CF9AE__SOURCEURL);</v>
+        <f t="shared" si="7"/>
+        <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/_SOURCEURL", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE__SOURCEURL);</v>
       </c>
     </row>
     <row r="271" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A271" t="s">
-        <v>930</v>
+        <v>803</v>
       </c>
       <c r="B271" t="s">
-        <v>931</v>
+        <v>928</v>
       </c>
       <c r="C271" t="s">
         <v>534</v>
       </c>
       <c r="E271" t="str">
-        <f t="shared" si="2"/>
-        <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/CONTENTTYPE", LanguageConsts._D5CDD505-2E9C-101B-9397-08002B2CF9AE_CONTENTTYPE);</v>
+        <f t="shared" si="7"/>
+        <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/CONTENTTYPE", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_CONTENTTYPE);</v>
       </c>
     </row>
     <row r="272" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A272" t="s">
-        <v>932</v>
+        <v>804</v>
       </c>
       <c r="B272" t="s">
-        <v>933</v>
+        <v>929</v>
       </c>
       <c r="C272" t="s">
         <v>540</v>
       </c>
       <c r="E272" t="str">
-        <f t="shared" si="2"/>
-        <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/CONTENTTYPEID", LanguageConsts._D5CDD505-2E9C-101B-9397-08002B2CF9AE_CONTENTTYPEID);</v>
+        <f t="shared" si="7"/>
+        <v>_properties.Add("D5CDD505-2E9C-101B-9397-08002B2CF9AE/CONTENTTYPEID", LanguageConsts._D5CDD505_2E9C_101B_9397_08002B2CF9AE_CONTENTTYPEID);</v>
       </c>
     </row>
   </sheetData>

</xml_diff>